<commit_message>
Fichiers d'initialisation (fixture) des différents types d'artefacts et de médias en base de données (entity TypeElement) et des champs qui les décrivent + Màj BackLog 16/04/13
</commit_message>
<xml_diff>
--- a/doc/Backlog [ACONIT].xlsx
+++ b/doc/Backlog [ACONIT].xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10155" yWindow="0" windowWidth="11490" windowHeight="10065" tabRatio="900"/>
+    <workbookView xWindow="10155" yWindow="0" windowWidth="11490" windowHeight="10065" tabRatio="900" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="20" r:id="rId1"/>
@@ -39,10 +39,10 @@
   </definedNames>
   <calcPr calcId="125725"/>
   <customWorkbookViews>
+    <customWorkbookView name="Yoann Regardin - Affichage personnalisé" guid="{29B12ED2-AD48-4E1C-B971-77E4D76C1B5F}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="609" activeSheetId="2"/>
+    <customWorkbookView name="uvba7442 - Affichage personnalisé" guid="{38566435-C99E-4958-9169-0C5C493EE97D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1213" windowHeight="665" activeSheetId="1"/>
+    <customWorkbookView name="Didier Lassissi - Affichage personnalisé" guid="{5E22A59B-ECE7-4B50-9619-81A99F53295A}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1064" windowHeight="552" activeSheetId="1"/>
     <customWorkbookView name="Bernard Notarianni - Affichage personnalisé" guid="{178C21D0-B00A-4B0E-B009-71AAC80909BC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="785" activeSheetId="1"/>
-    <customWorkbookView name="Didier Lassissi - Affichage personnalisé" guid="{5E22A59B-ECE7-4B50-9619-81A99F53295A}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1064" windowHeight="552" activeSheetId="1"/>
-    <customWorkbookView name="uvba7442 - Affichage personnalisé" guid="{38566435-C99E-4958-9169-0C5C493EE97D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1213" windowHeight="665" activeSheetId="1"/>
-    <customWorkbookView name="Yoann Regardin - Affichage personnalisé" guid="{29B12ED2-AD48-4E1C-B971-77E4D76C1B5F}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="609" activeSheetId="2"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
@@ -569,7 +569,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="29">
+  <fills count="30">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -716,6 +716,12 @@
     <fill>
       <patternFill patternType="lightUp">
         <bgColor theme="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1116,7 +1122,7 @@
     <xf numFmtId="0" fontId="26" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="170">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="5" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1610,6 +1616,12 @@
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1658,21 +1670,7 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vérification" xfId="42" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="60">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="51"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="58">
     <dxf>
       <fill>
         <patternFill>
@@ -2148,6 +2146,10 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFEBF89E"/>
+      <color rgb="FFE2F56F"/>
+    </mruColors>
   </colors>
 </styleSheet>
 </file>
@@ -2183,7 +2185,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.3703257666722507"/>
+          <c:x val="0.37032576667225087"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2200,10 +2202,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.5640078243859872E-2"/>
-          <c:y val="0.15742128935532329"/>
+          <c:x val="5.5640078243859858E-2"/>
+          <c:y val="0.15742128935532335"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192103"/>
+          <c:h val="0.70464767616192114"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2312,7 +2314,7 @@
                   <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>#N/A</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>#N/A</c:v>
@@ -2513,11 +2515,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="112002944"/>
-        <c:axId val="112021504"/>
+        <c:axId val="104142720"/>
+        <c:axId val="104157184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112002944"/>
+        <c:axId val="104142720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2549,7 +2551,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112021504"/>
+        <c:crossAx val="104157184"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2557,7 +2559,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112021504"/>
+        <c:axId val="104157184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2599,7 +2601,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112002944"/>
+        <c:crossAx val="104142720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2687,7 +2689,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000078" footer="0.49212598450000078"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000083" footer="0.49212598450000083"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2724,7 +2726,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225098"/>
+          <c:x val="0.37032576667225109"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2741,10 +2743,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.5640078243859852E-2"/>
-          <c:y val="0.15742128935532343"/>
+          <c:x val="5.5640078243859845E-2"/>
+          <c:y val="0.15742128935532348"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192125"/>
+          <c:h val="0.70464767616192137"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3054,11 +3056,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="112640768"/>
-        <c:axId val="112642688"/>
+        <c:axId val="104444672"/>
+        <c:axId val="104446592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112640768"/>
+        <c:axId val="104444672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3090,7 +3092,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112642688"/>
+        <c:crossAx val="104446592"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3098,7 +3100,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112642688"/>
+        <c:axId val="104446592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3140,7 +3142,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112640768"/>
+        <c:crossAx val="104444672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3228,7 +3230,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000089" footer="0.49212598450000089"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000095" footer="0.49212598450000095"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3265,7 +3267,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225126"/>
+          <c:x val="0.37032576667225142"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3283,9 +3285,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532354"/>
+          <c:y val="0.1574212893553236"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192159"/>
+          <c:h val="0.70464767616192181"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3595,11 +3597,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="112524288"/>
-        <c:axId val="112620672"/>
+        <c:axId val="103743872"/>
+        <c:axId val="103744640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112524288"/>
+        <c:axId val="103743872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3631,7 +3633,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112620672"/>
+        <c:crossAx val="103744640"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3639,7 +3641,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112620672"/>
+        <c:axId val="103744640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3681,7 +3683,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112524288"/>
+        <c:crossAx val="103743872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3769,7 +3771,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.492125984500001" footer="0.492125984500001"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000106" footer="0.49212598450000106"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3806,7 +3808,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225153"/>
+          <c:x val="0.3703257666722517"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3824,9 +3826,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532368"/>
+          <c:y val="0.15742128935532376"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192192"/>
+          <c:h val="0.70464767616192203"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -4136,11 +4138,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="112707072"/>
-        <c:axId val="112708992"/>
+        <c:axId val="104379904"/>
+        <c:axId val="104381824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112707072"/>
+        <c:axId val="104379904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4172,7 +4174,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112708992"/>
+        <c:crossAx val="104381824"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -4180,7 +4182,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112708992"/>
+        <c:axId val="104381824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4222,7 +4224,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112707072"/>
+        <c:crossAx val="104379904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4310,7 +4312,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000111" footer="0.49212598450000111"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000117" footer="0.49212598450000117"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -4754,11 +4756,11 @@
   </sheetPr>
   <dimension ref="A1:M307"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="5" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -5136,7 +5138,7 @@
         <v>32</v>
       </c>
       <c r="G16" s="76">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H16" s="75"/>
       <c r="I16" s="75"/>
@@ -5304,7 +5306,7 @@
         <v>75</v>
       </c>
       <c r="G22" s="73">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H22" s="30"/>
       <c r="I22" s="30"/>
@@ -6183,10 +6185,10 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="D21:D22 A54:A55 B48:C48 D49:E51 H48:K48 A47:A49 D38:E38 D41 B28:C33 A37:A44 B33:E33 H28:K33 A27:A33 B12:E12 D13:E13 B13:C17 H12:K17 E13:E15 E17:E22 D15 D23:E23 A13:A24 D28 D30 E28:E33">
-    <cfRule type="expression" dxfId="59" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="49" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="50" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6201,9 +6203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:DP85"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
@@ -6401,7 +6401,9 @@
       <c r="C3" s="73">
         <v>2</v>
       </c>
-      <c r="D3" s="34"/>
+      <c r="D3" s="73">
+        <v>2</v>
+      </c>
       <c r="E3" s="34"/>
       <c r="F3" s="34"/>
       <c r="G3" s="34"/>
@@ -6424,10 +6426,12 @@
       <c r="B4" s="76">
         <v>6</v>
       </c>
-      <c r="C4" s="73">
+      <c r="C4" s="170">
         <v>2</v>
       </c>
-      <c r="D4" s="34"/>
+      <c r="D4" s="73">
+        <v>1</v>
+      </c>
       <c r="E4" s="34"/>
       <c r="F4" s="34"/>
       <c r="G4" s="34"/>
@@ -6450,10 +6454,12 @@
       <c r="B5" s="76">
         <v>7</v>
       </c>
-      <c r="C5" s="73">
+      <c r="C5" s="170">
         <v>2</v>
       </c>
-      <c r="D5" s="34"/>
+      <c r="D5" s="73">
+        <v>1</v>
+      </c>
       <c r="E5" s="34"/>
       <c r="F5" s="34"/>
       <c r="G5" s="34"/>
@@ -6476,10 +6482,12 @@
       <c r="B6" s="76">
         <v>8</v>
       </c>
-      <c r="C6" s="73">
+      <c r="C6" s="170">
         <v>2</v>
       </c>
-      <c r="D6" s="34"/>
+      <c r="D6" s="73">
+        <v>1</v>
+      </c>
       <c r="E6" s="34"/>
       <c r="F6" s="34"/>
       <c r="G6" s="34"/>
@@ -6502,10 +6510,12 @@
       <c r="B7" s="76">
         <v>9</v>
       </c>
-      <c r="C7" s="76">
-        <v>10</v>
-      </c>
-      <c r="D7" s="34"/>
+      <c r="C7" s="171">
+        <v>5</v>
+      </c>
+      <c r="D7" s="76">
+        <v>2</v>
+      </c>
       <c r="E7" s="34"/>
       <c r="F7" s="34"/>
       <c r="G7" s="34"/>
@@ -6531,7 +6541,9 @@
       <c r="C8" s="73">
         <v>8</v>
       </c>
-      <c r="D8" s="34"/>
+      <c r="D8" s="73">
+        <v>8</v>
+      </c>
       <c r="E8" s="34"/>
       <c r="F8" s="34"/>
       <c r="G8" s="34"/>
@@ -6557,7 +6569,9 @@
       <c r="C9" s="73">
         <v>5</v>
       </c>
-      <c r="D9" s="43"/>
+      <c r="D9" s="73">
+        <v>5</v>
+      </c>
       <c r="E9" s="43"/>
       <c r="F9" s="43"/>
       <c r="G9" s="43"/>
@@ -6583,7 +6597,9 @@
       <c r="C10" s="73">
         <v>5</v>
       </c>
-      <c r="D10" s="34"/>
+      <c r="D10" s="73">
+        <v>5</v>
+      </c>
       <c r="E10" s="34"/>
       <c r="F10" s="34"/>
       <c r="G10" s="34"/>
@@ -6609,7 +6625,9 @@
       <c r="C11" s="73">
         <v>3</v>
       </c>
-      <c r="D11" s="73"/>
+      <c r="D11" s="73">
+        <v>3</v>
+      </c>
       <c r="E11" s="73"/>
       <c r="F11" s="73"/>
       <c r="G11" s="73"/>
@@ -6635,7 +6653,9 @@
       <c r="C12" s="73">
         <v>3</v>
       </c>
-      <c r="D12" s="73"/>
+      <c r="D12" s="73">
+        <v>3</v>
+      </c>
       <c r="E12" s="73"/>
       <c r="F12" s="73"/>
       <c r="G12" s="73"/>
@@ -6659,9 +6679,11 @@
         <v>15</v>
       </c>
       <c r="C13" s="73">
-        <v>8</v>
-      </c>
-      <c r="D13" s="112"/>
+        <v>13</v>
+      </c>
+      <c r="D13" s="73">
+        <v>13</v>
+      </c>
       <c r="E13" s="112"/>
       <c r="F13" s="112"/>
       <c r="G13" s="112"/>
@@ -6687,7 +6709,9 @@
       <c r="C14" s="73">
         <v>3</v>
       </c>
-      <c r="D14" s="145"/>
+      <c r="D14" s="73">
+        <v>3</v>
+      </c>
       <c r="E14" s="145"/>
       <c r="F14" s="145"/>
       <c r="G14" s="145"/>
@@ -6754,9 +6778,9 @@
         <f t="array" ref="C17">IF(ISBLANK(C3:C14),NA(), SUM(C3:C14))</f>
         <v>53</v>
       </c>
-      <c r="D17" s="39" t="e">
+      <c r="D17" s="39">
         <f t="array" ref="D17">IF(ISBLANK(D3:D14), NA(), SUM(D3:D14))</f>
-        <v>#N/A</v>
+        <v>47</v>
       </c>
       <c r="E17" s="39" t="e">
         <f t="array" ref="E17">IF(ISBLANK(E3:E14), NA(), SUM(E3:E14))</f>
@@ -6923,9 +6947,9 @@
         <v>38</v>
       </c>
       <c r="C18" s="39"/>
-      <c r="D18" s="39" t="e">
+      <c r="D18" s="39">
         <f>C17-D17</f>
-        <v>#N/A</v>
+        <v>6</v>
       </c>
       <c r="E18" s="39" t="e">
         <f t="shared" ref="E18:R18" si="0">D17-E17</f>
@@ -7165,9 +7189,9 @@
         <f>1-C17/$C$17</f>
         <v>0</v>
       </c>
-      <c r="D20" s="59" t="e">
+      <c r="D20" s="59">
         <f t="shared" ref="D20:R20" si="2">1-D17/$C$17</f>
-        <v>#N/A</v>
+        <v>0.1132075471698113</v>
       </c>
       <c r="E20" s="59" t="e">
         <f t="shared" si="2"/>
@@ -8527,91 +8551,91 @@
       <c r="R85" s="39"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A3:B13 O14 D3:R13">
-    <cfRule type="expression" dxfId="57" priority="53" stopIfTrue="1">
+  <conditionalFormatting sqref="A3:B13 O14 E3:R13">
+    <cfRule type="expression" dxfId="55" priority="53" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="54" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A12 B5:B13 A4:A5">
-    <cfRule type="expression" dxfId="55" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="31" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="32" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7 A12:A13">
-    <cfRule type="expression" dxfId="53" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="29" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="30" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B13">
-    <cfRule type="expression" dxfId="51" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="15" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="16" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A5">
-    <cfRule type="expression" dxfId="49" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="13" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="14" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7 A12:A14">
-    <cfRule type="expression" dxfId="47" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="11" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="12" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B14">
-    <cfRule type="expression" dxfId="45" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="9" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="10" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B14">
-    <cfRule type="expression" dxfId="43" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="7" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="8" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A4 A6 A11:A12 A14">
-    <cfRule type="expression" dxfId="41" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="5" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="6" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B14">
-    <cfRule type="expression" dxfId="39" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A4 A6 A12:A14">
-    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="1" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="2" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10847,42 +10871,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E7:R9 D7:D8 D3:R5 D11:R11 A3:A11 B3:B4 B6:B11">
-    <cfRule type="expression" dxfId="37" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="33" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="34" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A11 B10:B11 B4 B6:B8">
-    <cfRule type="expression" dxfId="35" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="31" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="32" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5 A7 A10:B10 B4 B6:B8">
-    <cfRule type="expression" dxfId="33" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="9" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="10" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:G6">
-    <cfRule type="expression" dxfId="31" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:G10">
-    <cfRule type="expression" dxfId="29" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="1" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="2" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12877,50 +12901,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:R9 A3:A9 B3 B5:B6 B8:B9">
-    <cfRule type="expression" dxfId="27" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="27" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="28" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9 A4:A7 B3 B5:B6 B8:B9">
-    <cfRule type="expression" dxfId="25" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="25" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="26" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5 A7">
-    <cfRule type="expression" dxfId="23" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="23" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="24" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3 B5:B6 B8:B10">
-    <cfRule type="expression" dxfId="21" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="5" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="6" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4 A7">
-    <cfRule type="expression" dxfId="19" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B10 B3 B5:B6">
-    <cfRule type="expression" dxfId="17" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="1" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="2" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15040,50 +15064,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:B6 D3:R6">
-    <cfRule type="expression" dxfId="15" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="25" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="26" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B6 A4:B6">
-    <cfRule type="expression" dxfId="13" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="23" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="24" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="expression" dxfId="11" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="21" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="22" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B5">
-    <cfRule type="expression" dxfId="9" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A7">
-    <cfRule type="expression" dxfId="7" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B5">
-    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Finalisation des tests des entity de la collection en base de données + Maj BackLog 18/04/13
</commit_message>
<xml_diff>
--- a/doc/Backlog [ACONIT].xlsx
+++ b/doc/Backlog [ACONIT].xlsx
@@ -39,10 +39,10 @@
   </definedNames>
   <calcPr calcId="125725"/>
   <customWorkbookViews>
+    <customWorkbookView name="Yoann Regardin - Affichage personnalisé" guid="{29B12ED2-AD48-4E1C-B971-77E4D76C1B5F}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="609" activeSheetId="2"/>
+    <customWorkbookView name="uvba7442 - Affichage personnalisé" guid="{38566435-C99E-4958-9169-0C5C493EE97D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1213" windowHeight="665" activeSheetId="1"/>
+    <customWorkbookView name="Didier Lassissi - Affichage personnalisé" guid="{5E22A59B-ECE7-4B50-9619-81A99F53295A}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1064" windowHeight="552" activeSheetId="1"/>
     <customWorkbookView name="Bernard Notarianni - Affichage personnalisé" guid="{178C21D0-B00A-4B0E-B009-71AAC80909BC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="785" activeSheetId="1"/>
-    <customWorkbookView name="Didier Lassissi - Affichage personnalisé" guid="{5E22A59B-ECE7-4B50-9619-81A99F53295A}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1064" windowHeight="552" activeSheetId="1"/>
-    <customWorkbookView name="uvba7442 - Affichage personnalisé" guid="{38566435-C99E-4958-9169-0C5C493EE97D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1213" windowHeight="665" activeSheetId="1"/>
-    <customWorkbookView name="Yoann Regardin - Affichage personnalisé" guid="{29B12ED2-AD48-4E1C-B971-77E4D76C1B5F}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="609" activeSheetId="2"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
@@ -1122,7 +1122,7 @@
     <xf numFmtId="0" fontId="26" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="173">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="5" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1599,6 +1599,9 @@
     <xf numFmtId="0" fontId="6" fillId="29" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1623,8 +1626,8 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -2188,7 +2191,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225098"/>
+          <c:x val="0.37032576667225109"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2205,10 +2208,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.5640078243859852E-2"/>
-          <c:y val="0.15742128935532343"/>
+          <c:x val="5.5640078243859845E-2"/>
+          <c:y val="0.15742128935532348"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192125"/>
+          <c:h val="0.70464767616192137"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2323,7 +2326,7 @@
                   <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>#N/A</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>#N/A</c:v>
@@ -2518,11 +2521,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="112138112"/>
-        <c:axId val="112152576"/>
+        <c:axId val="111089536"/>
+        <c:axId val="111104000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112138112"/>
+        <c:axId val="111089536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2554,7 +2557,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112152576"/>
+        <c:crossAx val="111104000"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2562,7 +2565,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112152576"/>
+        <c:axId val="111104000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2604,7 +2607,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112138112"/>
+        <c:crossAx val="111089536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2692,7 +2695,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000089" footer="0.49212598450000089"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000095" footer="0.49212598450000095"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2729,7 +2732,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225126"/>
+          <c:x val="0.37032576667225142"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2747,9 +2750,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532354"/>
+          <c:y val="0.1574212893553236"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192159"/>
+          <c:h val="0.70464767616192181"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3233,7 +3236,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.492125984500001" footer="0.492125984500001"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000106" footer="0.49212598450000106"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3270,7 +3273,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225153"/>
+          <c:x val="0.3703257666722517"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3288,9 +3291,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532368"/>
+          <c:y val="0.15742128935532376"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192192"/>
+          <c:h val="0.70464767616192203"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3600,11 +3603,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="112720896"/>
-        <c:axId val="112723072"/>
+        <c:axId val="112716800"/>
+        <c:axId val="112821376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112720896"/>
+        <c:axId val="112716800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3636,7 +3639,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112723072"/>
+        <c:crossAx val="112821376"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3644,7 +3647,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112723072"/>
+        <c:axId val="112821376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3686,7 +3689,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112720896"/>
+        <c:crossAx val="112716800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3774,7 +3777,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000111" footer="0.49212598450000111"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000117" footer="0.49212598450000117"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3811,7 +3814,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225187"/>
+          <c:x val="0.37032576667225198"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3829,9 +3832,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532382"/>
+          <c:y val="0.1574212893553239"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192214"/>
+          <c:h val="0.70464767616192225"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -4141,11 +4144,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="112903680"/>
-        <c:axId val="112905600"/>
+        <c:axId val="112899584"/>
+        <c:axId val="112901504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112903680"/>
+        <c:axId val="112899584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4177,7 +4180,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112905600"/>
+        <c:crossAx val="112901504"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -4185,7 +4188,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112905600"/>
+        <c:axId val="112901504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4227,7 +4230,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112903680"/>
+        <c:crossAx val="112899584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4315,7 +4318,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000122" footer="0.49212598450000122"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000128" footer="0.49212598450000128"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -4787,10 +4790,10 @@
         <v>18</v>
       </c>
       <c r="C1" s="25"/>
-      <c r="D1" s="169" t="s">
+      <c r="D1" s="170" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="169"/>
+      <c r="E1" s="170"/>
       <c r="F1" s="24"/>
       <c r="G1" s="24"/>
       <c r="H1" s="15"/>
@@ -4802,10 +4805,10 @@
       <c r="A2" s="65"/>
       <c r="B2" s="16"/>
       <c r="C2" s="14"/>
-      <c r="D2" s="170" t="s">
+      <c r="D2" s="171" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="171"/>
+      <c r="E2" s="172"/>
       <c r="F2" s="26"/>
       <c r="G2" s="60"/>
       <c r="H2" s="3"/>
@@ -4821,8 +4824,8 @@
         <f>MAX(A13:A48)+1</f>
         <v>35</v>
       </c>
-      <c r="D3" s="164"/>
-      <c r="E3" s="165"/>
+      <c r="D3" s="165"/>
+      <c r="E3" s="166"/>
       <c r="F3" s="26"/>
       <c r="G3" s="60"/>
       <c r="H3" s="3"/>
@@ -4830,9 +4833,9 @@
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:13" hidden="1">
-      <c r="A4" s="166"/>
-      <c r="B4" s="167"/>
-      <c r="C4" s="168"/>
+      <c r="A4" s="167"/>
+      <c r="B4" s="168"/>
+      <c r="C4" s="169"/>
       <c r="D4" s="17"/>
       <c r="E4" s="5"/>
       <c r="F4" s="27"/>
@@ -6207,7 +6210,7 @@
   <dimension ref="A1:DP85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -6412,7 +6415,9 @@
       <c r="E3" s="162">
         <v>1</v>
       </c>
-      <c r="F3" s="34"/>
+      <c r="F3" s="173">
+        <v>1</v>
+      </c>
       <c r="G3" s="34"/>
       <c r="H3" s="43"/>
       <c r="I3" s="43"/>
@@ -6442,7 +6447,9 @@
       <c r="E4" s="162">
         <v>1</v>
       </c>
-      <c r="F4" s="34"/>
+      <c r="F4" s="173">
+        <v>1</v>
+      </c>
       <c r="G4" s="34"/>
       <c r="H4" s="43"/>
       <c r="I4" s="43"/>
@@ -6472,7 +6479,9 @@
       <c r="E5" s="162">
         <v>1</v>
       </c>
-      <c r="F5" s="34"/>
+      <c r="F5" s="173">
+        <v>1</v>
+      </c>
       <c r="G5" s="34"/>
       <c r="H5" s="43"/>
       <c r="I5" s="43"/>
@@ -6493,7 +6502,7 @@
       <c r="B6" s="76">
         <v>8</v>
       </c>
-      <c r="C6" s="172">
+      <c r="C6" s="164">
         <v>2</v>
       </c>
       <c r="D6" s="162">
@@ -6502,7 +6511,9 @@
       <c r="E6" s="162">
         <v>1</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="173">
+        <v>1</v>
+      </c>
       <c r="G6" s="34"/>
       <c r="H6" s="43"/>
       <c r="I6" s="43"/>
@@ -6532,7 +6543,9 @@
       <c r="E7" s="163">
         <v>1</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="173">
+        <v>0</v>
+      </c>
       <c r="G7" s="34"/>
       <c r="H7" s="35"/>
       <c r="I7" s="35"/>
@@ -6562,7 +6575,9 @@
       <c r="E8" s="73">
         <v>8</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="73">
+        <v>8</v>
+      </c>
       <c r="G8" s="34"/>
       <c r="H8" s="35"/>
       <c r="I8" s="35"/>
@@ -6592,7 +6607,9 @@
       <c r="E9" s="73">
         <v>5</v>
       </c>
-      <c r="F9" s="43"/>
+      <c r="F9" s="73">
+        <v>5</v>
+      </c>
       <c r="G9" s="43"/>
       <c r="H9" s="35"/>
       <c r="I9" s="35"/>
@@ -6622,7 +6639,9 @@
       <c r="E10" s="73">
         <v>5</v>
       </c>
-      <c r="F10" s="34"/>
+      <c r="F10" s="73">
+        <v>5</v>
+      </c>
       <c r="G10" s="34"/>
       <c r="H10" s="35"/>
       <c r="I10" s="35"/>
@@ -6652,7 +6671,9 @@
       <c r="E11" s="73">
         <v>3</v>
       </c>
-      <c r="F11" s="73"/>
+      <c r="F11" s="73">
+        <v>3</v>
+      </c>
       <c r="G11" s="73"/>
       <c r="H11" s="112"/>
       <c r="I11" s="112"/>
@@ -6682,7 +6703,9 @@
       <c r="E12" s="73">
         <v>3</v>
       </c>
-      <c r="F12" s="73"/>
+      <c r="F12" s="73">
+        <v>3</v>
+      </c>
       <c r="G12" s="73"/>
       <c r="H12" s="112"/>
       <c r="I12" s="112"/>
@@ -6709,10 +6732,12 @@
       <c r="D13" s="73">
         <v>13</v>
       </c>
-      <c r="E13" s="73">
+      <c r="E13" s="162">
         <v>13</v>
       </c>
-      <c r="F13" s="112"/>
+      <c r="F13" s="162">
+        <v>11</v>
+      </c>
       <c r="G13" s="112"/>
       <c r="H13" s="112"/>
       <c r="I13" s="112"/>
@@ -6742,7 +6767,9 @@
       <c r="E14" s="73">
         <v>3</v>
       </c>
-      <c r="F14" s="145"/>
+      <c r="F14" s="73">
+        <v>3</v>
+      </c>
       <c r="G14" s="145"/>
       <c r="H14" s="145"/>
       <c r="I14" s="145"/>
@@ -6815,9 +6842,9 @@
         <f t="array" ref="E17">IF(ISBLANK(E3:E14), NA(), SUM(E3:E14))</f>
         <v>45</v>
       </c>
-      <c r="F17" s="39" t="e">
+      <c r="F17" s="39">
         <f t="array" ref="F17">IF(ISBLANK(F3:F14), NA(), SUM(F3:F14))</f>
-        <v>#N/A</v>
+        <v>42</v>
       </c>
       <c r="G17" s="39" t="e">
         <f t="array" ref="G17">IF(ISBLANK(G3:G14), NA(), SUM(G3:G14))</f>
@@ -6984,9 +7011,9 @@
         <f t="shared" ref="E18:R18" si="0">D17-E17</f>
         <v>3</v>
       </c>
-      <c r="F18" s="39" t="e">
+      <c r="F18" s="39">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>3</v>
       </c>
       <c r="G18" s="39" t="e">
         <f t="shared" si="0"/>
@@ -7226,9 +7253,9 @@
         <f t="shared" si="2"/>
         <v>0.15094339622641506</v>
       </c>
-      <c r="F20" s="59" t="e">
+      <c r="F20" s="59">
         <f t="shared" si="2"/>
-        <v>#N/A</v>
+        <v>0.20754716981132071</v>
       </c>
       <c r="G20" s="59" t="e">
         <f t="shared" si="2"/>
@@ -8580,7 +8607,7 @@
       <c r="R85" s="39"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A3:B13 O14 F3:R13">
+  <conditionalFormatting sqref="A3:B13 O14 G3:R13 F3:F7">
     <cfRule type="expression" dxfId="55" priority="53" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>

</xml_diff>

<commit_message>
page de dreation d'un artefact : ajout de la gestion des erreurs dans le formulaire
</commit_message>
<xml_diff>
--- a/doc/Backlog [ACONIT].xlsx
+++ b/doc/Backlog [ACONIT].xlsx
@@ -39,10 +39,10 @@
   </definedNames>
   <calcPr calcId="125725"/>
   <customWorkbookViews>
+    <customWorkbookView name="Bernard Notarianni - Affichage personnalisé" guid="{178C21D0-B00A-4B0E-B009-71AAC80909BC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="785" activeSheetId="1"/>
+    <customWorkbookView name="Didier Lassissi - Affichage personnalisé" guid="{5E22A59B-ECE7-4B50-9619-81A99F53295A}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1064" windowHeight="552" activeSheetId="1"/>
+    <customWorkbookView name="uvba7442 - Affichage personnalisé" guid="{38566435-C99E-4958-9169-0C5C493EE97D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1213" windowHeight="665" activeSheetId="1"/>
     <customWorkbookView name="Yoann Regardin - Affichage personnalisé" guid="{29B12ED2-AD48-4E1C-B971-77E4D76C1B5F}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="609" activeSheetId="2"/>
-    <customWorkbookView name="uvba7442 - Affichage personnalisé" guid="{38566435-C99E-4958-9169-0C5C493EE97D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1213" windowHeight="665" activeSheetId="1"/>
-    <customWorkbookView name="Didier Lassissi - Affichage personnalisé" guid="{5E22A59B-ECE7-4B50-9619-81A99F53295A}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1064" windowHeight="552" activeSheetId="1"/>
-    <customWorkbookView name="Bernard Notarianni - Affichage personnalisé" guid="{178C21D0-B00A-4B0E-B009-71AAC80909BC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="785" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
@@ -1679,7 +1679,21 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vérification" xfId="42" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="62">
+  <dxfs count="64">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2222,7 +2236,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225142"/>
+          <c:x val="0.37032576667225153"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2240,9 +2254,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.1574212893553236"/>
+          <c:y val="0.15742128935532368"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192181"/>
+          <c:h val="0.70464767616192192"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2369,7 +2383,7 @@
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>#N/A</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>#N/A</c:v>
@@ -2552,11 +2566,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="104994688"/>
-        <c:axId val="105009152"/>
+        <c:axId val="111286144"/>
+        <c:axId val="111300608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="104994688"/>
+        <c:axId val="111286144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2588,7 +2602,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105009152"/>
+        <c:crossAx val="111300608"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2596,7 +2610,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105009152"/>
+        <c:axId val="111300608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2638,7 +2652,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="104994688"/>
+        <c:crossAx val="111286144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2726,7 +2740,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000106" footer="0.49212598450000106"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000111" footer="0.49212598450000111"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2763,7 +2777,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.3703257666722517"/>
+          <c:x val="0.37032576667225187"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2781,9 +2795,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532376"/>
+          <c:y val="0.15742128935532382"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192203"/>
+          <c:h val="0.70464767616192214"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3093,11 +3107,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="105698048"/>
-        <c:axId val="105699968"/>
+        <c:axId val="112636672"/>
+        <c:axId val="112638592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105698048"/>
+        <c:axId val="112636672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3129,7 +3143,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105699968"/>
+        <c:crossAx val="112638592"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3137,7 +3151,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105699968"/>
+        <c:axId val="112638592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3179,7 +3193,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105698048"/>
+        <c:crossAx val="112636672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3267,7 +3281,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000117" footer="0.49212598450000117"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000122" footer="0.49212598450000122"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3304,7 +3318,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225198"/>
+          <c:x val="0.37032576667225209"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3322,9 +3336,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.1574212893553239"/>
+          <c:y val="0.15742128935532396"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192225"/>
+          <c:h val="0.70464767616192236"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3634,11 +3648,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="105577472"/>
-        <c:axId val="105579648"/>
+        <c:axId val="111214976"/>
+        <c:axId val="111215744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105577472"/>
+        <c:axId val="111214976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3670,7 +3684,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105579648"/>
+        <c:crossAx val="111215744"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3678,7 +3692,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105579648"/>
+        <c:axId val="111215744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3720,7 +3734,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105577472"/>
+        <c:crossAx val="111214976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3808,7 +3822,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000128" footer="0.49212598450000128"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000133" footer="0.49212598450000133"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3845,7 +3859,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225225"/>
+          <c:x val="0.37032576667225242"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3863,9 +3877,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532401"/>
+          <c:y val="0.15742128935532407"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192259"/>
+          <c:h val="0.70464767616192281"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -4175,11 +4189,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="105760256"/>
-        <c:axId val="105762176"/>
+        <c:axId val="112772608"/>
+        <c:axId val="112774528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105760256"/>
+        <c:axId val="112772608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4211,7 +4225,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105762176"/>
+        <c:crossAx val="112774528"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -4219,7 +4233,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105762176"/>
+        <c:axId val="112774528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4261,7 +4275,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105760256"/>
+        <c:crossAx val="112772608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4349,7 +4363,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000139" footer="0.49212598450000139"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000145" footer="0.49212598450000145"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -6222,10 +6236,10 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="D21:D22 A54:A55 B48:C48 D49:E51 H48:K48 A47:A49 D38:E38 D41 B28:C33 A37:A44 B33:E33 H28:K33 A27:A33 B12:E12 D13:E13 B13:C17 H12:K17 E13:E15 E17:E22 D15 D23:E23 A13:A24 D28 D30 E28:E33">
-    <cfRule type="expression" dxfId="61" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="49" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="50" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6240,7 +6254,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:DP85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
@@ -6456,7 +6472,9 @@
       <c r="I3" s="164">
         <v>0</v>
       </c>
-      <c r="J3" s="164"/>
+      <c r="J3" s="164">
+        <v>0</v>
+      </c>
       <c r="K3" s="164"/>
       <c r="L3" s="164"/>
       <c r="M3" s="164"/>
@@ -6494,7 +6512,9 @@
       <c r="I4" s="164">
         <v>0</v>
       </c>
-      <c r="J4" s="164"/>
+      <c r="J4" s="164">
+        <v>0</v>
+      </c>
       <c r="K4" s="164"/>
       <c r="L4" s="164"/>
       <c r="M4" s="164"/>
@@ -6532,7 +6552,9 @@
       <c r="I5" s="164">
         <v>0</v>
       </c>
-      <c r="J5" s="164"/>
+      <c r="J5" s="164">
+        <v>0</v>
+      </c>
       <c r="K5" s="164"/>
       <c r="L5" s="164"/>
       <c r="M5" s="164"/>
@@ -6570,7 +6592,9 @@
       <c r="I6" s="164">
         <v>0</v>
       </c>
-      <c r="J6" s="164"/>
+      <c r="J6" s="164">
+        <v>0</v>
+      </c>
       <c r="K6" s="164"/>
       <c r="L6" s="164"/>
       <c r="M6" s="164"/>
@@ -6608,7 +6632,9 @@
       <c r="I7" s="111">
         <v>0</v>
       </c>
-      <c r="J7" s="111"/>
+      <c r="J7" s="111">
+        <v>0</v>
+      </c>
       <c r="K7" s="111"/>
       <c r="L7" s="111"/>
       <c r="M7" s="111"/>
@@ -6646,8 +6672,10 @@
       <c r="I8" s="161">
         <v>6</v>
       </c>
-      <c r="J8" s="111"/>
-      <c r="K8" s="111"/>
+      <c r="J8" s="161">
+        <v>5</v>
+      </c>
+      <c r="K8" s="161"/>
       <c r="L8" s="111"/>
       <c r="M8" s="111"/>
       <c r="N8" s="111"/>
@@ -6684,8 +6712,10 @@
       <c r="I9" s="161">
         <v>3</v>
       </c>
-      <c r="J9" s="111"/>
-      <c r="K9" s="111"/>
+      <c r="J9" s="161">
+        <v>2</v>
+      </c>
+      <c r="K9" s="161"/>
       <c r="L9" s="111"/>
       <c r="M9" s="111"/>
       <c r="N9" s="111"/>
@@ -6722,8 +6752,10 @@
       <c r="I10" s="161">
         <v>5</v>
       </c>
-      <c r="J10" s="111"/>
-      <c r="K10" s="111"/>
+      <c r="J10" s="161">
+        <v>4</v>
+      </c>
+      <c r="K10" s="161"/>
       <c r="L10" s="111"/>
       <c r="M10" s="111"/>
       <c r="N10" s="111"/>
@@ -6760,7 +6792,9 @@
       <c r="I11" s="111">
         <v>3</v>
       </c>
-      <c r="J11" s="111"/>
+      <c r="J11" s="111">
+        <v>3</v>
+      </c>
       <c r="K11" s="111"/>
       <c r="L11" s="111"/>
       <c r="M11" s="111"/>
@@ -6798,7 +6832,9 @@
       <c r="I12" s="111">
         <v>3</v>
       </c>
-      <c r="J12" s="111"/>
+      <c r="J12" s="111">
+        <v>3</v>
+      </c>
       <c r="K12" s="111"/>
       <c r="L12" s="111"/>
       <c r="M12" s="111"/>
@@ -6836,8 +6872,10 @@
       <c r="I13" s="161">
         <v>4</v>
       </c>
-      <c r="J13" s="111"/>
-      <c r="K13" s="111"/>
+      <c r="J13" s="161">
+        <v>2</v>
+      </c>
+      <c r="K13" s="161"/>
       <c r="L13" s="111"/>
       <c r="M13" s="111"/>
       <c r="N13" s="111"/>
@@ -6874,7 +6912,9 @@
       <c r="I14" s="144">
         <v>3</v>
       </c>
-      <c r="J14" s="144"/>
+      <c r="J14" s="144">
+        <v>3</v>
+      </c>
       <c r="K14" s="144"/>
       <c r="L14" s="144"/>
       <c r="M14" s="144"/>
@@ -6959,9 +6999,9 @@
         <f t="array" ref="I17">IF(ISBLANK(I3:I14), NA(), SUM(I3:I14))</f>
         <v>27</v>
       </c>
-      <c r="J17" s="38" t="e">
+      <c r="J17" s="38">
         <f t="array" ref="J17">IF(ISBLANK(J3:J14), NA(), SUM(J3:J14))</f>
-        <v>#N/A</v>
+        <v>22</v>
       </c>
       <c r="K17" s="38" t="e">
         <f t="array" ref="K17">IF(ISBLANK(K3:K14), NA(), SUM(K3:K14))</f>
@@ -7128,9 +7168,9 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="J18" s="38" t="e">
+      <c r="J18" s="38">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>5</v>
       </c>
       <c r="K18" s="38" t="e">
         <f t="shared" si="0"/>
@@ -7370,9 +7410,9 @@
         <f t="shared" si="2"/>
         <v>0.49056603773584906</v>
       </c>
-      <c r="J20" s="58" t="e">
+      <c r="J20" s="58">
         <f t="shared" si="2"/>
-        <v>#N/A</v>
+        <v>0.58490566037735847</v>
       </c>
       <c r="K20" s="58" t="e">
         <f t="shared" si="2"/>
@@ -8709,90 +8749,90 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:B13 O14 F3:G7 G13 H3:R13">
-    <cfRule type="expression" dxfId="59" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="53" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="54" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A12 B5:B13 A4:A5">
-    <cfRule type="expression" dxfId="57" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="31" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="32" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7 A12:A13">
-    <cfRule type="expression" dxfId="55" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="29" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="30" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B13">
-    <cfRule type="expression" dxfId="53" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="15" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="16" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A5">
-    <cfRule type="expression" dxfId="51" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="13" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="14" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7 A12:A14">
-    <cfRule type="expression" dxfId="49" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="11" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="12" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B14">
-    <cfRule type="expression" dxfId="47" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="9" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="10" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B14">
-    <cfRule type="expression" dxfId="45" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="7" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="8" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A4 A6 A11:A12 A14">
-    <cfRule type="expression" dxfId="43" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="5" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="6" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B14">
-    <cfRule type="expression" dxfId="41" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A4 A6 A12:A14">
-    <cfRule type="expression" dxfId="39" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="1" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="2" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11028,42 +11068,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E7:R9 D7:D8 D3:R5 D11:R11 A3:A11 B3:B4 B6:B11">
-    <cfRule type="expression" dxfId="37" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="33" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="34" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A11 B10:B11 B4 B6:B8">
-    <cfRule type="expression" dxfId="35" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="31" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="32" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5 A7 A10:B10 B4 B6:B8">
-    <cfRule type="expression" dxfId="33" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="9" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="10" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:G6">
-    <cfRule type="expression" dxfId="31" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:G10">
-    <cfRule type="expression" dxfId="29" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="1" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="2" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13058,50 +13098,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:R9 A3:A9 B3 B5:B6 B8:B9">
-    <cfRule type="expression" dxfId="27" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="27" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="28" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9 A4:A7 B3 B5:B6 B8:B9">
-    <cfRule type="expression" dxfId="25" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="25" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="26" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5 A7">
-    <cfRule type="expression" dxfId="23" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="23" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="24" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3 B5:B6 B8:B10">
-    <cfRule type="expression" dxfId="21" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="5" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="6" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4 A7">
-    <cfRule type="expression" dxfId="19" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B10 B3 B5:B6">
-    <cfRule type="expression" dxfId="17" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="1" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="2" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15221,50 +15261,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:B6 D3:R6">
-    <cfRule type="expression" dxfId="15" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="25" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="26" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B6 A4:B6">
-    <cfRule type="expression" dxfId="13" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="23" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="24" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="expression" dxfId="11" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="21" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="22" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B5">
-    <cfRule type="expression" dxfId="9" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="5" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="6" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A7">
-    <cfRule type="expression" dxfId="7" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B5">
-    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="1" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Ajout des messages d'aides sur les pages
</commit_message>
<xml_diff>
--- a/doc/Backlog [ACONIT].xlsx
+++ b/doc/Backlog [ACONIT].xlsx
@@ -39,10 +39,10 @@
   </definedNames>
   <calcPr calcId="125725"/>
   <customWorkbookViews>
+    <customWorkbookView name="Bernard Notarianni - Affichage personnalisé" guid="{178C21D0-B00A-4B0E-B009-71AAC80909BC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="785" activeSheetId="1"/>
+    <customWorkbookView name="Didier Lassissi - Affichage personnalisé" guid="{5E22A59B-ECE7-4B50-9619-81A99F53295A}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1064" windowHeight="552" activeSheetId="1"/>
+    <customWorkbookView name="uvba7442 - Affichage personnalisé" guid="{38566435-C99E-4958-9169-0C5C493EE97D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1213" windowHeight="665" activeSheetId="1"/>
     <customWorkbookView name="Yoann Regardin - Affichage personnalisé" guid="{29B12ED2-AD48-4E1C-B971-77E4D76C1B5F}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="609" activeSheetId="2"/>
-    <customWorkbookView name="uvba7442 - Affichage personnalisé" guid="{38566435-C99E-4958-9169-0C5C493EE97D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1213" windowHeight="665" activeSheetId="1"/>
-    <customWorkbookView name="Didier Lassissi - Affichage personnalisé" guid="{5E22A59B-ECE7-4B50-9619-81A99F53295A}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1064" windowHeight="552" activeSheetId="1"/>
-    <customWorkbookView name="Bernard Notarianni - Affichage personnalisé" guid="{178C21D0-B00A-4B0E-B009-71AAC80909BC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="785" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
@@ -1122,7 +1122,7 @@
     <xf numFmtId="0" fontId="26" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="5" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1631,6 +1631,12 @@
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="13" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1679,7 +1685,21 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vérification" xfId="42" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="60">
+  <dxfs count="62">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2208,7 +2228,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225198"/>
+          <c:x val="0.37032576667225209"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2226,9 +2246,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.1574212893553239"/>
+          <c:y val="0.15742128935532396"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192225"/>
+          <c:h val="0.70464767616192236"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2367,10 +2387,10 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>#N/A</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>#N/A</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>#N/A</c:v>
@@ -2538,11 +2558,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="109516672"/>
-        <c:axId val="109531136"/>
+        <c:axId val="106043264"/>
+        <c:axId val="106057728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="109516672"/>
+        <c:axId val="106043264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2574,7 +2594,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="109531136"/>
+        <c:crossAx val="106057728"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2582,7 +2602,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109531136"/>
+        <c:axId val="106057728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2624,7 +2644,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="109516672"/>
+        <c:crossAx val="106043264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2712,7 +2732,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000128" footer="0.49212598450000128"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000133" footer="0.49212598450000133"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2749,7 +2769,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225225"/>
+          <c:x val="0.37032576667225242"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2767,9 +2787,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532401"/>
+          <c:y val="0.15742128935532407"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192259"/>
+          <c:h val="0.70464767616192281"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3079,11 +3099,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="109818624"/>
-        <c:axId val="109820544"/>
+        <c:axId val="107795200"/>
+        <c:axId val="107797120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="109818624"/>
+        <c:axId val="107795200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3115,7 +3135,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="109820544"/>
+        <c:crossAx val="107797120"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3123,7 +3143,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109820544"/>
+        <c:axId val="107797120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3165,7 +3185,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="109818624"/>
+        <c:crossAx val="107795200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3253,7 +3273,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000139" footer="0.49212598450000139"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000145" footer="0.49212598450000145"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3290,7 +3310,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225253"/>
+          <c:x val="0.3703257666722527"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3308,9 +3328,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532415"/>
+          <c:y val="0.15742128935532423"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192292"/>
+          <c:h val="0.70464767616192303"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3620,11 +3640,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="109894656"/>
-        <c:axId val="109900928"/>
+        <c:axId val="107670528"/>
+        <c:axId val="107775104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="109894656"/>
+        <c:axId val="107670528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3656,7 +3676,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="109900928"/>
+        <c:crossAx val="107775104"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3664,7 +3684,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109900928"/>
+        <c:axId val="107775104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3706,7 +3726,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="109894656"/>
+        <c:crossAx val="107670528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3794,7 +3814,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.4921259845000015" footer="0.4921259845000015"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000156" footer="0.49212598450000156"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3831,7 +3851,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225287"/>
+          <c:x val="0.37032576667225298"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3849,9 +3869,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532429"/>
+          <c:y val="0.15742128935532435"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192314"/>
+          <c:h val="0.70464767616192325"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -4161,11 +4181,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="109954560"/>
-        <c:axId val="109956480"/>
+        <c:axId val="107857408"/>
+        <c:axId val="107859328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="109954560"/>
+        <c:axId val="107857408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4197,7 +4217,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="109956480"/>
+        <c:crossAx val="107859328"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -4205,7 +4225,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109956480"/>
+        <c:axId val="107859328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4247,7 +4267,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="109954560"/>
+        <c:crossAx val="107857408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4335,7 +4355,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000161" footer="0.49212598450000161"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000167" footer="0.49212598450000167"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -6208,10 +6228,10 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="D21:D22 A54:A55 B48:C48 D49:E51 H48:K48 A47:A49 D38:E38 D41 B28:C33 A37:A44 B33:E33 H28:K33 A27:A33 B12:E12 D13:E13 B13:C17 H12:K17 E13:E15 E17:E22 D15 D23:E23 A13:A24 D28 D30 E28:E33">
-    <cfRule type="expression" dxfId="59" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="49" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="50" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6226,8 +6246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:DP85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -6456,8 +6476,12 @@
       <c r="M3" s="164">
         <v>0</v>
       </c>
-      <c r="N3" s="164"/>
-      <c r="O3" s="165"/>
+      <c r="N3" s="164">
+        <v>0</v>
+      </c>
+      <c r="O3" s="165">
+        <v>0</v>
+      </c>
       <c r="P3" s="164"/>
       <c r="Q3" s="164"/>
       <c r="R3" s="166"/>
@@ -6502,8 +6526,12 @@
       <c r="M4" s="164">
         <v>0</v>
       </c>
-      <c r="N4" s="164"/>
-      <c r="O4" s="165"/>
+      <c r="N4" s="164">
+        <v>0</v>
+      </c>
+      <c r="O4" s="165">
+        <v>0</v>
+      </c>
       <c r="P4" s="164"/>
       <c r="Q4" s="164"/>
       <c r="R4" s="166"/>
@@ -6548,8 +6576,12 @@
       <c r="M5" s="164">
         <v>0</v>
       </c>
-      <c r="N5" s="164"/>
-      <c r="O5" s="165"/>
+      <c r="N5" s="164">
+        <v>0</v>
+      </c>
+      <c r="O5" s="165">
+        <v>0</v>
+      </c>
       <c r="P5" s="164"/>
       <c r="Q5" s="164"/>
       <c r="R5" s="166"/>
@@ -6594,8 +6626,12 @@
       <c r="M6" s="164">
         <v>0</v>
       </c>
-      <c r="N6" s="164"/>
-      <c r="O6" s="165"/>
+      <c r="N6" s="164">
+        <v>0</v>
+      </c>
+      <c r="O6" s="165">
+        <v>0</v>
+      </c>
       <c r="P6" s="164"/>
       <c r="Q6" s="164"/>
       <c r="R6" s="166"/>
@@ -6640,8 +6676,12 @@
       <c r="M7" s="111">
         <v>0</v>
       </c>
-      <c r="N7" s="111"/>
-      <c r="O7" s="143"/>
+      <c r="N7" s="111">
+        <v>0</v>
+      </c>
+      <c r="O7" s="143">
+        <v>0</v>
+      </c>
       <c r="P7" s="111"/>
       <c r="Q7" s="111"/>
       <c r="R7" s="91"/>
@@ -6683,11 +6723,15 @@
       <c r="L8" s="161">
         <v>3</v>
       </c>
-      <c r="M8" s="111">
+      <c r="M8" s="161">
         <v>2</v>
       </c>
-      <c r="N8" s="111"/>
-      <c r="O8" s="143"/>
+      <c r="N8" s="161">
+        <v>1</v>
+      </c>
+      <c r="O8" s="175">
+        <v>1</v>
+      </c>
       <c r="P8" s="111"/>
       <c r="Q8" s="111"/>
       <c r="R8" s="91"/>
@@ -6729,11 +6773,15 @@
       <c r="L9" s="161">
         <v>1</v>
       </c>
-      <c r="M9" s="111">
+      <c r="M9" s="161">
         <v>1</v>
       </c>
-      <c r="N9" s="111"/>
-      <c r="O9" s="143"/>
+      <c r="N9" s="111">
+        <v>0</v>
+      </c>
+      <c r="O9" s="143">
+        <v>0</v>
+      </c>
       <c r="P9" s="111"/>
       <c r="Q9" s="111"/>
       <c r="R9" s="91"/>
@@ -6775,11 +6823,15 @@
       <c r="L10" s="161">
         <v>2</v>
       </c>
-      <c r="M10" s="111">
+      <c r="M10" s="161">
         <v>1</v>
       </c>
-      <c r="N10" s="111"/>
-      <c r="O10" s="143"/>
+      <c r="N10" s="111">
+        <v>0</v>
+      </c>
+      <c r="O10" s="143">
+        <v>0</v>
+      </c>
       <c r="P10" s="111"/>
       <c r="Q10" s="111"/>
       <c r="R10" s="91"/>
@@ -6821,11 +6873,15 @@
       <c r="L11" s="111">
         <v>3</v>
       </c>
-      <c r="M11" s="111">
+      <c r="M11" s="163">
         <v>3</v>
       </c>
-      <c r="N11" s="111"/>
-      <c r="O11" s="143"/>
+      <c r="N11" s="161">
+        <v>3</v>
+      </c>
+      <c r="O11" s="175">
+        <v>3</v>
+      </c>
       <c r="P11" s="111"/>
       <c r="Q11" s="111"/>
       <c r="R11" s="91"/>
@@ -6867,11 +6923,15 @@
       <c r="L12" s="111">
         <v>3</v>
       </c>
-      <c r="M12" s="111">
+      <c r="M12" s="163">
         <v>3</v>
       </c>
-      <c r="N12" s="111"/>
-      <c r="O12" s="143"/>
+      <c r="N12" s="161">
+        <v>3</v>
+      </c>
+      <c r="O12" s="175">
+        <v>3</v>
+      </c>
       <c r="P12" s="111"/>
       <c r="Q12" s="111"/>
       <c r="R12" s="91"/>
@@ -6916,8 +6976,12 @@
       <c r="M13" s="111">
         <v>0</v>
       </c>
-      <c r="N13" s="111"/>
-      <c r="O13" s="143"/>
+      <c r="N13" s="111">
+        <v>0</v>
+      </c>
+      <c r="O13" s="143">
+        <v>0</v>
+      </c>
       <c r="P13" s="111"/>
       <c r="Q13" s="111"/>
       <c r="R13" s="91"/>
@@ -6962,8 +7026,12 @@
       <c r="M14" s="144">
         <v>3</v>
       </c>
-      <c r="N14" s="144"/>
-      <c r="O14" s="143"/>
+      <c r="N14" s="144">
+        <v>3</v>
+      </c>
+      <c r="O14" s="176">
+        <v>3</v>
+      </c>
       <c r="P14" s="144"/>
       <c r="Q14" s="144"/>
       <c r="R14" s="145"/>
@@ -7059,13 +7127,13 @@
         <f t="array" ref="M17">IF(ISBLANK(M3:M14), NA(), SUM(M3:M14))</f>
         <v>13</v>
       </c>
-      <c r="N17" s="38" t="e">
+      <c r="N17" s="38">
         <f t="array" ref="N17">IF(ISBLANK(N3:N14), NA(), SUM(N3:N14))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O17" s="38" t="e">
+        <v>10</v>
+      </c>
+      <c r="O17" s="38">
         <f t="array" ref="O17">IF(ISBLANK(O3:O14), NA(), SUM(O3:O14))</f>
-        <v>#N/A</v>
+        <v>10</v>
       </c>
       <c r="P17" s="38" t="e">
         <f t="array" ref="P17">IF(ISBLANK(P3:P14), NA(), SUM(P3:P14))</f>
@@ -7228,13 +7296,13 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="N18" s="38" t="e">
+      <c r="N18" s="38">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="O18" s="38" t="e">
+        <v>3</v>
+      </c>
+      <c r="O18" s="38">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="P18" s="38" t="e">
         <f>O17-P17</f>
@@ -7470,13 +7538,13 @@
         <f t="shared" si="2"/>
         <v>0.75471698113207553</v>
       </c>
-      <c r="N20" s="58" t="e">
+      <c r="N20" s="58">
         <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="O20" s="58" t="e">
+        <v>0.81132075471698117</v>
+      </c>
+      <c r="O20" s="58">
         <f t="shared" si="2"/>
-        <v>#N/A</v>
+        <v>0.81132075471698117</v>
       </c>
       <c r="P20" s="58" t="e">
         <f t="shared" si="2"/>
@@ -8793,90 +8861,90 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:B13 O14 F3:G7 G13 H3:R13">
-    <cfRule type="expression" dxfId="57" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="53" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="54" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A12 B5:B13 A4:A5">
-    <cfRule type="expression" dxfId="55" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="31" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="32" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7 A12:A13">
-    <cfRule type="expression" dxfId="53" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="29" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="30" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B13">
-    <cfRule type="expression" dxfId="51" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="15" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="16" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A5">
-    <cfRule type="expression" dxfId="49" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="13" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="14" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7 A12:A14">
-    <cfRule type="expression" dxfId="47" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="11" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="12" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B14">
-    <cfRule type="expression" dxfId="45" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="9" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="10" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B14">
-    <cfRule type="expression" dxfId="43" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="7" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="8" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A4 A6 A11:A12 A14">
-    <cfRule type="expression" dxfId="41" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="5" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="6" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B14">
-    <cfRule type="expression" dxfId="39" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A4 A6 A12:A14">
-    <cfRule type="expression" dxfId="37" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="1" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="2" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11112,42 +11180,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E7:R9 D7:D8 D3:R5 D11:R11 A3:A11 B3:B4 B6:B11">
-    <cfRule type="expression" dxfId="35" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="33" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="34" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A11 B10:B11 B4 B6:B8">
-    <cfRule type="expression" dxfId="33" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="31" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="32" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5 A7 A10:B10 B4 B6:B8">
-    <cfRule type="expression" dxfId="31" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="9" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="10" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:G6">
-    <cfRule type="expression" dxfId="29" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:G10">
-    <cfRule type="expression" dxfId="27" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="1" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="2" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13142,50 +13210,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:R9 A3:A9 B3 B5:B6 B8:B9">
-    <cfRule type="expression" dxfId="25" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="27" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="28" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9 A4:A7 B3 B5:B6 B8:B9">
-    <cfRule type="expression" dxfId="23" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="25" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="26" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5 A7">
-    <cfRule type="expression" dxfId="21" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="23" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="24" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3 B5:B6 B8:B10">
-    <cfRule type="expression" dxfId="19" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="5" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="6" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4 A7">
-    <cfRule type="expression" dxfId="17" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B10 B3 B5:B6">
-    <cfRule type="expression" dxfId="15" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="1" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="2" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15305,50 +15373,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:B6 D3:R6">
-    <cfRule type="expression" dxfId="13" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="25" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="26" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B6 A4:B6">
-    <cfRule type="expression" dxfId="11" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="23" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="24" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="expression" dxfId="9" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="21" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="22" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B5">
-    <cfRule type="expression" dxfId="7" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="5" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="6" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A7">
-    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B5">
-    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Maj création d'un artefact/média avec le nouveau modèle
</commit_message>
<xml_diff>
--- a/doc/Backlog [ACONIT].xlsx
+++ b/doc/Backlog [ACONIT].xlsx
@@ -32,24 +32,24 @@
     <definedName name="_Toc347234371" localSheetId="0">'Product backlog'!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Product backlog'!$5:$5</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Iteration 1'!$R$12:$Z$22</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Iteration 2'!$R$18:$Z$27</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Iteration 2'!$R$16:$Z$25</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Iteration 3'!$R$10:$Z$17</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'Iteration 4'!$R$7:$Z$16</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Product backlog'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <customWorkbookViews>
+    <customWorkbookView name="Yoann Regardin - Affichage personnalisé" guid="{29B12ED2-AD48-4E1C-B971-77E4D76C1B5F}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="609" activeSheetId="2"/>
+    <customWorkbookView name="uvba7442 - Affichage personnalisé" guid="{38566435-C99E-4958-9169-0C5C493EE97D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1213" windowHeight="665" activeSheetId="1"/>
+    <customWorkbookView name="Didier Lassissi - Affichage personnalisé" guid="{5E22A59B-ECE7-4B50-9619-81A99F53295A}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1064" windowHeight="552" activeSheetId="1"/>
     <customWorkbookView name="Bernard Notarianni - Affichage personnalisé" guid="{178C21D0-B00A-4B0E-B009-71AAC80909BC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="785" activeSheetId="1"/>
-    <customWorkbookView name="Didier Lassissi - Affichage personnalisé" guid="{5E22A59B-ECE7-4B50-9619-81A99F53295A}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1064" windowHeight="552" activeSheetId="1"/>
-    <customWorkbookView name="uvba7442 - Affichage personnalisé" guid="{38566435-C99E-4958-9169-0C5C493EE97D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1213" windowHeight="665" activeSheetId="1"/>
-    <customWorkbookView name="Yoann Regardin - Affichage personnalisé" guid="{29B12ED2-AD48-4E1C-B971-77E4D76C1B5F}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="609" activeSheetId="2"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="109">
   <si>
     <t>Itération</t>
   </si>
@@ -397,6 +397,9 @@
   </si>
   <si>
     <t>Suppression du ficer à la suppression du champ de type fichier ou d'un type d'élément</t>
+  </si>
+  <si>
+    <t>Modification du modèle de données (Data)</t>
   </si>
 </sst>
 </file>
@@ -1129,7 +1132,7 @@
     <xf numFmtId="0" fontId="26" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="172">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="5" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1594,6 +1597,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="13" xfId="43" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1618,16 +1631,16 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="13" xfId="43" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" xfId="43" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20 % - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1675,21 +1688,7 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vérification" xfId="42" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="36">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="51"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="34">
     <dxf>
       <fill>
         <patternFill>
@@ -2036,7 +2035,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225242"/>
+          <c:x val="0.37032576667225253"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2054,9 +2053,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532407"/>
+          <c:y val="0.15742128935532415"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192281"/>
+          <c:h val="0.70464767616192292"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2366,11 +2365,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="110360448"/>
-        <c:axId val="110637056"/>
+        <c:axId val="100857728"/>
+        <c:axId val="101138432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="110360448"/>
+        <c:axId val="100857728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2402,7 +2401,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="110637056"/>
+        <c:crossAx val="101138432"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2410,7 +2409,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110637056"/>
+        <c:axId val="101138432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2452,7 +2451,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="110360448"/>
+        <c:crossAx val="100857728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2540,7 +2539,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000145" footer="0.49212598450000145"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.4921259845000015" footer="0.4921259845000015"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2577,7 +2576,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.3703257666722527"/>
+          <c:x val="0.37032576667225287"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2595,9 +2594,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532423"/>
+          <c:y val="0.15742128935532429"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192303"/>
+          <c:h val="0.70464767616192314"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2607,7 +2606,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Iteration 2'!$B$19</c:f>
+              <c:f>'Iteration 2'!$B$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2698,12 +2697,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Iteration 2'!$C$19:$R$19</c:f>
+              <c:f>'Iteration 2'!$C$17:$R$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>57</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
@@ -2759,7 +2758,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Iteration 2'!$B$21</c:f>
+              <c:f>'Iteration 2'!$B$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2850,68 +2849,68 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Iteration 2'!$C$21:$R$21</c:f>
+              <c:f>'Iteration 2'!$C$19:$R$19</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>57</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>53.2</c:v>
+                  <c:v>50.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49.400000000000006</c:v>
+                  <c:v>46.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45.600000000000009</c:v>
+                  <c:v>43.199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41.800000000000011</c:v>
+                  <c:v>39.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38.000000000000014</c:v>
+                  <c:v>35.999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34.200000000000017</c:v>
+                  <c:v>32.399999999999991</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30.400000000000016</c:v>
+                  <c:v>28.79999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>26.600000000000016</c:v>
+                  <c:v>25.199999999999989</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22.800000000000015</c:v>
+                  <c:v>21.599999999999987</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19.000000000000014</c:v>
+                  <c:v>17.999999999999986</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15.200000000000014</c:v>
+                  <c:v>14.399999999999986</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11.400000000000013</c:v>
+                  <c:v>10.799999999999986</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.600000000000013</c:v>
+                  <c:v>7.1999999999999869</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.8000000000000131</c:v>
+                  <c:v>3.5999999999999868</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.3322676295501878E-14</c:v>
+                  <c:v>-1.3322676295501878E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="110867200"/>
-        <c:axId val="110869120"/>
+        <c:axId val="101556992"/>
+        <c:axId val="101558912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="110867200"/>
+        <c:axId val="101556992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2943,7 +2942,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="110869120"/>
+        <c:crossAx val="101558912"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2951,7 +2950,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110869120"/>
+        <c:axId val="101558912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2993,7 +2992,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="110867200"/>
+        <c:crossAx val="101556992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3081,7 +3080,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000156" footer="0.49212598450000156"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000161" footer="0.49212598450000161"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3118,7 +3117,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225298"/>
+          <c:x val="0.37032576667225309"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3136,9 +3135,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532435"/>
+          <c:y val="0.15742128935532443"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192325"/>
+          <c:h val="0.70464767616192336"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3448,11 +3447,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="110935040"/>
-        <c:axId val="110937216"/>
+        <c:axId val="101370880"/>
+        <c:axId val="101377152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="110935040"/>
+        <c:axId val="101370880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3484,7 +3483,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="110937216"/>
+        <c:crossAx val="101377152"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3492,7 +3491,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110937216"/>
+        <c:axId val="101377152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3534,7 +3533,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="110935040"/>
+        <c:crossAx val="101370880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3622,7 +3621,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000167" footer="0.49212598450000167"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000172" footer="0.49212598450000172"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3659,7 +3658,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225325"/>
+          <c:x val="0.37032576667225342"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3677,9 +3676,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532448"/>
+          <c:y val="0.15742128935532454"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192359"/>
+          <c:h val="0.70464767616192381"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3989,11 +3988,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="110986752"/>
-        <c:axId val="110988672"/>
+        <c:axId val="101623296"/>
+        <c:axId val="101625216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="110986752"/>
+        <c:axId val="101623296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4025,7 +4024,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="110988672"/>
+        <c:crossAx val="101625216"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -4033,7 +4032,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110988672"/>
+        <c:axId val="101625216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4075,7 +4074,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="110986752"/>
+        <c:crossAx val="101623296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4163,7 +4162,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000178" footer="0.49212598450000178"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000183" footer="0.49212598450000183"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -4212,13 +4211,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>100854</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>31826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>156884</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>28385</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4608,10 +4607,10 @@
   <dimension ref="A1:M307"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="E21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="E24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D39" sqref="D39"/>
+      <selection pane="bottomRight" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -4635,10 +4634,10 @@
         <v>18</v>
       </c>
       <c r="C1" s="25"/>
-      <c r="D1" s="165" t="s">
+      <c r="D1" s="169" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="165"/>
+      <c r="E1" s="169"/>
       <c r="F1" s="24"/>
       <c r="G1" s="24"/>
       <c r="H1" s="15"/>
@@ -4650,10 +4649,10 @@
       <c r="A2" s="64"/>
       <c r="B2" s="16"/>
       <c r="C2" s="14"/>
-      <c r="D2" s="166" t="s">
+      <c r="D2" s="170" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="167"/>
+      <c r="E2" s="171"/>
       <c r="F2" s="26"/>
       <c r="G2" s="59"/>
       <c r="H2" s="3"/>
@@ -4669,8 +4668,8 @@
         <f>MAX(A13:A48)+1</f>
         <v>35</v>
       </c>
-      <c r="D3" s="160"/>
-      <c r="E3" s="161"/>
+      <c r="D3" s="164"/>
+      <c r="E3" s="165"/>
       <c r="F3" s="26"/>
       <c r="G3" s="59"/>
       <c r="H3" s="3"/>
@@ -4678,9 +4677,9 @@
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:13" hidden="1">
-      <c r="A4" s="162"/>
-      <c r="B4" s="163"/>
-      <c r="C4" s="164"/>
+      <c r="A4" s="166"/>
+      <c r="B4" s="167"/>
+      <c r="C4" s="168"/>
       <c r="D4" s="17"/>
       <c r="E4" s="5"/>
       <c r="F4" s="27"/>
@@ -5166,8 +5165,8 @@
       <c r="E23" s="35"/>
       <c r="F23" s="33"/>
       <c r="G23" s="33">
-        <f>SUM(G24:G35)</f>
-        <v>60</v>
+        <f>SUM(G24:G33)</f>
+        <v>58</v>
       </c>
       <c r="H23" s="141"/>
       <c r="I23" s="32"/>
@@ -5192,7 +5191,7 @@
         <v>32</v>
       </c>
       <c r="G24" s="72">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H24" s="30"/>
       <c r="I24" s="30"/>
@@ -5376,138 +5375,138 @@
       <c r="J31" s="29"/>
       <c r="K31" s="29"/>
     </row>
-    <row r="32" spans="1:13" s="12" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A32" s="75"/>
-      <c r="B32" s="79"/>
-      <c r="C32" s="75"/>
-      <c r="D32" s="89" t="s">
-        <v>62</v>
-      </c>
-      <c r="E32" s="90" t="s">
-        <v>64</v>
-      </c>
-      <c r="F32" s="91"/>
-      <c r="G32" s="91"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="11"/>
+    <row r="32" spans="1:13" ht="24.95" customHeight="1">
+      <c r="A32" s="68">
+        <v>24</v>
+      </c>
+      <c r="B32" s="69">
+        <v>2</v>
+      </c>
+      <c r="C32" s="68"/>
+      <c r="D32" s="70" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" s="71"/>
+      <c r="F32" s="72" t="s">
+        <v>28</v>
+      </c>
+      <c r="G32" s="72">
+        <v>3</v>
+      </c>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="22"/>
       <c r="K32" s="11"/>
     </row>
-    <row r="33" spans="1:13" s="12" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A33" s="75">
+    <row r="33" spans="1:13" ht="24.95" customHeight="1">
+      <c r="A33" s="68">
+        <v>25</v>
+      </c>
+      <c r="B33" s="69">
+        <v>2</v>
+      </c>
+      <c r="C33" s="68"/>
+      <c r="D33" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="79">
-        <v>2</v>
-      </c>
-      <c r="C33" s="68">
-        <v>1</v>
-      </c>
-      <c r="D33" s="70" t="s">
-        <v>88</v>
-      </c>
-      <c r="E33" s="70"/>
+      <c r="E33" s="71"/>
       <c r="F33" s="72" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="G33" s="72">
-        <v>12</v>
-      </c>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
+        <v>3</v>
+      </c>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
       <c r="J33" s="22"/>
       <c r="K33" s="11"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-    </row>
-    <row r="34" spans="1:13" ht="24.95" customHeight="1">
-      <c r="A34" s="68">
-        <v>24</v>
-      </c>
-      <c r="B34" s="69">
-        <v>2</v>
-      </c>
-      <c r="C34" s="68"/>
-      <c r="D34" s="70" t="s">
-        <v>66</v>
-      </c>
-      <c r="E34" s="71"/>
-      <c r="F34" s="72" t="s">
-        <v>28</v>
-      </c>
-      <c r="G34" s="72">
+    </row>
+    <row r="34" spans="1:13" s="13" customFormat="1">
+      <c r="A34" s="65"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="60" t="s">
+        <v>93</v>
+      </c>
+      <c r="E34" s="35"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="33">
+        <f>SUM(G35:G44)</f>
+        <v>59</v>
+      </c>
+      <c r="H34" s="141"/>
+      <c r="I34" s="114"/>
+      <c r="J34" s="115"/>
+      <c r="K34" s="113"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
+    </row>
+    <row r="35" spans="1:13" ht="24.95" customHeight="1">
+      <c r="A35" s="75">
+        <v>26</v>
+      </c>
+      <c r="B35" s="69">
         <v>3</v>
-      </c>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="22"/>
-      <c r="K34" s="11"/>
-    </row>
-    <row r="35" spans="1:13" ht="24.95" customHeight="1">
-      <c r="A35" s="68">
-        <v>25</v>
-      </c>
-      <c r="B35" s="69">
-        <v>2</v>
       </c>
       <c r="C35" s="68"/>
       <c r="D35" s="70" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E35" s="71"/>
       <c r="F35" s="72" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G35" s="72">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H35" s="30"/>
       <c r="I35" s="30"/>
       <c r="J35" s="22"/>
       <c r="K35" s="11"/>
     </row>
-    <row r="36" spans="1:13" s="13" customFormat="1">
-      <c r="A36" s="65"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="60" t="s">
-        <v>93</v>
-      </c>
-      <c r="E36" s="35"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="33">
-        <f>SUM(G37:G45)</f>
-        <v>55</v>
-      </c>
-      <c r="H36" s="141"/>
-      <c r="I36" s="114"/>
-      <c r="J36" s="115"/>
-      <c r="K36" s="113"/>
-      <c r="L36" s="12"/>
-      <c r="M36" s="12"/>
-    </row>
-    <row r="37" spans="1:13" ht="24.95" customHeight="1">
+    <row r="36" spans="1:13" s="12" customFormat="1" ht="24.95" customHeight="1">
+      <c r="A36" s="75"/>
+      <c r="B36" s="79"/>
+      <c r="C36" s="75"/>
+      <c r="D36" s="89" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36" s="90" t="s">
+        <v>64</v>
+      </c>
+      <c r="F36" s="91"/>
+      <c r="G36" s="91"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+    </row>
+    <row r="37" spans="1:13" s="12" customFormat="1" ht="24.95" customHeight="1">
       <c r="A37" s="75">
-        <v>26</v>
-      </c>
-      <c r="B37" s="69">
-        <v>3</v>
-      </c>
-      <c r="C37" s="68"/>
+        <v>23</v>
+      </c>
+      <c r="B37" s="79">
+        <v>2</v>
+      </c>
+      <c r="C37" s="68">
+        <v>1</v>
+      </c>
       <c r="D37" s="70" t="s">
-        <v>19</v>
-      </c>
-      <c r="E37" s="71"/>
+        <v>88</v>
+      </c>
+      <c r="E37" s="70"/>
       <c r="F37" s="72" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="G37" s="72">
-        <v>10</v>
-      </c>
-      <c r="H37" s="30"/>
-      <c r="I37" s="30"/>
+        <v>12</v>
+      </c>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
       <c r="J37" s="22"/>
       <c r="K37" s="11"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
     </row>
     <row r="38" spans="1:13" ht="24.95" customHeight="1">
       <c r="A38" s="75"/>
@@ -5643,98 +5642,98 @@
       <c r="J43" s="22"/>
       <c r="K43" s="11"/>
     </row>
-    <row r="44" spans="1:13" ht="24.95" customHeight="1">
-      <c r="A44" s="75">
-        <v>31</v>
+    <row r="44" spans="1:13" s="13" customFormat="1" ht="24.95" customHeight="1">
+      <c r="A44" s="68">
+        <v>32</v>
       </c>
       <c r="B44" s="69">
         <v>3</v>
       </c>
-      <c r="C44" s="68">
-        <v>2</v>
-      </c>
+      <c r="C44" s="68"/>
       <c r="D44" s="70" t="s">
-        <v>86</v>
-      </c>
-      <c r="E44" s="70" t="s">
-        <v>87</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="E44" s="71"/>
       <c r="F44" s="72" t="s">
+        <v>28</v>
+      </c>
+      <c r="G44" s="111">
+        <v>3</v>
+      </c>
+      <c r="H44" s="112"/>
+      <c r="I44" s="116"/>
+      <c r="J44" s="116"/>
+      <c r="K44" s="116"/>
+      <c r="L44" s="12"/>
+      <c r="M44" s="12"/>
+    </row>
+    <row r="45" spans="1:13" ht="12.75" customHeight="1">
+      <c r="A45" s="65"/>
+      <c r="B45" s="31"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="E45" s="35"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="33">
+        <f>SUM(G46:G52)</f>
+        <v>53</v>
+      </c>
+      <c r="H45" s="142"/>
+      <c r="I45" s="114"/>
+      <c r="J45" s="115"/>
+      <c r="K45" s="118"/>
+    </row>
+    <row r="46" spans="1:13" ht="24.95" customHeight="1">
+      <c r="A46" s="75">
+        <v>33</v>
+      </c>
+      <c r="B46" s="69">
+        <v>4</v>
+      </c>
+      <c r="C46" s="68"/>
+      <c r="D46" s="70" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" s="71"/>
+      <c r="F46" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="72">
-        <v>8</v>
-      </c>
-      <c r="H44" s="30"/>
-      <c r="I44" s="30"/>
-      <c r="J44" s="22"/>
-      <c r="K44" s="11"/>
-    </row>
-    <row r="45" spans="1:13" s="13" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A45" s="68">
-        <v>32</v>
-      </c>
-      <c r="B45" s="69">
-        <v>3</v>
-      </c>
-      <c r="C45" s="68"/>
-      <c r="D45" s="70" t="s">
-        <v>24</v>
-      </c>
-      <c r="E45" s="71"/>
-      <c r="F45" s="72" t="s">
-        <v>28</v>
-      </c>
-      <c r="G45" s="111">
-        <v>3</v>
-      </c>
-      <c r="H45" s="112"/>
-      <c r="I45" s="116"/>
-      <c r="J45" s="116"/>
-      <c r="K45" s="116"/>
-      <c r="L45" s="12"/>
-      <c r="M45" s="12"/>
-    </row>
-    <row r="46" spans="1:13" ht="12.75" customHeight="1">
-      <c r="A46" s="65"/>
-      <c r="B46" s="31"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="E46" s="35"/>
-      <c r="F46" s="33"/>
-      <c r="G46" s="33">
-        <f>SUM(G47:G52)</f>
-        <v>45</v>
-      </c>
-      <c r="H46" s="142"/>
-      <c r="I46" s="114"/>
-      <c r="J46" s="115"/>
-      <c r="K46" s="118"/>
+      <c r="G46" s="111">
+        <v>10</v>
+      </c>
+      <c r="H46" s="30"/>
+      <c r="I46" s="117"/>
+      <c r="J46" s="61"/>
+      <c r="K46" s="62"/>
     </row>
     <row r="47" spans="1:13" ht="24.95" customHeight="1">
       <c r="A47" s="75">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B47" s="69">
-        <v>4</v>
-      </c>
-      <c r="C47" s="68"/>
+        <v>3</v>
+      </c>
+      <c r="C47" s="68">
+        <v>2</v>
+      </c>
       <c r="D47" s="70" t="s">
-        <v>21</v>
-      </c>
-      <c r="E47" s="71"/>
+        <v>86</v>
+      </c>
+      <c r="E47" s="70" t="s">
+        <v>87</v>
+      </c>
       <c r="F47" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="G47" s="111">
-        <v>10</v>
+      <c r="G47" s="72">
+        <v>8</v>
       </c>
       <c r="H47" s="30"/>
-      <c r="I47" s="117"/>
-      <c r="J47" s="61"/>
-      <c r="K47" s="62"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="22"/>
+      <c r="K47" s="11"/>
     </row>
     <row r="48" spans="1:13" s="12" customFormat="1" ht="24.95" customHeight="1">
       <c r="A48" s="75">
@@ -6035,11 +6034,11 @@
     <mergeCell ref="D2:E2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="D26 A54:A55 B48:C48 D49:E51 H48:K48 A47:A49 D38:E38 D41 B28:C33 A37:A44 B33:E33 H28:K33 D20:E21 E25:E26 A25:A33 D28 D30 E28:E33 B12:E12 D13:E13 B13:C17 H12:K17 E13:E15 E17:E19 D15 A13:A22">
-    <cfRule type="expression" dxfId="35" priority="49" stopIfTrue="1">
+  <conditionalFormatting sqref="A54:A55 B48:C48 D49:E51 H48:K48 A46:A49 B37:E37 D15 D38:E38 D41 B36:C37 H36:K37 E36:E37 A35:A43 D26 B28:C31 A13:A22 H28:K31 D20:E21 E25:E26 A25:A31 D28 D30 E28:E31 B12:E12 D13:E13 B13:C17 H12:K17 E13:E15 E17:E19">
+    <cfRule type="expression" dxfId="5" priority="49" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="50" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8595,10 +8594,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DP87"/>
+  <dimension ref="A1:DP85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -8788,13 +8787,13 @@
       <c r="DP2" s="41"/>
     </row>
     <row r="3" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A3" s="168" t="s">
+      <c r="A3" s="160" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="169">
+      <c r="B3" s="161">
         <v>16</v>
       </c>
-      <c r="C3" s="170"/>
+      <c r="C3" s="162"/>
       <c r="D3" s="49"/>
       <c r="E3" s="49"/>
       <c r="F3" s="48"/>
@@ -8811,39 +8810,43 @@
       <c r="Q3" s="48"/>
       <c r="R3" s="48"/>
     </row>
-    <row r="4" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A4" s="70" t="s">
-        <v>104</v>
-      </c>
-      <c r="B4" s="68"/>
-      <c r="C4" s="97">
-        <v>4</v>
-      </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="159"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="42"/>
-      <c r="O4" s="42"/>
-      <c r="P4" s="42"/>
-      <c r="Q4" s="42"/>
-      <c r="R4" s="48"/>
+    <row r="4" spans="1:120" s="175" customFormat="1" ht="24.95" customHeight="1">
+      <c r="A4" s="172" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="173"/>
+      <c r="C4" s="174">
+        <v>10</v>
+      </c>
+      <c r="D4" s="174">
+        <v>10</v>
+      </c>
+      <c r="E4" s="94"/>
+      <c r="F4" s="95"/>
+      <c r="G4" s="95"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="95"/>
+      <c r="J4" s="95"/>
+      <c r="K4" s="95"/>
+      <c r="L4" s="95"/>
+      <c r="M4" s="95"/>
+      <c r="N4" s="95"/>
+      <c r="O4" s="95"/>
+      <c r="P4" s="95"/>
+      <c r="Q4" s="95"/>
+      <c r="R4" s="95"/>
     </row>
     <row r="5" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
       <c r="A5" s="70" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" s="68"/>
       <c r="C5" s="97">
-        <v>1</v>
-      </c>
-      <c r="D5" s="34"/>
+        <v>4</v>
+      </c>
+      <c r="D5" s="97">
+        <v>4</v>
+      </c>
       <c r="E5" s="159"/>
       <c r="F5" s="42"/>
       <c r="G5" s="42"/>
@@ -8861,13 +8864,15 @@
     </row>
     <row r="6" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
       <c r="A6" s="70" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B6" s="68"/>
       <c r="C6" s="97">
         <v>1</v>
       </c>
-      <c r="D6" s="34"/>
+      <c r="D6" s="97">
+        <v>1</v>
+      </c>
       <c r="E6" s="159"/>
       <c r="F6" s="42"/>
       <c r="G6" s="42"/>
@@ -8885,13 +8890,15 @@
     </row>
     <row r="7" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
       <c r="A7" s="70" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B7" s="68"/>
       <c r="C7" s="97">
-        <v>4</v>
-      </c>
-      <c r="D7" s="34"/>
+        <v>1</v>
+      </c>
+      <c r="D7" s="97">
+        <v>1</v>
+      </c>
       <c r="E7" s="159"/>
       <c r="F7" s="42"/>
       <c r="G7" s="42"/>
@@ -8908,16 +8915,16 @@
       <c r="R7" s="48"/>
     </row>
     <row r="8" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A8" s="82" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="75">
-        <v>17</v>
-      </c>
+      <c r="A8" s="70" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="68"/>
       <c r="C8" s="97">
         <v>4</v>
       </c>
-      <c r="D8" s="34"/>
+      <c r="D8" s="97">
+        <v>4</v>
+      </c>
       <c r="E8" s="159"/>
       <c r="F8" s="42"/>
       <c r="G8" s="42"/>
@@ -8934,16 +8941,18 @@
       <c r="R8" s="48"/>
     </row>
     <row r="9" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A9" s="70" t="s">
-        <v>96</v>
+      <c r="A9" s="82" t="s">
+        <v>47</v>
       </c>
       <c r="B9" s="75">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="97">
         <v>4</v>
       </c>
-      <c r="D9" s="34"/>
+      <c r="D9" s="97">
+        <v>4</v>
+      </c>
       <c r="E9" s="159"/>
       <c r="F9" s="42"/>
       <c r="G9" s="42"/>
@@ -8961,15 +8970,17 @@
     </row>
     <row r="10" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
       <c r="A10" s="70" t="s">
-        <v>58</v>
+        <v>96</v>
       </c>
       <c r="B10" s="75">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="97">
-        <v>6</v>
-      </c>
-      <c r="D10" s="34"/>
+        <v>4</v>
+      </c>
+      <c r="D10" s="97">
+        <v>4</v>
+      </c>
       <c r="E10" s="159"/>
       <c r="F10" s="42"/>
       <c r="G10" s="42"/>
@@ -8986,90 +8997,96 @@
       <c r="R10" s="48"/>
     </row>
     <row r="11" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A11" s="89" t="s">
+      <c r="A11" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="75">
+        <v>19</v>
+      </c>
+      <c r="C11" s="97">
+        <v>6</v>
+      </c>
+      <c r="D11" s="97">
+        <v>6</v>
+      </c>
+      <c r="E11" s="159"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="42"/>
+      <c r="O11" s="42"/>
+      <c r="P11" s="42"/>
+      <c r="Q11" s="42"/>
+      <c r="R11" s="48"/>
+    </row>
+    <row r="12" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
+      <c r="A12" s="89" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="91"/>
-      <c r="C11" s="98"/>
-      <c r="D11" s="92"/>
-      <c r="E11" s="92"/>
-      <c r="F11" s="92"/>
-      <c r="G11" s="93"/>
-      <c r="H11" s="93"/>
-      <c r="I11" s="93"/>
-      <c r="J11" s="93"/>
-      <c r="K11" s="93"/>
-      <c r="L11" s="93"/>
-      <c r="M11" s="93"/>
-      <c r="N11" s="93"/>
-      <c r="O11" s="93"/>
-      <c r="P11" s="93"/>
-      <c r="Q11" s="93"/>
-      <c r="R11" s="48"/>
-    </row>
-    <row r="12" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A12" s="82" t="s">
+      <c r="B12" s="91"/>
+      <c r="C12" s="98"/>
+      <c r="D12" s="98"/>
+      <c r="E12" s="92"/>
+      <c r="F12" s="92"/>
+      <c r="G12" s="93"/>
+      <c r="H12" s="93"/>
+      <c r="I12" s="93"/>
+      <c r="J12" s="93"/>
+      <c r="K12" s="93"/>
+      <c r="L12" s="93"/>
+      <c r="M12" s="93"/>
+      <c r="N12" s="93"/>
+      <c r="O12" s="93"/>
+      <c r="P12" s="93"/>
+      <c r="Q12" s="93"/>
+      <c r="R12" s="48"/>
+    </row>
+    <row r="13" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
+      <c r="A13" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="75">
+      <c r="B13" s="75">
         <v>20</v>
-      </c>
-      <c r="C12" s="97">
-        <v>6</v>
-      </c>
-      <c r="D12" s="102"/>
-      <c r="E12" s="159"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="102"/>
-      <c r="I12" s="102"/>
-      <c r="J12" s="102"/>
-      <c r="K12" s="102"/>
-      <c r="L12" s="102"/>
-      <c r="M12" s="102"/>
-      <c r="N12" s="102"/>
-      <c r="O12" s="102"/>
-      <c r="P12" s="102"/>
-      <c r="Q12" s="102"/>
-      <c r="R12" s="171"/>
-    </row>
-    <row r="13" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A13" s="70" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="75">
-        <v>21</v>
       </c>
       <c r="C13" s="97">
         <v>6</v>
       </c>
-      <c r="D13" s="94"/>
+      <c r="D13" s="97">
+        <v>6</v>
+      </c>
       <c r="E13" s="159"/>
-      <c r="F13" s="159"/>
-      <c r="G13" s="159"/>
-      <c r="H13" s="94"/>
-      <c r="I13" s="94"/>
-      <c r="J13" s="94"/>
-      <c r="K13" s="94"/>
-      <c r="L13" s="94"/>
-      <c r="M13" s="94"/>
-      <c r="N13" s="94"/>
-      <c r="O13" s="94"/>
-      <c r="P13" s="94"/>
-      <c r="Q13" s="94"/>
-      <c r="R13" s="49"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="102"/>
+      <c r="I13" s="102"/>
+      <c r="J13" s="102"/>
+      <c r="K13" s="102"/>
+      <c r="L13" s="102"/>
+      <c r="M13" s="102"/>
+      <c r="N13" s="102"/>
+      <c r="O13" s="102"/>
+      <c r="P13" s="102"/>
+      <c r="Q13" s="102"/>
+      <c r="R13" s="163"/>
     </row>
     <row r="14" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A14" s="82" t="s">
-        <v>59</v>
+      <c r="A14" s="70" t="s">
+        <v>60</v>
       </c>
       <c r="B14" s="75">
-        <v>22</v>
-      </c>
-      <c r="C14" s="99">
+        <v>21</v>
+      </c>
+      <c r="C14" s="97">
         <v>6</v>
       </c>
-      <c r="D14" s="94"/>
+      <c r="D14" s="97">
+        <v>6</v>
+      </c>
       <c r="E14" s="159"/>
       <c r="F14" s="159"/>
       <c r="G14" s="159"/>
@@ -9086,585 +9103,579 @@
       <c r="R14" s="49"/>
     </row>
     <row r="15" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A15" s="89" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" s="92"/>
-      <c r="C15" s="98"/>
-      <c r="D15" s="91"/>
-      <c r="E15" s="92"/>
-      <c r="F15" s="92"/>
-      <c r="G15" s="92"/>
-      <c r="H15" s="92"/>
-      <c r="I15" s="92"/>
-      <c r="J15" s="92"/>
-      <c r="K15" s="92"/>
-      <c r="L15" s="92"/>
-      <c r="M15" s="92"/>
-      <c r="N15" s="92"/>
-      <c r="O15" s="92"/>
-      <c r="P15" s="92"/>
-      <c r="Q15" s="92"/>
+      <c r="A15" s="82" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="75">
+        <v>22</v>
+      </c>
+      <c r="C15" s="97">
+        <v>6</v>
+      </c>
+      <c r="D15" s="97">
+        <v>6</v>
+      </c>
+      <c r="E15" s="159"/>
+      <c r="F15" s="159"/>
+      <c r="G15" s="159"/>
+      <c r="H15" s="94"/>
+      <c r="I15" s="94"/>
+      <c r="J15" s="94"/>
+      <c r="K15" s="94"/>
+      <c r="L15" s="94"/>
+      <c r="M15" s="94"/>
+      <c r="N15" s="94"/>
+      <c r="O15" s="94"/>
+      <c r="P15" s="94"/>
+      <c r="Q15" s="94"/>
       <c r="R15" s="49"/>
     </row>
-    <row r="16" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A16" s="70" t="s">
-        <v>88</v>
-      </c>
-      <c r="B16" s="75">
-        <v>23</v>
-      </c>
-      <c r="C16" s="97">
-        <v>12</v>
-      </c>
-      <c r="D16" s="102"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="102"/>
-      <c r="I16" s="102"/>
-      <c r="J16" s="102"/>
-      <c r="K16" s="102"/>
-      <c r="L16" s="102"/>
-      <c r="M16" s="102"/>
-      <c r="N16" s="102"/>
-      <c r="O16" s="102"/>
-      <c r="P16" s="102"/>
-      <c r="Q16" s="102"/>
-      <c r="R16" s="171"/>
-    </row>
-    <row r="17" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A17" s="70" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="68">
-        <v>24</v>
-      </c>
-      <c r="C17" s="97">
-        <v>3</v>
-      </c>
-      <c r="D17" s="94"/>
-      <c r="E17" s="159"/>
-      <c r="F17" s="159"/>
-      <c r="G17" s="159"/>
-      <c r="H17" s="94"/>
-      <c r="I17" s="94"/>
-      <c r="J17" s="94"/>
-      <c r="K17" s="94"/>
-      <c r="L17" s="94"/>
-      <c r="M17" s="94"/>
-      <c r="N17" s="94"/>
-      <c r="O17" s="94"/>
-      <c r="P17" s="94"/>
-      <c r="Q17" s="94"/>
-      <c r="R17" s="49"/>
-    </row>
-    <row r="18" spans="1:120">
+    <row r="16" spans="1:120">
+      <c r="A16" s="38"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="38"/>
+      <c r="P16" s="38"/>
+      <c r="Q16" s="38"/>
+      <c r="R16" s="51"/>
+    </row>
+    <row r="17" spans="1:120">
+      <c r="A17" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="38">
+        <f>IF(ISBLANK(C5:C15), NA(), SUM(C5:C15))</f>
+        <v>42</v>
+      </c>
+      <c r="D17" s="38" t="e">
+        <f t="array" ref="D17">IF(ISBLANK(D3:D15), NA(), SUM(D3:D15))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E17" s="38" t="e">
+        <f t="array" ref="E17">IF(ISBLANK(E3:E15), NA(), SUM(E3:E15))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F17" s="38" t="e">
+        <f t="array" ref="F17">IF(ISBLANK(F3:F15), NA(), SUM(F3:F15))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G17" s="38" t="e">
+        <f t="array" ref="G17">IF(ISBLANK(G3:G15), NA(), SUM(G3:G15))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H17" s="38" t="e">
+        <f t="array" ref="H17">IF(ISBLANK(H3:H15), NA(), SUM(H3:H15))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I17" s="38" t="e">
+        <f t="array" ref="I17">IF(ISBLANK(I3:I15), NA(), SUM(I3:I15))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J17" s="38" t="e">
+        <f t="array" ref="J17">IF(ISBLANK(J3:J15), NA(), SUM(J3:J15))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K17" s="38" t="e">
+        <f t="array" ref="K17">IF(ISBLANK(K3:K15), NA(), SUM(K3:K15))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L17" s="38" t="e">
+        <f t="array" ref="L17">IF(ISBLANK(L3:L15), NA(), SUM(L3:L15))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M17" s="38" t="e">
+        <f t="array" ref="M17">IF(ISBLANK(M3:M15), NA(), SUM(M3:M15))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N17" s="38" t="e">
+        <f t="array" ref="N17">IF(ISBLANK(N3:N15), NA(), SUM(N3:N15))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O17" s="38" t="e">
+        <f t="array" ref="O17">IF(ISBLANK(O3:O15), NA(), SUM(O3:O15))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P17" s="38" t="e">
+        <f t="array" ref="P17">IF(ISBLANK(P3:P15), NA(), SUM(P3:P15))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q17" s="38" t="e">
+        <f t="array" ref="Q17">IF(ISBLANK(Q3:Q15), NA(), SUM(Q3:Q15))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R17" s="38" t="e">
+        <f t="array" ref="R17">IF(ISBLANK(R3:R15), NA(), SUM(R3:R15))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="S17" s="38"/>
+      <c r="T17" s="38"/>
+      <c r="U17" s="38"/>
+      <c r="V17" s="38"/>
+      <c r="W17" s="38"/>
+      <c r="X17" s="38"/>
+      <c r="Y17" s="38"/>
+      <c r="Z17" s="38"/>
+      <c r="AA17" s="38"/>
+      <c r="AB17" s="38"/>
+      <c r="AC17" s="38"/>
+      <c r="AD17" s="38"/>
+      <c r="AE17" s="38"/>
+      <c r="AF17" s="38"/>
+      <c r="AG17" s="38"/>
+      <c r="AH17" s="38"/>
+      <c r="AI17" s="38"/>
+      <c r="AJ17" s="38"/>
+      <c r="AK17" s="38"/>
+      <c r="AL17" s="38"/>
+      <c r="AM17" s="38"/>
+      <c r="AN17" s="38"/>
+      <c r="AO17" s="38"/>
+      <c r="AP17" s="38"/>
+      <c r="AQ17" s="38"/>
+      <c r="AR17" s="38"/>
+      <c r="AS17" s="38"/>
+      <c r="AT17" s="38"/>
+      <c r="AU17" s="38"/>
+      <c r="AV17" s="38"/>
+      <c r="AW17" s="38"/>
+      <c r="AX17" s="38"/>
+      <c r="AY17" s="38"/>
+      <c r="AZ17" s="38"/>
+      <c r="BA17" s="38"/>
+      <c r="BB17" s="38"/>
+      <c r="BC17" s="38"/>
+      <c r="BD17" s="38"/>
+      <c r="BE17" s="38"/>
+      <c r="BF17" s="38"/>
+      <c r="BG17" s="38"/>
+      <c r="BH17" s="38"/>
+      <c r="BI17" s="38"/>
+      <c r="BJ17" s="38"/>
+      <c r="BK17" s="38"/>
+      <c r="BL17" s="38"/>
+      <c r="BM17" s="38"/>
+      <c r="BN17" s="38"/>
+      <c r="BO17" s="38"/>
+      <c r="BP17" s="38"/>
+      <c r="BQ17" s="38"/>
+      <c r="BR17" s="38"/>
+      <c r="BS17" s="38"/>
+      <c r="BT17" s="38"/>
+      <c r="BU17" s="38"/>
+      <c r="BV17" s="38"/>
+      <c r="BW17" s="38"/>
+      <c r="BX17" s="38"/>
+      <c r="BY17" s="38"/>
+      <c r="BZ17" s="38"/>
+      <c r="CA17" s="38"/>
+      <c r="CB17" s="38"/>
+      <c r="CC17" s="38"/>
+      <c r="CD17" s="38"/>
+      <c r="CE17" s="38"/>
+      <c r="CF17" s="38"/>
+      <c r="CG17" s="38"/>
+      <c r="CH17" s="38"/>
+      <c r="CI17" s="38"/>
+      <c r="CJ17" s="38"/>
+      <c r="CK17" s="38"/>
+      <c r="CL17" s="38"/>
+      <c r="CM17" s="38"/>
+      <c r="CN17" s="38"/>
+      <c r="CO17" s="38"/>
+      <c r="CP17" s="38"/>
+      <c r="CQ17" s="38"/>
+      <c r="CR17" s="38"/>
+      <c r="CS17" s="38"/>
+      <c r="CT17" s="38"/>
+      <c r="CU17" s="38"/>
+      <c r="CV17" s="38"/>
+      <c r="CW17" s="38"/>
+      <c r="CX17" s="38"/>
+      <c r="CY17" s="38"/>
+      <c r="CZ17" s="38"/>
+      <c r="DA17" s="38"/>
+      <c r="DB17" s="38"/>
+      <c r="DC17" s="38"/>
+      <c r="DD17" s="38"/>
+      <c r="DE17" s="38"/>
+      <c r="DF17" s="38"/>
+      <c r="DG17" s="38"/>
+      <c r="DH17" s="38"/>
+      <c r="DI17" s="38"/>
+      <c r="DJ17" s="38"/>
+      <c r="DK17" s="38"/>
+      <c r="DL17" s="38"/>
+      <c r="DM17" s="38"/>
+      <c r="DN17" s="38"/>
+      <c r="DO17" s="38"/>
+      <c r="DP17" s="38"/>
+    </row>
+    <row r="18" spans="1:120" ht="25.5">
       <c r="A18" s="38"/>
-      <c r="B18" s="38"/>
+      <c r="B18" s="43" t="s">
+        <v>38</v>
+      </c>
       <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
-      <c r="L18" s="38"/>
-      <c r="M18" s="38"/>
-      <c r="N18" s="38"/>
-      <c r="O18" s="38"/>
-      <c r="P18" s="38"/>
-      <c r="Q18" s="38"/>
-      <c r="R18" s="51"/>
-    </row>
-    <row r="19" spans="1:120">
-      <c r="A19" s="54" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="43" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="38">
-        <f>IF(ISBLANK(C4:C17), NA(), SUM(C4:C17))</f>
-        <v>57</v>
-      </c>
-      <c r="D19" s="38" t="e">
-        <f t="array" ref="D19">IF(ISBLANK(D3:D17), NA(), SUM(D3:D17))</f>
+      <c r="D18" s="38" t="e">
+        <f>C17-D17</f>
         <v>#N/A</v>
       </c>
-      <c r="E19" s="38" t="e">
-        <f t="array" ref="E19">IF(ISBLANK(E3:E17), NA(), SUM(E3:E17))</f>
+      <c r="E18" s="38" t="e">
+        <f t="shared" ref="E18:R18" si="0">D17-E17</f>
         <v>#N/A</v>
       </c>
-      <c r="F19" s="38" t="e">
-        <f t="array" ref="F19">IF(ISBLANK(F3:F17), NA(), SUM(F3:F17))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G19" s="38" t="e">
-        <f t="array" ref="G19">IF(ISBLANK(G3:G17), NA(), SUM(G3:G17))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H19" s="38" t="e">
-        <f t="array" ref="H19">IF(ISBLANK(H3:H17), NA(), SUM(H3:H17))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I19" s="38" t="e">
-        <f t="array" ref="I19">IF(ISBLANK(I3:I17), NA(), SUM(I3:I17))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J19" s="38" t="e">
-        <f t="array" ref="J19">IF(ISBLANK(J3:J17), NA(), SUM(J3:J17))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K19" s="38" t="e">
-        <f t="array" ref="K19">IF(ISBLANK(K3:K17), NA(), SUM(K3:K17))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L19" s="38" t="e">
-        <f t="array" ref="L19">IF(ISBLANK(L3:L17), NA(), SUM(L3:L17))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M19" s="38" t="e">
-        <f t="array" ref="M19">IF(ISBLANK(M3:M17), NA(), SUM(M3:M17))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N19" s="38" t="e">
-        <f t="array" ref="N19">IF(ISBLANK(N3:N17), NA(), SUM(N3:N17))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O19" s="38" t="e">
-        <f t="array" ref="O19">IF(ISBLANK(O3:O17), NA(), SUM(O3:O17))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P19" s="38" t="e">
-        <f t="array" ref="P19">IF(ISBLANK(P3:P17), NA(), SUM(P3:P17))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q19" s="38" t="e">
-        <f t="array" ref="Q19">IF(ISBLANK(Q3:Q17), NA(), SUM(Q3:Q17))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R19" s="38" t="e">
-        <f t="array" ref="R19">IF(ISBLANK(R3:R17), NA(), SUM(R3:R17))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S19" s="38"/>
-      <c r="T19" s="38"/>
-      <c r="U19" s="38"/>
-      <c r="V19" s="38"/>
-      <c r="W19" s="38"/>
-      <c r="X19" s="38"/>
-      <c r="Y19" s="38"/>
-      <c r="Z19" s="38"/>
-      <c r="AA19" s="38"/>
-      <c r="AB19" s="38"/>
-      <c r="AC19" s="38"/>
-      <c r="AD19" s="38"/>
-      <c r="AE19" s="38"/>
-      <c r="AF19" s="38"/>
-      <c r="AG19" s="38"/>
-      <c r="AH19" s="38"/>
-      <c r="AI19" s="38"/>
-      <c r="AJ19" s="38"/>
-      <c r="AK19" s="38"/>
-      <c r="AL19" s="38"/>
-      <c r="AM19" s="38"/>
-      <c r="AN19" s="38"/>
-      <c r="AO19" s="38"/>
-      <c r="AP19" s="38"/>
-      <c r="AQ19" s="38"/>
-      <c r="AR19" s="38"/>
-      <c r="AS19" s="38"/>
-      <c r="AT19" s="38"/>
-      <c r="AU19" s="38"/>
-      <c r="AV19" s="38"/>
-      <c r="AW19" s="38"/>
-      <c r="AX19" s="38"/>
-      <c r="AY19" s="38"/>
-      <c r="AZ19" s="38"/>
-      <c r="BA19" s="38"/>
-      <c r="BB19" s="38"/>
-      <c r="BC19" s="38"/>
-      <c r="BD19" s="38"/>
-      <c r="BE19" s="38"/>
-      <c r="BF19" s="38"/>
-      <c r="BG19" s="38"/>
-      <c r="BH19" s="38"/>
-      <c r="BI19" s="38"/>
-      <c r="BJ19" s="38"/>
-      <c r="BK19" s="38"/>
-      <c r="BL19" s="38"/>
-      <c r="BM19" s="38"/>
-      <c r="BN19" s="38"/>
-      <c r="BO19" s="38"/>
-      <c r="BP19" s="38"/>
-      <c r="BQ19" s="38"/>
-      <c r="BR19" s="38"/>
-      <c r="BS19" s="38"/>
-      <c r="BT19" s="38"/>
-      <c r="BU19" s="38"/>
-      <c r="BV19" s="38"/>
-      <c r="BW19" s="38"/>
-      <c r="BX19" s="38"/>
-      <c r="BY19" s="38"/>
-      <c r="BZ19" s="38"/>
-      <c r="CA19" s="38"/>
-      <c r="CB19" s="38"/>
-      <c r="CC19" s="38"/>
-      <c r="CD19" s="38"/>
-      <c r="CE19" s="38"/>
-      <c r="CF19" s="38"/>
-      <c r="CG19" s="38"/>
-      <c r="CH19" s="38"/>
-      <c r="CI19" s="38"/>
-      <c r="CJ19" s="38"/>
-      <c r="CK19" s="38"/>
-      <c r="CL19" s="38"/>
-      <c r="CM19" s="38"/>
-      <c r="CN19" s="38"/>
-      <c r="CO19" s="38"/>
-      <c r="CP19" s="38"/>
-      <c r="CQ19" s="38"/>
-      <c r="CR19" s="38"/>
-      <c r="CS19" s="38"/>
-      <c r="CT19" s="38"/>
-      <c r="CU19" s="38"/>
-      <c r="CV19" s="38"/>
-      <c r="CW19" s="38"/>
-      <c r="CX19" s="38"/>
-      <c r="CY19" s="38"/>
-      <c r="CZ19" s="38"/>
-      <c r="DA19" s="38"/>
-      <c r="DB19" s="38"/>
-      <c r="DC19" s="38"/>
-      <c r="DD19" s="38"/>
-      <c r="DE19" s="38"/>
-      <c r="DF19" s="38"/>
-      <c r="DG19" s="38"/>
-      <c r="DH19" s="38"/>
-      <c r="DI19" s="38"/>
-      <c r="DJ19" s="38"/>
-      <c r="DK19" s="38"/>
-      <c r="DL19" s="38"/>
-      <c r="DM19" s="38"/>
-      <c r="DN19" s="38"/>
-      <c r="DO19" s="38"/>
-      <c r="DP19" s="38"/>
-    </row>
-    <row r="20" spans="1:120" ht="25.5">
-      <c r="A20" s="38"/>
-      <c r="B20" s="43" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38" t="e">
-        <f>C19-D19</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E20" s="38" t="e">
-        <f t="shared" ref="E20:R20" si="0">D19-E19</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F20" s="38" t="e">
+      <c r="F18" s="38" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="G20" s="38" t="e">
+      <c r="G18" s="38" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="H20" s="38" t="e">
+      <c r="H18" s="38" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="I20" s="38" t="e">
+      <c r="I18" s="38" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="J20" s="38" t="e">
+      <c r="J18" s="38" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="K20" s="38" t="e">
+      <c r="K18" s="38" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="L20" s="38" t="e">
+      <c r="L18" s="38" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="M20" s="38" t="e">
+      <c r="M18" s="38" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="N20" s="38" t="e">
+      <c r="N18" s="38" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="O20" s="38" t="e">
+      <c r="O18" s="38" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="P20" s="38" t="e">
+      <c r="P18" s="38" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="Q20" s="38" t="e">
+      <c r="Q18" s="38" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="R20" s="51" t="e">
+      <c r="R18" s="51" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="S20" s="38"/>
-      <c r="T20" s="38"/>
-      <c r="U20" s="38"/>
-      <c r="V20" s="38"/>
-      <c r="W20" s="38"/>
-      <c r="X20" s="38"/>
-      <c r="Y20" s="38"/>
-      <c r="Z20" s="38"/>
-      <c r="AA20" s="38"/>
-      <c r="AB20" s="38"/>
-      <c r="AC20" s="38"/>
-      <c r="AD20" s="38"/>
-      <c r="AE20" s="38"/>
-      <c r="AF20" s="38"/>
-      <c r="AG20" s="38"/>
-      <c r="AH20" s="38"/>
-      <c r="AI20" s="38"/>
-      <c r="AJ20" s="38"/>
-      <c r="AK20" s="38"/>
-      <c r="AL20" s="38"/>
-      <c r="AM20" s="38"/>
-      <c r="AN20" s="38"/>
-      <c r="AO20" s="38"/>
-      <c r="AP20" s="38"/>
-      <c r="AQ20" s="38"/>
-      <c r="AR20" s="38"/>
-      <c r="AS20" s="38"/>
-      <c r="AT20" s="38"/>
-      <c r="AU20" s="38"/>
-      <c r="AV20" s="38"/>
-      <c r="AW20" s="38"/>
-      <c r="AX20" s="38"/>
-      <c r="AY20" s="38"/>
-      <c r="AZ20" s="38"/>
-      <c r="BA20" s="38"/>
-      <c r="BB20" s="38"/>
-      <c r="BC20" s="38"/>
-      <c r="BD20" s="38"/>
-      <c r="BE20" s="38"/>
-      <c r="BF20" s="38"/>
-      <c r="BG20" s="38"/>
-      <c r="BH20" s="38"/>
-      <c r="BI20" s="38"/>
-      <c r="BJ20" s="38"/>
-      <c r="BK20" s="38"/>
-      <c r="BL20" s="38"/>
-      <c r="BM20" s="38"/>
-      <c r="BN20" s="38"/>
-      <c r="BO20" s="38"/>
-      <c r="BP20" s="38"/>
-      <c r="BQ20" s="38"/>
-      <c r="BR20" s="38"/>
-      <c r="BS20" s="38"/>
-      <c r="BT20" s="38"/>
-      <c r="BU20" s="38"/>
-      <c r="BV20" s="38"/>
-      <c r="BW20" s="38"/>
-      <c r="BX20" s="38"/>
-      <c r="BY20" s="38"/>
-      <c r="BZ20" s="38"/>
-      <c r="CA20" s="38"/>
-      <c r="CB20" s="38"/>
-      <c r="CC20" s="38"/>
-      <c r="CD20" s="38"/>
-      <c r="CE20" s="38"/>
-      <c r="CF20" s="38"/>
-      <c r="CG20" s="38"/>
-      <c r="CH20" s="38"/>
-      <c r="CI20" s="38"/>
-      <c r="CJ20" s="38"/>
-      <c r="CK20" s="38"/>
-      <c r="CL20" s="38"/>
-      <c r="CM20" s="38"/>
-      <c r="CN20" s="38"/>
-      <c r="CO20" s="38"/>
-      <c r="CP20" s="38"/>
-      <c r="CQ20" s="38"/>
-      <c r="CR20" s="38"/>
-      <c r="CS20" s="38"/>
-      <c r="CT20" s="38"/>
-      <c r="CU20" s="38"/>
-      <c r="CV20" s="38"/>
-      <c r="CW20" s="38"/>
-      <c r="CX20" s="38"/>
-      <c r="CY20" s="38"/>
-      <c r="CZ20" s="38"/>
-      <c r="DA20" s="38"/>
-      <c r="DB20" s="38"/>
-      <c r="DC20" s="38"/>
-      <c r="DD20" s="38"/>
-      <c r="DE20" s="38"/>
-      <c r="DF20" s="38"/>
-      <c r="DG20" s="38"/>
-      <c r="DH20" s="38"/>
-      <c r="DI20" s="38"/>
-      <c r="DJ20" s="38"/>
-      <c r="DK20" s="38"/>
-      <c r="DL20" s="38"/>
-      <c r="DM20" s="38"/>
-      <c r="DN20" s="38"/>
-      <c r="DO20" s="38"/>
-      <c r="DP20" s="38"/>
+      <c r="S18" s="38"/>
+      <c r="T18" s="38"/>
+      <c r="U18" s="38"/>
+      <c r="V18" s="38"/>
+      <c r="W18" s="38"/>
+      <c r="X18" s="38"/>
+      <c r="Y18" s="38"/>
+      <c r="Z18" s="38"/>
+      <c r="AA18" s="38"/>
+      <c r="AB18" s="38"/>
+      <c r="AC18" s="38"/>
+      <c r="AD18" s="38"/>
+      <c r="AE18" s="38"/>
+      <c r="AF18" s="38"/>
+      <c r="AG18" s="38"/>
+      <c r="AH18" s="38"/>
+      <c r="AI18" s="38"/>
+      <c r="AJ18" s="38"/>
+      <c r="AK18" s="38"/>
+      <c r="AL18" s="38"/>
+      <c r="AM18" s="38"/>
+      <c r="AN18" s="38"/>
+      <c r="AO18" s="38"/>
+      <c r="AP18" s="38"/>
+      <c r="AQ18" s="38"/>
+      <c r="AR18" s="38"/>
+      <c r="AS18" s="38"/>
+      <c r="AT18" s="38"/>
+      <c r="AU18" s="38"/>
+      <c r="AV18" s="38"/>
+      <c r="AW18" s="38"/>
+      <c r="AX18" s="38"/>
+      <c r="AY18" s="38"/>
+      <c r="AZ18" s="38"/>
+      <c r="BA18" s="38"/>
+      <c r="BB18" s="38"/>
+      <c r="BC18" s="38"/>
+      <c r="BD18" s="38"/>
+      <c r="BE18" s="38"/>
+      <c r="BF18" s="38"/>
+      <c r="BG18" s="38"/>
+      <c r="BH18" s="38"/>
+      <c r="BI18" s="38"/>
+      <c r="BJ18" s="38"/>
+      <c r="BK18" s="38"/>
+      <c r="BL18" s="38"/>
+      <c r="BM18" s="38"/>
+      <c r="BN18" s="38"/>
+      <c r="BO18" s="38"/>
+      <c r="BP18" s="38"/>
+      <c r="BQ18" s="38"/>
+      <c r="BR18" s="38"/>
+      <c r="BS18" s="38"/>
+      <c r="BT18" s="38"/>
+      <c r="BU18" s="38"/>
+      <c r="BV18" s="38"/>
+      <c r="BW18" s="38"/>
+      <c r="BX18" s="38"/>
+      <c r="BY18" s="38"/>
+      <c r="BZ18" s="38"/>
+      <c r="CA18" s="38"/>
+      <c r="CB18" s="38"/>
+      <c r="CC18" s="38"/>
+      <c r="CD18" s="38"/>
+      <c r="CE18" s="38"/>
+      <c r="CF18" s="38"/>
+      <c r="CG18" s="38"/>
+      <c r="CH18" s="38"/>
+      <c r="CI18" s="38"/>
+      <c r="CJ18" s="38"/>
+      <c r="CK18" s="38"/>
+      <c r="CL18" s="38"/>
+      <c r="CM18" s="38"/>
+      <c r="CN18" s="38"/>
+      <c r="CO18" s="38"/>
+      <c r="CP18" s="38"/>
+      <c r="CQ18" s="38"/>
+      <c r="CR18" s="38"/>
+      <c r="CS18" s="38"/>
+      <c r="CT18" s="38"/>
+      <c r="CU18" s="38"/>
+      <c r="CV18" s="38"/>
+      <c r="CW18" s="38"/>
+      <c r="CX18" s="38"/>
+      <c r="CY18" s="38"/>
+      <c r="CZ18" s="38"/>
+      <c r="DA18" s="38"/>
+      <c r="DB18" s="38"/>
+      <c r="DC18" s="38"/>
+      <c r="DD18" s="38"/>
+      <c r="DE18" s="38"/>
+      <c r="DF18" s="38"/>
+      <c r="DG18" s="38"/>
+      <c r="DH18" s="38"/>
+      <c r="DI18" s="38"/>
+      <c r="DJ18" s="38"/>
+      <c r="DK18" s="38"/>
+      <c r="DL18" s="38"/>
+      <c r="DM18" s="38"/>
+      <c r="DN18" s="38"/>
+      <c r="DO18" s="38"/>
+      <c r="DP18" s="38"/>
+    </row>
+    <row r="19" spans="1:120">
+      <c r="A19" s="38"/>
+      <c r="B19" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="45">
+        <f>C17</f>
+        <v>42</v>
+      </c>
+      <c r="D19" s="46">
+        <f>C19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <v>39.200000000000003</v>
+      </c>
+      <c r="E19" s="46">
+        <f>D19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <v>36.400000000000006</v>
+      </c>
+      <c r="F19" s="46">
+        <f>E19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <v>33.600000000000009</v>
+      </c>
+      <c r="G19" s="46">
+        <f>F19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <v>30.800000000000008</v>
+      </c>
+      <c r="H19" s="46">
+        <f>G19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <v>28.000000000000007</v>
+      </c>
+      <c r="I19" s="46">
+        <f>H19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <v>25.200000000000006</v>
+      </c>
+      <c r="J19" s="46">
+        <f>I19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <v>22.400000000000006</v>
+      </c>
+      <c r="K19" s="46">
+        <f>J19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <v>19.600000000000005</v>
+      </c>
+      <c r="L19" s="46">
+        <f>K19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <v>16.800000000000004</v>
+      </c>
+      <c r="M19" s="46">
+        <f>L19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <v>14.000000000000004</v>
+      </c>
+      <c r="N19" s="46">
+        <f>M19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <v>11.200000000000003</v>
+      </c>
+      <c r="O19" s="46">
+        <f>N19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <v>8.4000000000000021</v>
+      </c>
+      <c r="P19" s="46">
+        <f>O19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <v>5.6000000000000023</v>
+      </c>
+      <c r="Q19" s="46">
+        <f>P19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <v>2.8000000000000025</v>
+      </c>
+      <c r="R19" s="46">
+        <f>Q19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:120" s="56" customFormat="1">
+      <c r="A20" s="55"/>
+      <c r="B20" s="57" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="58">
+        <f>1-C17/$C$17</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="58" t="e">
+        <f t="shared" ref="D20:R20" si="1">1-D17/$C$17</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E20" s="58" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F20" s="58" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="G20" s="58" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H20" s="58" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="I20" s="58" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J20" s="58" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="K20" s="58" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="L20" s="58" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M20" s="58" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N20" s="58" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="O20" s="58" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P20" s="58" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q20" s="58" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R20" s="58" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="21" spans="1:120">
       <c r="A21" s="38"/>
-      <c r="B21" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="45">
-        <f>C19</f>
-        <v>57</v>
-      </c>
-      <c r="D21" s="46">
-        <f>C21-$C$19/COUNTA($C$2:$Q$2)</f>
-        <v>53.2</v>
-      </c>
-      <c r="E21" s="46">
-        <f t="shared" ref="E21:R21" si="1">D21-$C$19/COUNTA($C$2:$Q$2)</f>
-        <v>49.400000000000006</v>
-      </c>
-      <c r="F21" s="46">
-        <f t="shared" si="1"/>
-        <v>45.600000000000009</v>
-      </c>
-      <c r="G21" s="46">
-        <f t="shared" si="1"/>
-        <v>41.800000000000011</v>
-      </c>
-      <c r="H21" s="46">
-        <f t="shared" si="1"/>
-        <v>38.000000000000014</v>
-      </c>
-      <c r="I21" s="46">
-        <f t="shared" si="1"/>
-        <v>34.200000000000017</v>
-      </c>
-      <c r="J21" s="46">
-        <f t="shared" si="1"/>
-        <v>30.400000000000016</v>
-      </c>
-      <c r="K21" s="46">
-        <f t="shared" si="1"/>
-        <v>26.600000000000016</v>
-      </c>
-      <c r="L21" s="46">
-        <f t="shared" si="1"/>
-        <v>22.800000000000015</v>
-      </c>
-      <c r="M21" s="46">
-        <f t="shared" si="1"/>
-        <v>19.000000000000014</v>
-      </c>
-      <c r="N21" s="46">
-        <f t="shared" si="1"/>
-        <v>15.200000000000014</v>
-      </c>
-      <c r="O21" s="46">
-        <f t="shared" si="1"/>
-        <v>11.400000000000013</v>
-      </c>
-      <c r="P21" s="46">
-        <f t="shared" si="1"/>
-        <v>7.600000000000013</v>
-      </c>
-      <c r="Q21" s="46">
-        <f t="shared" si="1"/>
-        <v>3.8000000000000131</v>
-      </c>
-      <c r="R21" s="46">
-        <f t="shared" si="1"/>
-        <v>1.3322676295501878E-14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:120" s="56" customFormat="1">
-      <c r="A22" s="55"/>
-      <c r="B22" s="57" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="58">
-        <f>1-C19/$C$19</f>
-        <v>0</v>
-      </c>
-      <c r="D22" s="58" t="e">
-        <f t="shared" ref="D22:R22" si="2">1-D19/$C$19</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E22" s="58" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F22" s="58" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="G22" s="58" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H22" s="58" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I22" s="58" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J22" s="58" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="K22" s="58" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="L22" s="58" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M22" s="58" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="N22" s="58" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="O22" s="58" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="P22" s="58" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="Q22" s="58" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R22" s="58" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="38"/>
+      <c r="O21" s="38"/>
+      <c r="P21" s="38"/>
+      <c r="Q21" s="38"/>
+      <c r="R21" s="38"/>
+    </row>
+    <row r="22" spans="1:120">
+      <c r="A22" s="38"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="38"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="38"/>
+      <c r="P22" s="38"/>
+      <c r="Q22" s="38"/>
+      <c r="R22" s="38"/>
     </row>
     <row r="23" spans="1:120">
       <c r="A23" s="38"/>
-      <c r="B23" s="38"/>
+      <c r="B23" s="43"/>
       <c r="C23" s="38"/>
       <c r="D23" s="38"/>
       <c r="E23" s="38"/>
@@ -9684,9 +9695,9 @@
     </row>
     <row r="24" spans="1:120">
       <c r="A24" s="38"/>
-      <c r="B24" s="43"/>
+      <c r="B24" s="38"/>
       <c r="C24" s="38"/>
-      <c r="D24" s="43"/>
+      <c r="D24" s="38"/>
       <c r="E24" s="38"/>
       <c r="F24" s="38"/>
       <c r="G24" s="38"/>
@@ -9704,7 +9715,7 @@
     </row>
     <row r="25" spans="1:120">
       <c r="A25" s="38"/>
-      <c r="B25" s="43"/>
+      <c r="B25" s="38"/>
       <c r="C25" s="38"/>
       <c r="D25" s="38"/>
       <c r="E25" s="38"/>
@@ -10922,60 +10933,12 @@
       <c r="Q85" s="38"/>
       <c r="R85" s="38"/>
     </row>
-    <row r="86" spans="1:18">
-      <c r="A86" s="38"/>
-      <c r="B86" s="38"/>
-      <c r="C86" s="38"/>
-      <c r="D86" s="38"/>
-      <c r="E86" s="38"/>
-      <c r="F86" s="38"/>
-      <c r="G86" s="38"/>
-      <c r="H86" s="38"/>
-      <c r="I86" s="38"/>
-      <c r="J86" s="38"/>
-      <c r="K86" s="38"/>
-      <c r="L86" s="38"/>
-      <c r="M86" s="38"/>
-      <c r="N86" s="38"/>
-      <c r="O86" s="38"/>
-      <c r="P86" s="38"/>
-      <c r="Q86" s="38"/>
-      <c r="R86" s="38"/>
-    </row>
-    <row r="87" spans="1:18">
-      <c r="A87" s="38"/>
-      <c r="B87" s="38"/>
-      <c r="C87" s="38"/>
-      <c r="D87" s="38"/>
-      <c r="E87" s="38"/>
-      <c r="F87" s="38"/>
-      <c r="G87" s="38"/>
-      <c r="H87" s="38"/>
-      <c r="I87" s="38"/>
-      <c r="J87" s="38"/>
-      <c r="K87" s="38"/>
-      <c r="L87" s="38"/>
-      <c r="M87" s="38"/>
-      <c r="N87" s="38"/>
-      <c r="O87" s="38"/>
-      <c r="P87" s="38"/>
-      <c r="Q87" s="38"/>
-      <c r="R87" s="38"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="E13:R15 D13:D14 D3:R11 D17:R17 A3:A17 A16:B16 B3:B10 B12:B17 E12:G12 E16:G16 C4:C7">
-    <cfRule type="expression" dxfId="5" priority="37" stopIfTrue="1">
+  <conditionalFormatting sqref="D14:R15 D3:R12 B13:B15 E13:G13 B3:B11 A3:A15 C5:D8">
+    <cfRule type="expression" dxfId="3" priority="37" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="38" stopIfTrue="1">
-      <formula>#REF!="O"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8:B10 A9">
-    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
-      <formula>#REF!="N"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="38" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Edition d'un art/media fonctionne avec le nouveau modèle de Data
</commit_message>
<xml_diff>
--- a/doc/Backlog [ACONIT].xlsx
+++ b/doc/Backlog [ACONIT].xlsx
@@ -39,10 +39,10 @@
   </definedNames>
   <calcPr calcId="125725"/>
   <customWorkbookViews>
+    <customWorkbookView name="Bernard Notarianni - Affichage personnalisé" guid="{178C21D0-B00A-4B0E-B009-71AAC80909BC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="785" activeSheetId="1"/>
+    <customWorkbookView name="Didier Lassissi - Affichage personnalisé" guid="{5E22A59B-ECE7-4B50-9619-81A99F53295A}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1064" windowHeight="552" activeSheetId="1"/>
+    <customWorkbookView name="uvba7442 - Affichage personnalisé" guid="{38566435-C99E-4958-9169-0C5C493EE97D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1213" windowHeight="665" activeSheetId="1"/>
     <customWorkbookView name="Yoann Regardin - Affichage personnalisé" guid="{29B12ED2-AD48-4E1C-B971-77E4D76C1B5F}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="609" activeSheetId="2"/>
-    <customWorkbookView name="uvba7442 - Affichage personnalisé" guid="{38566435-C99E-4958-9169-0C5C493EE97D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1213" windowHeight="665" activeSheetId="1"/>
-    <customWorkbookView name="Didier Lassissi - Affichage personnalisé" guid="{5E22A59B-ECE7-4B50-9619-81A99F53295A}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1064" windowHeight="552" activeSheetId="1"/>
-    <customWorkbookView name="Bernard Notarianni - Affichage personnalisé" guid="{178C21D0-B00A-4B0E-B009-71AAC80909BC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="785" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
@@ -1631,6 +1631,42 @@
     <xf numFmtId="0" fontId="1" fillId="29" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="13" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="43" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="13" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1654,42 +1690,6 @@
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="13" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="43" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="13" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1738,35 +1738,7 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vérification" xfId="42" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="36">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="51"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="51"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="32">
     <dxf>
       <fill>
         <patternFill>
@@ -2099,7 +2071,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225287"/>
+          <c:x val="0.37032576667225298"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2117,9 +2089,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532429"/>
+          <c:y val="0.15742128935532435"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192314"/>
+          <c:h val="0.70464767616192325"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2429,11 +2401,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="89847680"/>
-        <c:axId val="93339648"/>
+        <c:axId val="101373824"/>
+        <c:axId val="101728256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="89847680"/>
+        <c:axId val="101373824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2465,7 +2437,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93339648"/>
+        <c:crossAx val="101728256"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2473,7 +2445,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93339648"/>
+        <c:axId val="101728256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2515,7 +2487,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89847680"/>
+        <c:crossAx val="101373824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2603,7 +2575,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000161" footer="0.49212598450000161"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000167" footer="0.49212598450000167"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2640,7 +2612,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225309"/>
+          <c:x val="0.37032576667225325"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2658,9 +2630,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532443"/>
+          <c:y val="0.15742128935532448"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192336"/>
+          <c:h val="0.70464767616192359"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2970,11 +2942,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="93696768"/>
-        <c:axId val="93698688"/>
+        <c:axId val="102085376"/>
+        <c:axId val="102087296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="93696768"/>
+        <c:axId val="102085376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3006,7 +2978,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93698688"/>
+        <c:crossAx val="102087296"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3014,7 +2986,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93698688"/>
+        <c:axId val="102087296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3056,7 +3028,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93696768"/>
+        <c:crossAx val="102085376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3144,7 +3116,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000172" footer="0.49212598450000172"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000178" footer="0.49212598450000178"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3181,7 +3153,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225342"/>
+          <c:x val="0.37032576667225353"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3199,9 +3171,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532454"/>
+          <c:y val="0.1574212893553246"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192381"/>
+          <c:h val="0.70464767616192392"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3511,11 +3483,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="93760512"/>
-        <c:axId val="93762688"/>
+        <c:axId val="102157312"/>
+        <c:axId val="102159488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="93760512"/>
+        <c:axId val="102157312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3547,7 +3519,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93762688"/>
+        <c:crossAx val="102159488"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3555,7 +3527,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93762688"/>
+        <c:axId val="102159488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3597,7 +3569,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93760512"/>
+        <c:crossAx val="102157312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3685,7 +3657,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000183" footer="0.49212598450000183"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000189" footer="0.49212598450000189"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3722,7 +3694,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.3703257666722537"/>
+          <c:x val="0.37032576667225386"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3740,9 +3712,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532468"/>
+          <c:y val="0.15742128935532476"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192403"/>
+          <c:h val="0.70464767616192414"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -4052,11 +4024,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="93550080"/>
-        <c:axId val="93552000"/>
+        <c:axId val="101946880"/>
+        <c:axId val="101948800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="93550080"/>
+        <c:axId val="101946880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4088,7 +4060,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93552000"/>
+        <c:crossAx val="101948800"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -4096,7 +4068,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93552000"/>
+        <c:axId val="101948800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4138,7 +4110,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93550080"/>
+        <c:crossAx val="101946880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4226,7 +4198,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000195" footer="0.49212598450000195"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.492125984500002" footer="0.492125984500002"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -4242,10 +4214,10 @@
       <xdr:rowOff>31826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>156884</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>28385</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>705971</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4274,15 +4246,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>120428</xdr:colOff>
+      <xdr:colOff>120427</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>127076</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>99734</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>717175</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4698,10 +4670,10 @@
         <v>18</v>
       </c>
       <c r="C1" s="25"/>
-      <c r="D1" s="171" t="s">
+      <c r="D1" s="183" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="171"/>
+      <c r="E1" s="183"/>
       <c r="F1" s="24"/>
       <c r="G1" s="24"/>
       <c r="H1" s="15"/>
@@ -4713,10 +4685,10 @@
       <c r="A2" s="64"/>
       <c r="B2" s="16"/>
       <c r="C2" s="14"/>
-      <c r="D2" s="172" t="s">
+      <c r="D2" s="184" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="173"/>
+      <c r="E2" s="185"/>
       <c r="F2" s="26"/>
       <c r="G2" s="59"/>
       <c r="H2" s="3"/>
@@ -4732,8 +4704,8 @@
         <f>MAX(A13:A48)+1</f>
         <v>35</v>
       </c>
-      <c r="D3" s="166"/>
-      <c r="E3" s="167"/>
+      <c r="D3" s="178"/>
+      <c r="E3" s="179"/>
       <c r="F3" s="26"/>
       <c r="G3" s="59"/>
       <c r="H3" s="3"/>
@@ -4741,9 +4713,9 @@
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:13" hidden="1">
-      <c r="A4" s="168"/>
-      <c r="B4" s="169"/>
-      <c r="C4" s="170"/>
+      <c r="A4" s="180"/>
+      <c r="B4" s="181"/>
+      <c r="C4" s="182"/>
       <c r="D4" s="17"/>
       <c r="E4" s="5"/>
       <c r="F4" s="27"/>
@@ -6099,10 +6071,10 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A54:A55 B48:C48 D49:E51 H48:K48 A46:A49 B37:E37 D15 D38:E38 D41 B36:C37 H36:K37 E36:E37 A35:A43 D26 B28:C31 A13:A22 H28:K31 D20:E21 E25:E26 A25:A31 D28 D30 E28:E31 B12:E12 D13:E13 B13:C17 H12:K17 E13:E15 E17:E19">
-    <cfRule type="expression" dxfId="35" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="49" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="50" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6117,7 +6089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:DP82"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
@@ -8636,18 +8608,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11 A3:B11 F3:G7 H3:R11">
-    <cfRule type="expression" dxfId="33" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="53" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="54" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B10 A3:A7 A11:B11">
-    <cfRule type="expression" dxfId="31" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="31" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="32" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8663,7 +8635,7 @@
   <dimension ref="A1:DP85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -8890,21 +8862,21 @@
       <c r="E4" s="153">
         <v>6</v>
       </c>
-      <c r="F4" s="174">
+      <c r="F4" s="166">
         <v>5</v>
       </c>
-      <c r="G4" s="175"/>
-      <c r="H4" s="176"/>
-      <c r="I4" s="175"/>
-      <c r="J4" s="175"/>
-      <c r="K4" s="175"/>
-      <c r="L4" s="175"/>
-      <c r="M4" s="175"/>
-      <c r="N4" s="175"/>
-      <c r="O4" s="175"/>
-      <c r="P4" s="175"/>
-      <c r="Q4" s="175"/>
-      <c r="R4" s="175"/>
+      <c r="G4" s="167"/>
+      <c r="H4" s="168"/>
+      <c r="I4" s="167"/>
+      <c r="J4" s="167"/>
+      <c r="K4" s="167"/>
+      <c r="L4" s="167"/>
+      <c r="M4" s="167"/>
+      <c r="N4" s="167"/>
+      <c r="O4" s="167"/>
+      <c r="P4" s="167"/>
+      <c r="Q4" s="167"/>
+      <c r="R4" s="171"/>
     </row>
     <row r="5" spans="1:120" s="162" customFormat="1" ht="24.95" customHeight="1">
       <c r="A5" s="159" t="s">
@@ -8920,21 +8892,21 @@
       <c r="E5" s="155">
         <v>1</v>
       </c>
-      <c r="F5" s="174">
+      <c r="F5" s="166">
         <v>0</v>
       </c>
-      <c r="G5" s="175"/>
-      <c r="H5" s="176"/>
-      <c r="I5" s="175"/>
-      <c r="J5" s="175"/>
-      <c r="K5" s="175"/>
-      <c r="L5" s="175"/>
-      <c r="M5" s="175"/>
-      <c r="N5" s="175"/>
-      <c r="O5" s="175"/>
-      <c r="P5" s="175"/>
-      <c r="Q5" s="175"/>
-      <c r="R5" s="175"/>
+      <c r="G5" s="167"/>
+      <c r="H5" s="168"/>
+      <c r="I5" s="167"/>
+      <c r="J5" s="167"/>
+      <c r="K5" s="167"/>
+      <c r="L5" s="167"/>
+      <c r="M5" s="167"/>
+      <c r="N5" s="167"/>
+      <c r="O5" s="167"/>
+      <c r="P5" s="167"/>
+      <c r="Q5" s="167"/>
+      <c r="R5" s="171"/>
     </row>
     <row r="6" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
       <c r="A6" s="70" t="s">
@@ -8954,7 +8926,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="156"/>
-      <c r="H6" s="177"/>
+      <c r="H6" s="169"/>
       <c r="I6" s="156"/>
       <c r="J6" s="156"/>
       <c r="K6" s="156"/>
@@ -8964,7 +8936,7 @@
       <c r="O6" s="156"/>
       <c r="P6" s="156"/>
       <c r="Q6" s="156"/>
-      <c r="R6" s="178"/>
+      <c r="R6" s="170"/>
     </row>
     <row r="7" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
       <c r="A7" s="70" t="s">
@@ -8984,7 +8956,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="156"/>
-      <c r="H7" s="177"/>
+      <c r="H7" s="169"/>
       <c r="I7" s="156"/>
       <c r="J7" s="156"/>
       <c r="K7" s="156"/>
@@ -8994,7 +8966,7 @@
       <c r="O7" s="156"/>
       <c r="P7" s="156"/>
       <c r="Q7" s="156"/>
-      <c r="R7" s="178"/>
+      <c r="R7" s="170"/>
     </row>
     <row r="8" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
       <c r="A8" s="70" t="s">
@@ -9010,11 +8982,11 @@
       <c r="E8" s="153">
         <v>2</v>
       </c>
-      <c r="F8" s="174">
+      <c r="F8" s="166">
         <v>1</v>
       </c>
       <c r="G8" s="156"/>
-      <c r="H8" s="177"/>
+      <c r="H8" s="169"/>
       <c r="I8" s="156"/>
       <c r="J8" s="156"/>
       <c r="K8" s="156"/>
@@ -9024,7 +8996,7 @@
       <c r="O8" s="156"/>
       <c r="P8" s="156"/>
       <c r="Q8" s="156"/>
-      <c r="R8" s="178"/>
+      <c r="R8" s="170"/>
     </row>
     <row r="9" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
       <c r="A9" s="82" t="s">
@@ -9046,7 +9018,7 @@
         <v>5</v>
       </c>
       <c r="G9" s="156"/>
-      <c r="H9" s="177"/>
+      <c r="H9" s="169"/>
       <c r="I9" s="156"/>
       <c r="J9" s="156"/>
       <c r="K9" s="156"/>
@@ -9056,7 +9028,7 @@
       <c r="O9" s="156"/>
       <c r="P9" s="156"/>
       <c r="Q9" s="156"/>
-      <c r="R9" s="178"/>
+      <c r="R9" s="170"/>
     </row>
     <row r="10" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
       <c r="A10" s="70" t="s">
@@ -9078,7 +9050,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="156"/>
-      <c r="H10" s="177"/>
+      <c r="H10" s="169"/>
       <c r="I10" s="156"/>
       <c r="J10" s="156"/>
       <c r="K10" s="156"/>
@@ -9088,7 +9060,7 @@
       <c r="O10" s="156"/>
       <c r="P10" s="156"/>
       <c r="Q10" s="156"/>
-      <c r="R10" s="178"/>
+      <c r="R10" s="170"/>
     </row>
     <row r="11" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
       <c r="A11" s="70" t="s">
@@ -9110,7 +9082,7 @@
         <v>6</v>
       </c>
       <c r="G11" s="156"/>
-      <c r="H11" s="177"/>
+      <c r="H11" s="169"/>
       <c r="I11" s="156"/>
       <c r="J11" s="156"/>
       <c r="K11" s="156"/>
@@ -9120,7 +9092,7 @@
       <c r="O11" s="156"/>
       <c r="P11" s="156"/>
       <c r="Q11" s="156"/>
-      <c r="R11" s="178"/>
+      <c r="R11" s="170"/>
     </row>
     <row r="12" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
       <c r="A12" s="89" t="s">
@@ -9131,18 +9103,18 @@
       <c r="D12" s="91"/>
       <c r="E12" s="91"/>
       <c r="F12" s="91"/>
-      <c r="G12" s="179"/>
-      <c r="H12" s="180"/>
-      <c r="I12" s="179"/>
-      <c r="J12" s="179"/>
-      <c r="K12" s="179"/>
-      <c r="L12" s="179"/>
-      <c r="M12" s="179"/>
-      <c r="N12" s="179"/>
-      <c r="O12" s="179"/>
-      <c r="P12" s="179"/>
-      <c r="Q12" s="179"/>
-      <c r="R12" s="178"/>
+      <c r="G12" s="171"/>
+      <c r="H12" s="172"/>
+      <c r="I12" s="171"/>
+      <c r="J12" s="171"/>
+      <c r="K12" s="171"/>
+      <c r="L12" s="171"/>
+      <c r="M12" s="171"/>
+      <c r="N12" s="171"/>
+      <c r="O12" s="171"/>
+      <c r="P12" s="171"/>
+      <c r="Q12" s="171"/>
+      <c r="R12" s="170"/>
     </row>
     <row r="13" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
       <c r="A13" s="82" t="s">
@@ -9164,17 +9136,17 @@
         <v>6</v>
       </c>
       <c r="G13" s="156"/>
-      <c r="H13" s="181"/>
-      <c r="I13" s="182"/>
-      <c r="J13" s="182"/>
-      <c r="K13" s="182"/>
-      <c r="L13" s="182"/>
-      <c r="M13" s="182"/>
-      <c r="N13" s="182"/>
-      <c r="O13" s="182"/>
-      <c r="P13" s="182"/>
-      <c r="Q13" s="182"/>
-      <c r="R13" s="183"/>
+      <c r="H13" s="173"/>
+      <c r="I13" s="174"/>
+      <c r="J13" s="174"/>
+      <c r="K13" s="174"/>
+      <c r="L13" s="174"/>
+      <c r="M13" s="174"/>
+      <c r="N13" s="174"/>
+      <c r="O13" s="174"/>
+      <c r="P13" s="174"/>
+      <c r="Q13" s="174"/>
+      <c r="R13" s="175"/>
     </row>
     <row r="14" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
       <c r="A14" s="70" t="s">
@@ -9196,7 +9168,7 @@
         <v>6</v>
       </c>
       <c r="G14" s="105"/>
-      <c r="H14" s="184"/>
+      <c r="H14" s="176"/>
       <c r="I14" s="155"/>
       <c r="J14" s="155"/>
       <c r="K14" s="155"/>
@@ -9206,7 +9178,7 @@
       <c r="O14" s="155"/>
       <c r="P14" s="155"/>
       <c r="Q14" s="155"/>
-      <c r="R14" s="185"/>
+      <c r="R14" s="177"/>
     </row>
     <row r="15" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
       <c r="A15" s="82" t="s">
@@ -9228,7 +9200,7 @@
         <v>6</v>
       </c>
       <c r="G15" s="105"/>
-      <c r="H15" s="184"/>
+      <c r="H15" s="176"/>
       <c r="I15" s="155"/>
       <c r="J15" s="155"/>
       <c r="K15" s="155"/>
@@ -9238,7 +9210,7 @@
       <c r="O15" s="155"/>
       <c r="P15" s="155"/>
       <c r="Q15" s="155"/>
-      <c r="R15" s="185"/>
+      <c r="R15" s="177"/>
     </row>
     <row r="16" spans="1:120">
       <c r="A16" s="38"/>
@@ -9613,63 +9585,63 @@
         <v>49</v>
       </c>
       <c r="D19" s="46">
-        <f>C19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" ref="D19:R19" si="1">C19-$C$17/COUNTA($C$2:$Q$2)</f>
         <v>45.733333333333334</v>
       </c>
       <c r="E19" s="46">
-        <f>D19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>42.466666666666669</v>
       </c>
       <c r="F19" s="46">
-        <f>E19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>39.200000000000003</v>
       </c>
       <c r="G19" s="46">
-        <f>F19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>35.933333333333337</v>
       </c>
       <c r="H19" s="46">
-        <f>G19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>32.666666666666671</v>
       </c>
       <c r="I19" s="46">
-        <f>H19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>29.400000000000006</v>
       </c>
       <c r="J19" s="46">
-        <f>I19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>26.13333333333334</v>
       </c>
       <c r="K19" s="46">
-        <f>J19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>22.866666666666674</v>
       </c>
       <c r="L19" s="46">
-        <f>K19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>19.600000000000009</v>
       </c>
       <c r="M19" s="46">
-        <f>L19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>16.333333333333343</v>
       </c>
       <c r="N19" s="46">
-        <f>M19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>13.066666666666677</v>
       </c>
       <c r="O19" s="46">
-        <f>N19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>9.8000000000000114</v>
       </c>
       <c r="P19" s="46">
-        <f>O19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>6.5333333333333448</v>
       </c>
       <c r="Q19" s="46">
-        <f>P19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>3.2666666666666782</v>
       </c>
       <c r="R19" s="46">
-        <f>Q19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>1.1546319456101628E-14</v>
       </c>
     </row>
@@ -9683,63 +9655,63 @@
         <v>0</v>
       </c>
       <c r="D20" s="58">
-        <f t="shared" ref="D20:R20" si="1">1-D17/$C$17</f>
+        <f t="shared" ref="D20:R20" si="2">1-D17/$C$17</f>
         <v>0</v>
       </c>
       <c r="E20" s="58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.12244897959183676</v>
       </c>
       <c r="F20" s="58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.18367346938775508</v>
       </c>
       <c r="G20" s="58" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="H20" s="58" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="I20" s="58" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="J20" s="58" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="K20" s="58" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="L20" s="58" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="M20" s="58" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="N20" s="58" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="O20" s="58" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="P20" s="58" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="Q20" s="58" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="R20" s="58" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -11045,10 +11017,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B13:B15 E13:G13 B3:B11 A3:A15 C6:D8 D14:R15 D3:R12">
-    <cfRule type="expression" dxfId="1" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="37" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="38" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13043,50 +13015,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:R9 A3:A9 B3 B5:B6 B8:B9">
-    <cfRule type="expression" dxfId="29" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="27" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="28" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9 A4:A7 B3 B5:B6 B8:B9">
-    <cfRule type="expression" dxfId="27" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="25" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="26" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5 A7">
-    <cfRule type="expression" dxfId="25" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="23" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="24" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3 B5:B6 B8:B10">
-    <cfRule type="expression" dxfId="23" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="5" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="6" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4 A7">
-    <cfRule type="expression" dxfId="21" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B10 B3 B5:B6">
-    <cfRule type="expression" dxfId="19" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="1" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="2" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15206,50 +15178,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:B6 D3:R6">
-    <cfRule type="expression" dxfId="17" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="25" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="26" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B6 A4:B6">
-    <cfRule type="expression" dxfId="15" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="23" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="24" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="expression" dxfId="13" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="21" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="22" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B5">
-    <cfRule type="expression" dxfId="11" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A7">
-    <cfRule type="expression" dxfId="9" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B5">
-    <cfRule type="expression" dxfId="7" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Maj BackLog 17/05/2013 + textarea wysihtml fluide dans la création artefact/média
</commit_message>
<xml_diff>
--- a/doc/Backlog [ACONIT].xlsx
+++ b/doc/Backlog [ACONIT].xlsx
@@ -2747,7 +2747,7 @@
                   <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>#N/A</c:v>
@@ -8634,9 +8634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:DP85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
@@ -8893,7 +8891,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="166">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="167"/>
       <c r="H5" s="168"/>
@@ -9253,7 +9251,7 @@
       </c>
       <c r="F17" s="38">
         <f t="array" ref="F17">IF(ISBLANK(F4:F15), NA(), SUM(F4:F15))</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G17" s="38" t="e">
         <f t="array" ref="G17">IF(ISBLANK(G4:G15), NA(), SUM(G4:G15))</f>
@@ -9422,7 +9420,7 @@
       </c>
       <c r="F18" s="38">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G18" s="38" t="e">
         <f t="shared" si="0"/>
@@ -9664,7 +9662,7 @@
       </c>
       <c r="F20" s="58">
         <f t="shared" si="2"/>
-        <v>0.18367346938775508</v>
+        <v>0.16326530612244894</v>
       </c>
       <c r="G20" s="58" t="e">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Ajout de la fonctionnalité modification d'un fichier uploadé
</commit_message>
<xml_diff>
--- a/doc/Backlog [ACONIT].xlsx
+++ b/doc/Backlog [ACONIT].xlsx
@@ -39,10 +39,10 @@
   </definedNames>
   <calcPr calcId="125725"/>
   <customWorkbookViews>
+    <customWorkbookView name="Yoann Regardin - Affichage personnalisé" guid="{29B12ED2-AD48-4E1C-B971-77E4D76C1B5F}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="609" activeSheetId="2"/>
+    <customWorkbookView name="uvba7442 - Affichage personnalisé" guid="{38566435-C99E-4958-9169-0C5C493EE97D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1213" windowHeight="665" activeSheetId="1"/>
+    <customWorkbookView name="Didier Lassissi - Affichage personnalisé" guid="{5E22A59B-ECE7-4B50-9619-81A99F53295A}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1064" windowHeight="552" activeSheetId="1"/>
     <customWorkbookView name="Bernard Notarianni - Affichage personnalisé" guid="{178C21D0-B00A-4B0E-B009-71AAC80909BC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="785" activeSheetId="1"/>
-    <customWorkbookView name="Didier Lassissi - Affichage personnalisé" guid="{5E22A59B-ECE7-4B50-9619-81A99F53295A}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1064" windowHeight="552" activeSheetId="1"/>
-    <customWorkbookView name="uvba7442 - Affichage personnalisé" guid="{38566435-C99E-4958-9169-0C5C493EE97D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1213" windowHeight="665" activeSheetId="1"/>
-    <customWorkbookView name="Yoann Regardin - Affichage personnalisé" guid="{29B12ED2-AD48-4E1C-B971-77E4D76C1B5F}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="609" activeSheetId="2"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
@@ -587,7 +587,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="32">
+  <fills count="30">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -741,17 +741,6 @@
       <patternFill patternType="lightUp">
         <fgColor theme="1"/>
         <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightUp">
-        <fgColor theme="1"/>
-        <bgColor theme="0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightUp">
-        <fgColor theme="1"/>
       </patternFill>
     </fill>
   </fills>
@@ -1152,7 +1141,7 @@
     <xf numFmtId="0" fontId="26" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="186">
+  <cellXfs count="182">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="5" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1637,33 +1626,18 @@
     <xf numFmtId="0" fontId="1" fillId="26" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="25" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="13" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="43" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="13" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1690,6 +1664,9 @@
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1738,7 +1715,49 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vérification" xfId="42" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="38">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2071,7 +2090,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225298"/>
+          <c:x val="0.37032576667225309"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2089,9 +2108,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532435"/>
+          <c:y val="0.15742128935532443"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192325"/>
+          <c:h val="0.70464767616192336"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2401,11 +2420,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="101373824"/>
-        <c:axId val="101728256"/>
+        <c:axId val="110950272"/>
+        <c:axId val="111296512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101373824"/>
+        <c:axId val="110950272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2437,7 +2456,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101728256"/>
+        <c:crossAx val="111296512"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2445,7 +2464,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101728256"/>
+        <c:axId val="111296512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2487,7 +2506,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101373824"/>
+        <c:crossAx val="110950272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2575,7 +2594,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000167" footer="0.49212598450000167"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000172" footer="0.49212598450000172"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2612,7 +2631,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225325"/>
+          <c:x val="0.37032576667225342"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2630,9 +2649,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532448"/>
+          <c:y val="0.15742128935532454"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192359"/>
+          <c:h val="0.70464767616192381"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2744,13 +2763,13 @@
                   <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>#N/A</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>#N/A</c:v>
@@ -2942,11 +2961,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="102085376"/>
-        <c:axId val="102087296"/>
+        <c:axId val="112702208"/>
+        <c:axId val="112704128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="102085376"/>
+        <c:axId val="112702208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2978,7 +2997,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="102087296"/>
+        <c:crossAx val="112704128"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2986,7 +3005,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102087296"/>
+        <c:axId val="112704128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3028,7 +3047,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="102085376"/>
+        <c:crossAx val="112702208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3116,7 +3135,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000178" footer="0.49212598450000178"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000183" footer="0.49212598450000183"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3153,7 +3172,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225353"/>
+          <c:x val="0.3703257666722537"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3171,9 +3190,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.1574212893553246"/>
+          <c:y val="0.15742128935532468"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192392"/>
+          <c:h val="0.70464767616192403"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3483,11 +3502,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="102157312"/>
-        <c:axId val="102159488"/>
+        <c:axId val="112770048"/>
+        <c:axId val="112772224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="102157312"/>
+        <c:axId val="112770048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3519,7 +3538,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="102159488"/>
+        <c:crossAx val="112772224"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3527,7 +3546,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102159488"/>
+        <c:axId val="112772224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3569,7 +3588,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="102157312"/>
+        <c:crossAx val="112770048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3657,7 +3676,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000189" footer="0.49212598450000189"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000195" footer="0.49212598450000195"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3694,7 +3713,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225386"/>
+          <c:x val="0.37032576667225398"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3712,9 +3731,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532476"/>
+          <c:y val="0.15742128935532482"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192414"/>
+          <c:h val="0.70464767616192425"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -4024,11 +4043,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="101946880"/>
-        <c:axId val="101948800"/>
+        <c:axId val="112559616"/>
+        <c:axId val="112561536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101946880"/>
+        <c:axId val="112559616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4060,7 +4079,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101948800"/>
+        <c:crossAx val="112561536"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -4068,7 +4087,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101948800"/>
+        <c:axId val="112561536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4110,7 +4129,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101946880"/>
+        <c:crossAx val="112559616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4198,7 +4217,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.492125984500002" footer="0.492125984500002"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000206" footer="0.49212598450000206"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -4670,10 +4689,10 @@
         <v>18</v>
       </c>
       <c r="C1" s="25"/>
-      <c r="D1" s="183" t="s">
+      <c r="D1" s="178" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="183"/>
+      <c r="E1" s="178"/>
       <c r="F1" s="24"/>
       <c r="G1" s="24"/>
       <c r="H1" s="15"/>
@@ -4685,10 +4704,10 @@
       <c r="A2" s="64"/>
       <c r="B2" s="16"/>
       <c r="C2" s="14"/>
-      <c r="D2" s="184" t="s">
+      <c r="D2" s="179" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="185"/>
+      <c r="E2" s="180"/>
       <c r="F2" s="26"/>
       <c r="G2" s="59"/>
       <c r="H2" s="3"/>
@@ -4704,8 +4723,8 @@
         <f>MAX(A13:A48)+1</f>
         <v>35</v>
       </c>
-      <c r="D3" s="178"/>
-      <c r="E3" s="179"/>
+      <c r="D3" s="173"/>
+      <c r="E3" s="174"/>
       <c r="F3" s="26"/>
       <c r="G3" s="59"/>
       <c r="H3" s="3"/>
@@ -4713,9 +4732,9 @@
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:13" hidden="1">
-      <c r="A4" s="180"/>
-      <c r="B4" s="181"/>
-      <c r="C4" s="182"/>
+      <c r="A4" s="175"/>
+      <c r="B4" s="176"/>
+      <c r="C4" s="177"/>
       <c r="D4" s="17"/>
       <c r="E4" s="5"/>
       <c r="F4" s="27"/>
@@ -6071,10 +6090,10 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A54:A55 B48:C48 D49:E51 H48:K48 A46:A49 B37:E37 D15 D38:E38 D41 B36:C37 H36:K37 E36:E37 A35:A43 D26 B28:C31 A13:A22 H28:K31 D20:E21 E25:E26 A25:A31 D28 D30 E28:E31 B12:E12 D13:E13 B13:C17 H12:K17 E13:E15 E17:E19">
-    <cfRule type="expression" dxfId="31" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="49" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="50" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8608,18 +8627,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11 A3:B11 F3:G7 H3:R11">
-    <cfRule type="expression" dxfId="29" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="53" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="54" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B10 A3:A7 A11:B11">
-    <cfRule type="expression" dxfId="27" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="31" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="32" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8634,7 +8653,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:DP85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
@@ -8863,8 +8884,10 @@
       <c r="F4" s="166">
         <v>5</v>
       </c>
-      <c r="G4" s="167"/>
-      <c r="H4" s="168"/>
+      <c r="G4" s="167">
+        <v>0</v>
+      </c>
+      <c r="H4" s="181"/>
       <c r="I4" s="167"/>
       <c r="J4" s="167"/>
       <c r="K4" s="167"/>
@@ -8874,7 +8897,7 @@
       <c r="O4" s="167"/>
       <c r="P4" s="167"/>
       <c r="Q4" s="167"/>
-      <c r="R4" s="171"/>
+      <c r="R4" s="169"/>
     </row>
     <row r="5" spans="1:120" s="162" customFormat="1" ht="24.95" customHeight="1">
       <c r="A5" s="159" t="s">
@@ -8893,8 +8916,10 @@
       <c r="F5" s="166">
         <v>1</v>
       </c>
-      <c r="G5" s="167"/>
-      <c r="H5" s="168"/>
+      <c r="G5" s="167">
+        <v>0</v>
+      </c>
+      <c r="H5" s="181"/>
       <c r="I5" s="167"/>
       <c r="J5" s="167"/>
       <c r="K5" s="167"/>
@@ -8904,7 +8929,7 @@
       <c r="O5" s="167"/>
       <c r="P5" s="167"/>
       <c r="Q5" s="167"/>
-      <c r="R5" s="171"/>
+      <c r="R5" s="169"/>
     </row>
     <row r="6" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
       <c r="A6" s="70" t="s">
@@ -8923,8 +8948,10 @@
       <c r="F6" s="156">
         <v>1</v>
       </c>
-      <c r="G6" s="156"/>
-      <c r="H6" s="169"/>
+      <c r="G6" s="156">
+        <v>1</v>
+      </c>
+      <c r="H6" s="181"/>
       <c r="I6" s="156"/>
       <c r="J6" s="156"/>
       <c r="K6" s="156"/>
@@ -8934,7 +8961,7 @@
       <c r="O6" s="156"/>
       <c r="P6" s="156"/>
       <c r="Q6" s="156"/>
-      <c r="R6" s="170"/>
+      <c r="R6" s="168"/>
     </row>
     <row r="7" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
       <c r="A7" s="70" t="s">
@@ -8948,13 +8975,15 @@
         <v>1</v>
       </c>
       <c r="E7" s="105">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="156">
-        <v>1</v>
-      </c>
-      <c r="G7" s="156"/>
-      <c r="H7" s="169"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="156">
+        <v>0</v>
+      </c>
+      <c r="H7" s="181"/>
       <c r="I7" s="156"/>
       <c r="J7" s="156"/>
       <c r="K7" s="156"/>
@@ -8964,7 +8993,7 @@
       <c r="O7" s="156"/>
       <c r="P7" s="156"/>
       <c r="Q7" s="156"/>
-      <c r="R7" s="170"/>
+      <c r="R7" s="168"/>
     </row>
     <row r="8" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
       <c r="A8" s="70" t="s">
@@ -8983,9 +9012,11 @@
       <c r="F8" s="166">
         <v>1</v>
       </c>
-      <c r="G8" s="156"/>
-      <c r="H8" s="169"/>
-      <c r="I8" s="156"/>
+      <c r="G8" s="167">
+        <v>0</v>
+      </c>
+      <c r="H8" s="181"/>
+      <c r="I8" s="167"/>
       <c r="J8" s="156"/>
       <c r="K8" s="156"/>
       <c r="L8" s="156"/>
@@ -8994,7 +9025,7 @@
       <c r="O8" s="156"/>
       <c r="P8" s="156"/>
       <c r="Q8" s="156"/>
-      <c r="R8" s="170"/>
+      <c r="R8" s="168"/>
     </row>
     <row r="9" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
       <c r="A9" s="82" t="s">
@@ -9015,9 +9046,11 @@
       <c r="F9" s="72">
         <v>5</v>
       </c>
-      <c r="G9" s="156"/>
-      <c r="H9" s="169"/>
-      <c r="I9" s="156"/>
+      <c r="G9" s="72">
+        <v>5</v>
+      </c>
+      <c r="H9" s="158"/>
+      <c r="I9" s="72"/>
       <c r="J9" s="156"/>
       <c r="K9" s="156"/>
       <c r="L9" s="156"/>
@@ -9026,7 +9059,7 @@
       <c r="O9" s="156"/>
       <c r="P9" s="156"/>
       <c r="Q9" s="156"/>
-      <c r="R9" s="170"/>
+      <c r="R9" s="168"/>
     </row>
     <row r="10" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
       <c r="A10" s="70" t="s">
@@ -9047,9 +9080,11 @@
       <c r="F10" s="72">
         <v>3</v>
       </c>
-      <c r="G10" s="156"/>
-      <c r="H10" s="169"/>
-      <c r="I10" s="156"/>
+      <c r="G10" s="72">
+        <v>3</v>
+      </c>
+      <c r="H10" s="158"/>
+      <c r="I10" s="72"/>
       <c r="J10" s="156"/>
       <c r="K10" s="156"/>
       <c r="L10" s="156"/>
@@ -9058,7 +9093,7 @@
       <c r="O10" s="156"/>
       <c r="P10" s="156"/>
       <c r="Q10" s="156"/>
-      <c r="R10" s="170"/>
+      <c r="R10" s="168"/>
     </row>
     <row r="11" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
       <c r="A11" s="70" t="s">
@@ -9079,9 +9114,11 @@
       <c r="F11" s="72">
         <v>6</v>
       </c>
-      <c r="G11" s="156"/>
-      <c r="H11" s="169"/>
-      <c r="I11" s="156"/>
+      <c r="G11" s="72">
+        <v>6</v>
+      </c>
+      <c r="H11" s="158"/>
+      <c r="I11" s="72"/>
       <c r="J11" s="156"/>
       <c r="K11" s="156"/>
       <c r="L11" s="156"/>
@@ -9090,7 +9127,7 @@
       <c r="O11" s="156"/>
       <c r="P11" s="156"/>
       <c r="Q11" s="156"/>
-      <c r="R11" s="170"/>
+      <c r="R11" s="168"/>
     </row>
     <row r="12" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
       <c r="A12" s="89" t="s">
@@ -9101,18 +9138,18 @@
       <c r="D12" s="91"/>
       <c r="E12" s="91"/>
       <c r="F12" s="91"/>
-      <c r="G12" s="171"/>
-      <c r="H12" s="172"/>
-      <c r="I12" s="171"/>
-      <c r="J12" s="171"/>
-      <c r="K12" s="171"/>
-      <c r="L12" s="171"/>
-      <c r="M12" s="171"/>
-      <c r="N12" s="171"/>
-      <c r="O12" s="171"/>
-      <c r="P12" s="171"/>
-      <c r="Q12" s="171"/>
-      <c r="R12" s="170"/>
+      <c r="G12" s="91"/>
+      <c r="H12" s="158"/>
+      <c r="I12" s="91"/>
+      <c r="J12" s="169"/>
+      <c r="K12" s="169"/>
+      <c r="L12" s="169"/>
+      <c r="M12" s="169"/>
+      <c r="N12" s="169"/>
+      <c r="O12" s="169"/>
+      <c r="P12" s="169"/>
+      <c r="Q12" s="169"/>
+      <c r="R12" s="168"/>
     </row>
     <row r="13" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
       <c r="A13" s="82" t="s">
@@ -9133,18 +9170,20 @@
       <c r="F13" s="72">
         <v>6</v>
       </c>
-      <c r="G13" s="156"/>
-      <c r="H13" s="173"/>
-      <c r="I13" s="174"/>
-      <c r="J13" s="174"/>
-      <c r="K13" s="174"/>
-      <c r="L13" s="174"/>
-      <c r="M13" s="174"/>
-      <c r="N13" s="174"/>
-      <c r="O13" s="174"/>
-      <c r="P13" s="174"/>
-      <c r="Q13" s="174"/>
-      <c r="R13" s="175"/>
+      <c r="G13" s="72">
+        <v>6</v>
+      </c>
+      <c r="H13" s="158"/>
+      <c r="I13" s="72"/>
+      <c r="J13" s="170"/>
+      <c r="K13" s="170"/>
+      <c r="L13" s="170"/>
+      <c r="M13" s="170"/>
+      <c r="N13" s="170"/>
+      <c r="O13" s="170"/>
+      <c r="P13" s="170"/>
+      <c r="Q13" s="170"/>
+      <c r="R13" s="171"/>
     </row>
     <row r="14" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
       <c r="A14" s="70" t="s">
@@ -9165,9 +9204,11 @@
       <c r="F14" s="72">
         <v>6</v>
       </c>
-      <c r="G14" s="105"/>
-      <c r="H14" s="176"/>
-      <c r="I14" s="155"/>
+      <c r="G14" s="72">
+        <v>6</v>
+      </c>
+      <c r="H14" s="158"/>
+      <c r="I14" s="72"/>
       <c r="J14" s="155"/>
       <c r="K14" s="155"/>
       <c r="L14" s="155"/>
@@ -9176,7 +9217,7 @@
       <c r="O14" s="155"/>
       <c r="P14" s="155"/>
       <c r="Q14" s="155"/>
-      <c r="R14" s="177"/>
+      <c r="R14" s="172"/>
     </row>
     <row r="15" spans="1:120" s="151" customFormat="1" ht="24.95" customHeight="1">
       <c r="A15" s="82" t="s">
@@ -9197,9 +9238,11 @@
       <c r="F15" s="72">
         <v>6</v>
       </c>
-      <c r="G15" s="105"/>
-      <c r="H15" s="176"/>
-      <c r="I15" s="155"/>
+      <c r="G15" s="72">
+        <v>6</v>
+      </c>
+      <c r="H15" s="158"/>
+      <c r="I15" s="72"/>
       <c r="J15" s="155"/>
       <c r="K15" s="155"/>
       <c r="L15" s="155"/>
@@ -9208,7 +9251,7 @@
       <c r="O15" s="155"/>
       <c r="P15" s="155"/>
       <c r="Q15" s="155"/>
-      <c r="R15" s="177"/>
+      <c r="R15" s="172"/>
     </row>
     <row r="16" spans="1:120">
       <c r="A16" s="38"/>
@@ -9247,15 +9290,15 @@
       </c>
       <c r="E17" s="38">
         <f t="array" ref="E17">IF(ISBLANK(E4:E15), NA(), SUM(E4:E15))</f>
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F17" s="38">
         <f t="array" ref="F17">IF(ISBLANK(F4:F15), NA(), SUM(F4:F15))</f>
-        <v>41</v>
-      </c>
-      <c r="G17" s="38" t="e">
+        <v>40</v>
+      </c>
+      <c r="G17" s="38">
         <f t="array" ref="G17">IF(ISBLANK(G4:G15), NA(), SUM(G4:G15))</f>
-        <v>#N/A</v>
+        <v>33</v>
       </c>
       <c r="H17" s="38" t="e">
         <f t="array" ref="H17">IF(ISBLANK(H4:H15), NA(), SUM(H4:H15))</f>
@@ -9416,15 +9459,15 @@
       </c>
       <c r="E18" s="38">
         <f t="shared" ref="E18:R18" si="0">D17-E17</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F18" s="38">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G18" s="38" t="e">
+      <c r="G18" s="38">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>7</v>
       </c>
       <c r="H18" s="38" t="e">
         <f t="shared" si="0"/>
@@ -9658,15 +9701,15 @@
       </c>
       <c r="E20" s="58">
         <f t="shared" si="2"/>
-        <v>0.12244897959183676</v>
+        <v>0.1428571428571429</v>
       </c>
       <c r="F20" s="58">
         <f t="shared" si="2"/>
-        <v>0.16326530612244894</v>
-      </c>
-      <c r="G20" s="58" t="e">
+        <v>0.18367346938775508</v>
+      </c>
+      <c r="G20" s="58">
         <f t="shared" si="2"/>
-        <v>#N/A</v>
+        <v>0.32653061224489799</v>
       </c>
       <c r="H20" s="58" t="e">
         <f t="shared" si="2"/>
@@ -11014,11 +11057,11 @@
       <c r="R85" s="38"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B13:B15 E13:G13 B3:B11 A3:A15 C6:D8 D14:R15 D3:R12">
-    <cfRule type="expression" dxfId="25" priority="37" stopIfTrue="1">
+  <conditionalFormatting sqref="B13:B15 E13:G13 B3:B11 A3:A15 C6:D8 D14:R15 D3:R12 G4:I15">
+    <cfRule type="expression" dxfId="31" priority="37" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="38" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13013,50 +13056,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:R9 A3:A9 B3 B5:B6 B8:B9">
-    <cfRule type="expression" dxfId="23" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="27" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="28" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9 A4:A7 B3 B5:B6 B8:B9">
-    <cfRule type="expression" dxfId="21" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="25" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="26" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5 A7">
-    <cfRule type="expression" dxfId="19" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="23" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="24" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3 B5:B6 B8:B10">
-    <cfRule type="expression" dxfId="17" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="5" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="6" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4 A7">
-    <cfRule type="expression" dxfId="15" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B10 B3 B5:B6">
-    <cfRule type="expression" dxfId="13" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="1" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="2" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15176,50 +15219,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:B6 D3:R6">
-    <cfRule type="expression" dxfId="11" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="25" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="26" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B6 A4:B6">
-    <cfRule type="expression" dxfId="9" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="23" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="24" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="expression" dxfId="7" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="21" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="22" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B5">
-    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="5" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="6" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A7">
-    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B5">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="1" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
ajout de la page des sémantiques des transitions
</commit_message>
<xml_diff>
--- a/doc/Backlog [ACONIT].xlsx
+++ b/doc/Backlog [ACONIT].xlsx
@@ -1715,21 +1715,7 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vérification" xfId="42" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="34">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="51"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="32">
     <dxf>
       <fill>
         <patternFill>
@@ -2062,7 +2048,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225325"/>
+          <c:x val="0.37032576667225353"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2080,9 +2066,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532448"/>
+          <c:y val="0.1574212893553246"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192359"/>
+          <c:h val="0.70464767616192392"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2392,11 +2378,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="102619008"/>
-        <c:axId val="105074688"/>
+        <c:axId val="100456320"/>
+        <c:axId val="100548608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="102619008"/>
+        <c:axId val="100456320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2428,7 +2414,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105074688"/>
+        <c:crossAx val="100548608"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2436,7 +2422,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105074688"/>
+        <c:axId val="100548608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2478,548 +2464,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="102619008"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.82639198178585549"/>
-          <c:y val="3.2983508245877091E-2"/>
-          <c:w val="0.11675295106908352"/>
-          <c:h val="9.145427286356822E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="3175">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1445" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:ea typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
-    </a:solidFill>
-    <a:ln w="3175">
-      <a:solidFill>
-        <a:srgbClr val="000000"/>
-      </a:solidFill>
-      <a:prstDash val="solid"/>
-    </a:ln>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr sz="1575" b="0" i="0" u="none" strike="noStrike" baseline="0">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:latin typeface="Arial"/>
-          <a:ea typeface="Arial"/>
-          <a:cs typeface="Arial"/>
-        </a:defRPr>
-      </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000178" footer="0.49212598450000178"/>
-    <c:pageSetup paperSize="9" orientation="landscape"/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="fr-FR"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1900" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-                <a:ea typeface="Arial"/>
-                <a:cs typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="fr-FR"/>
-              <a:t>Suivi charge Iteration 2</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.37032576667225353"/>
-          <c:y val="2.6986506746626688E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="25400">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.1574212893553246"/>
-          <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192392"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Iteration 2'!$B$17</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Iteration </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="12700">
-              <a:solidFill>
-                <a:srgbClr val="000080"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="000080"/>
-              </a:solidFill>
-              <a:ln>
-                <a:solidFill>
-                  <a:srgbClr val="000080"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Iteration 2'!$C$2:$R$2</c:f>
-              <c:numCache>
-                <c:formatCode>[$-40C]d\-mmm;@</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>41407</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41408</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41409</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>41410</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>41411</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>41414</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>41415</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>41416</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>41417</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>41418</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>41421</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41422</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41423</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41424</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41425</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>41428</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Iteration 2'!$C$17:$R$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Iteration 2'!$B$19</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>REF</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="12700">
-              <a:solidFill>
-                <a:srgbClr val="FF00FF"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FF00FF"/>
-              </a:solidFill>
-              <a:ln>
-                <a:solidFill>
-                  <a:srgbClr val="FF00FF"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Iteration 2'!$C$2:$R$2</c:f>
-              <c:numCache>
-                <c:formatCode>[$-40C]d\-mmm;@</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>41407</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41408</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41409</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>41410</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>41411</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>41414</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>41415</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>41416</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>41417</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>41418</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>41421</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41422</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41423</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41424</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41425</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>41428</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Iteration 2'!$C$19:$R$19</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>45.733333333333334</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42.466666666666669</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>39.200000000000003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>35.933333333333337</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.666666666666671</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>29.400000000000006</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>26.13333333333334</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>22.866666666666674</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>19.600000000000009</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>16.333333333333343</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>13.066666666666677</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>9.8000000000000114</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6.5333333333333448</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.2666666666666782</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.1546319456101628E-14</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="105423616"/>
-        <c:axId val="105425536"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="105423616"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="[$-40C]d\-mmm;@" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="3175">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:prstDash val="solid"/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="0" vert="horz"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1575" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-                <a:ea typeface="Arial"/>
-                <a:cs typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="105425536"/>
-        <c:crosses val="autoZero"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:tickLblSkip val="1"/>
-        <c:tickMarkSkip val="1"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="105425536"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="3175">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="3175">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:prstDash val="solid"/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="0" vert="horz"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1575" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-                <a:ea typeface="Arial"/>
-                <a:cs typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="105423616"/>
+        <c:crossAx val="100456320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3113,7 +2558,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="fr-FR"/>
   <c:chart>
@@ -3135,7 +2580,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-FR"/>
-              <a:t>Suivi charge Iteration 3</a:t>
+              <a:t>Suivi charge Iteration 2</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3174,7 +2619,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Iteration 3'!$B$12</c:f>
+              <c:f>'Iteration 2'!$B$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3208,87 +2653,87 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Iteration 3'!$C$2:$R$2</c:f>
+              <c:f>'Iteration 2'!$C$2:$R$2</c:f>
               <c:numCache>
                 <c:formatCode>[$-40C]d\-mmm;@</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
+                  <c:v>41407</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41408</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41409</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41410</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41411</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41414</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41415</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41416</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41417</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41418</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>41421</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="11">
                   <c:v>41422</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="12">
                   <c:v>41423</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="13">
                   <c:v>41424</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="14">
                   <c:v>41425</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="15">
                   <c:v>41428</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>41429</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>41430</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>41431</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>41432</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>41435</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41436</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41437</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41438</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41439</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>41442</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Iteration 3'!$C$12:$R$12</c:f>
+              <c:f>'Iteration 2'!$C$17:$R$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>52</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>#N/A</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>#N/A</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>#N/A</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>#N/A</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>#N/A</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>#N/A</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>#N/A</c:v>
@@ -3326,7 +2771,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Iteration 3'!$B$14</c:f>
+              <c:f>'Iteration 2'!$B$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3360,125 +2805,125 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Iteration 3'!$C$2:$R$2</c:f>
+              <c:f>'Iteration 2'!$C$2:$R$2</c:f>
               <c:numCache>
                 <c:formatCode>[$-40C]d\-mmm;@</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
+                  <c:v>41407</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41408</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41409</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41410</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41411</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41414</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41415</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41416</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41417</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41418</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>41421</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="11">
                   <c:v>41422</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="12">
                   <c:v>41423</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="13">
                   <c:v>41424</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="14">
                   <c:v>41425</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="15">
                   <c:v>41428</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>41429</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>41430</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>41431</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>41432</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>41435</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41436</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41437</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41438</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41439</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>41442</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Iteration 3'!$C$14:$R$14</c:f>
+              <c:f>'Iteration 2'!$C$19:$R$19</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>52</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48.533333333333331</c:v>
+                  <c:v>45.733333333333334</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45.066666666666663</c:v>
+                  <c:v>42.466666666666669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41.599999999999994</c:v>
+                  <c:v>39.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38.133333333333326</c:v>
+                  <c:v>35.933333333333337</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34.666666666666657</c:v>
+                  <c:v>32.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31.199999999999989</c:v>
+                  <c:v>29.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27.73333333333332</c:v>
+                  <c:v>26.13333333333334</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>24.266666666666652</c:v>
+                  <c:v>22.866666666666674</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20.799999999999983</c:v>
+                  <c:v>19.600000000000009</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>17.333333333333314</c:v>
+                  <c:v>16.333333333333343</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13.866666666666648</c:v>
+                  <c:v>13.066666666666677</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10.399999999999981</c:v>
+                  <c:v>9.8000000000000114</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.933333333333314</c:v>
+                  <c:v>6.5333333333333448</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.4666666666666472</c:v>
+                  <c:v>3.2666666666666782</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-1.9539925233402755E-14</c:v>
+                  <c:v>1.1546319456101628E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="105303040"/>
-        <c:axId val="105305216"/>
+        <c:axId val="104309504"/>
+        <c:axId val="104311424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105303040"/>
+        <c:axId val="104309504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3510,7 +2955,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105305216"/>
+        <c:crossAx val="104311424"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3518,7 +2963,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105305216"/>
+        <c:axId val="104311424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3560,7 +3005,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105303040"/>
+        <c:crossAx val="104309504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3654,7 +3099,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="fr-FR"/>
   <c:chart>
@@ -3676,7 +3121,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-FR"/>
-              <a:t>Suivi charge Iteration 4</a:t>
+              <a:t>Suivi charge Iteration 3</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3715,7 +3160,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Iteration 4'!$B$8</c:f>
+              <c:f>'Iteration 3'!$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3749,69 +3194,69 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Iteration 4'!$C$2:$R$2</c:f>
+              <c:f>'Iteration 3'!$C$2:$R$2</c:f>
               <c:numCache>
                 <c:formatCode>[$-40C]d\-mmm;@</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
+                  <c:v>41421</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41422</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41423</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41424</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41425</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41428</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41429</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41430</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41431</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41432</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41435</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41436</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41437</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41438</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41439</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>41442</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41443</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41444</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>41445</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>41446</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>41449</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>41450</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>41451</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>41452</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>41453</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>41456</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41457</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41458</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41459</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41460</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>41463</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Iteration 4'!$C$8:$R$8</c:f>
+              <c:f>'Iteration 3'!$C$12:$R$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>28</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
@@ -3867,7 +3312,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Iteration 4'!$B$10</c:f>
+              <c:f>'Iteration 3'!$B$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3901,125 +3346,125 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Iteration 4'!$C$2:$R$2</c:f>
+              <c:f>'Iteration 3'!$C$2:$R$2</c:f>
               <c:numCache>
                 <c:formatCode>[$-40C]d\-mmm;@</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
+                  <c:v>41421</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41422</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41423</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41424</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41425</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41428</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41429</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41430</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41431</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41432</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41435</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41436</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41437</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41438</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41439</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>41442</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41443</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41444</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>41445</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>41446</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>41449</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>41450</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>41451</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>41452</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>41453</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>41456</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41457</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41458</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41459</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41460</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>41463</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Iteration 4'!$C$10:$R$10</c:f>
+              <c:f>'Iteration 3'!$C$14:$R$14</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>28</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.133333333333333</c:v>
+                  <c:v>48.533333333333331</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.266666666666666</c:v>
+                  <c:v>45.066666666666663</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.4</c:v>
+                  <c:v>41.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.533333333333331</c:v>
+                  <c:v>38.133333333333326</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18.666666666666664</c:v>
+                  <c:v>34.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16.799999999999997</c:v>
+                  <c:v>31.199999999999989</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.93333333333333</c:v>
+                  <c:v>27.73333333333332</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13.066666666666663</c:v>
+                  <c:v>24.266666666666652</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11.199999999999996</c:v>
+                  <c:v>20.799999999999983</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.3333333333333286</c:v>
+                  <c:v>17.333333333333314</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.4666666666666615</c:v>
+                  <c:v>13.866666666666648</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.5999999999999943</c:v>
+                  <c:v>10.399999999999981</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.7333333333333276</c:v>
+                  <c:v>6.933333333333314</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.8666666666666609</c:v>
+                  <c:v>3.4666666666666472</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-5.773159728050814E-15</c:v>
+                  <c:v>-1.9539925233402755E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="105350656"/>
-        <c:axId val="105352576"/>
+        <c:axId val="104385536"/>
+        <c:axId val="104387712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105350656"/>
+        <c:axId val="104385536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4051,7 +3496,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105352576"/>
+        <c:crossAx val="104387712"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -4059,7 +3504,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105352576"/>
+        <c:axId val="104387712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4101,7 +3546,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105350656"/>
+        <c:crossAx val="104385536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4190,6 +3635,547 @@
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
     <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000211" footer="0.49212598450000211"/>
+    <c:pageSetup paperSize="9" orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="fr-FR"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1900" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Suivi charge Iteration 4</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.37032576667225442"/>
+          <c:y val="2.6986506746626688E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.5640078243859845E-2"/>
+          <c:y val="0.15742128935532501"/>
+          <c:w val="0.92946294640153049"/>
+          <c:h val="0.70464767616192481"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Iteration 4'!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Iteration </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:srgbClr val="000080"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="000080"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="000080"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Iteration 4'!$C$2:$R$2</c:f>
+              <c:numCache>
+                <c:formatCode>[$-40C]d\-mmm;@</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>41442</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41443</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41444</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41445</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41446</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41449</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41450</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41451</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41452</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41453</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41456</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41457</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41458</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41459</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41460</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41463</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Iteration 4'!$C$8:$R$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Iteration 4'!$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>REF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:srgbClr val="FF00FF"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF00FF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="FF00FF"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Iteration 4'!$C$2:$R$2</c:f>
+              <c:numCache>
+                <c:formatCode>[$-40C]d\-mmm;@</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>41442</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41443</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41444</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41445</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41446</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41449</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41450</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41451</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41452</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41453</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41456</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41457</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41458</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41459</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41460</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41463</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Iteration 4'!$C$10:$R$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.133333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.266666666666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.533333333333331</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.93333333333333</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.066666666666663</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.3333333333333286</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.4666666666666615</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.5999999999999943</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.7333333333333276</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.8666666666666609</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-5.773159728050814E-15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="104171008"/>
+        <c:axId val="104172928"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="104171008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="[$-40C]d\-mmm;@" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="3175">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1575" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="104172928"/>
+        <c:crosses val="autoZero"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="104172928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="3175">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="3175">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1575" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="104171008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.82639198178585549"/>
+          <c:y val="3.2983508245877091E-2"/>
+          <c:w val="0.11675295106908352"/>
+          <c:h val="9.145427286356822E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="3175">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1445" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:ea typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln w="3175">
+      <a:solidFill>
+        <a:srgbClr val="000000"/>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1575" b="0" i="0" u="none" strike="noStrike" baseline="0">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Arial"/>
+          <a:ea typeface="Arial"/>
+          <a:cs typeface="Arial"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter alignWithMargins="0"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000222" footer="0.49212598450000222"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -4637,7 +4623,7 @@
       <pane xSplit="4" ySplit="5" topLeftCell="E21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="G24" sqref="G24"/>
+      <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -6062,10 +6048,10 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A54:A55 B48:C48 D49:E51 H48:K48 A46:A49 B37:E37 D15 D38:E38 D41 B36:C37 H36:K37 E36:E37 A35:A43 D26 B28:C31 A13:A22 H28:K31 D20:E21 E25:E26 A25:A31 D28 D30 E28:E31 B12:E12 D13:E13 B13:C17 H12:K17 E13:E15 E17:E19">
-    <cfRule type="expression" dxfId="33" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="49" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="50" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6080,8 +6066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:DP82"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R12" sqref="R1:R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -8599,18 +8585,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11 A3:B11 F3:G7 H3:R11">
-    <cfRule type="expression" dxfId="31" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="53" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="54" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B10 A3:A7 A11:B11">
-    <cfRule type="expression" dxfId="29" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="31" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="32" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8625,9 +8611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:DP85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
@@ -11074,10 +11058,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B13:B15 E13:G13 B3:B11 A3:A15 C6:D8 D14:R15 D3:R12 G4:I15">
-    <cfRule type="expression" dxfId="27" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="37" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="38" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13072,50 +13056,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:R9 A3:A9 B3 B5:B6 B8:B9">
-    <cfRule type="expression" dxfId="25" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="27" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="28" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9 A4:A7 B3 B5:B6 B8:B9">
-    <cfRule type="expression" dxfId="23" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="25" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="26" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5 A7">
-    <cfRule type="expression" dxfId="21" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="23" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="24" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3 B5:B6 B8:B10">
-    <cfRule type="expression" dxfId="19" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="5" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="6" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4 A7">
-    <cfRule type="expression" dxfId="17" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B10 B3 B5:B6">
-    <cfRule type="expression" dxfId="15" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="1" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="2" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15235,50 +15219,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:B6 D3:R6">
-    <cfRule type="expression" dxfId="13" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="25" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="26" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B6 A4:B6">
-    <cfRule type="expression" dxfId="11" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="23" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="24" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="expression" dxfId="9" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="21" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="22" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B5">
-    <cfRule type="expression" dxfId="7" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A7">
-    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B5">
-    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Ajout de la vérif quand on supprime une sémantique transition : on ne peut pas si elle est utilisée dans une transition
</commit_message>
<xml_diff>
--- a/doc/Backlog [ACONIT].xlsx
+++ b/doc/Backlog [ACONIT].xlsx
@@ -1715,21 +1715,7 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vérification" xfId="42" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="34">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="51"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="32">
     <dxf>
       <fill>
         <patternFill>
@@ -6062,10 +6048,10 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A54:A55 B48:C48 D49:E51 H48:K48 A46:A49 B37:E37 D15 D38:E38 D41 B36:C37 H36:K37 E36:E37 A35:A43 D26 B28:C31 A13:A22 H28:K31 D20:E21 E25:E26 A25:A31 D28 D30 E28:E31 B12:E12 D13:E13 B13:C17 H12:K17 E13:E15 E17:E19">
-    <cfRule type="expression" dxfId="33" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="49" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="50" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8599,18 +8585,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11 A3:B11 F3:G7 H3:R11">
-    <cfRule type="expression" dxfId="31" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="53" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="54" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B10 A3:A7 A11:B11">
-    <cfRule type="expression" dxfId="29" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="31" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="32" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8626,7 +8612,7 @@
   <dimension ref="A1:DP85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -9664,63 +9650,63 @@
         <v>49</v>
       </c>
       <c r="D19" s="46">
-        <f t="shared" ref="D19:R19" si="1">C19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f>C19-$C$17/COUNTA($C$2:$Q$2)</f>
         <v>45.733333333333334</v>
       </c>
       <c r="E19" s="46">
-        <f t="shared" si="1"/>
+        <f>D19-$C$17/COUNTA($C$2:$Q$2)</f>
         <v>42.466666666666669</v>
       </c>
       <c r="F19" s="46">
-        <f t="shared" si="1"/>
+        <f>E19-$C$17/COUNTA($C$2:$Q$2)</f>
         <v>39.200000000000003</v>
       </c>
       <c r="G19" s="46">
-        <f t="shared" si="1"/>
+        <f>F19-$C$17/COUNTA($C$2:$Q$2)</f>
         <v>35.933333333333337</v>
       </c>
       <c r="H19" s="46">
-        <f t="shared" si="1"/>
+        <f>G19-$C$17/COUNTA($C$2:$Q$2)</f>
         <v>32.666666666666671</v>
       </c>
       <c r="I19" s="46">
-        <f t="shared" si="1"/>
+        <f>H19-$C$17/COUNTA($C$2:$Q$2)</f>
         <v>29.400000000000006</v>
       </c>
       <c r="J19" s="46">
-        <f t="shared" si="1"/>
+        <f>I19-$C$17/COUNTA($C$2:$Q$2)</f>
         <v>26.13333333333334</v>
       </c>
       <c r="K19" s="46">
-        <f t="shared" si="1"/>
+        <f>J19-$C$17/COUNTA($C$2:$Q$2)</f>
         <v>22.866666666666674</v>
       </c>
       <c r="L19" s="46">
-        <f t="shared" si="1"/>
+        <f>K19-$C$17/COUNTA($C$2:$Q$2)</f>
         <v>19.600000000000009</v>
       </c>
       <c r="M19" s="46">
-        <f t="shared" si="1"/>
+        <f>L19-$C$17/COUNTA($C$2:$Q$2)</f>
         <v>16.333333333333343</v>
       </c>
       <c r="N19" s="46">
-        <f t="shared" si="1"/>
+        <f>M19-$C$17/COUNTA($C$2:$Q$2)</f>
         <v>13.066666666666677</v>
       </c>
       <c r="O19" s="46">
-        <f t="shared" si="1"/>
+        <f>N19-$C$17/COUNTA($C$2:$Q$2)</f>
         <v>9.8000000000000114</v>
       </c>
       <c r="P19" s="46">
-        <f t="shared" si="1"/>
+        <f>O19-$C$17/COUNTA($C$2:$Q$2)</f>
         <v>6.5333333333333448</v>
       </c>
       <c r="Q19" s="46">
-        <f t="shared" si="1"/>
+        <f>P19-$C$17/COUNTA($C$2:$Q$2)</f>
         <v>3.2666666666666782</v>
       </c>
       <c r="R19" s="46">
-        <f t="shared" si="1"/>
+        <f>Q19-$C$17/COUNTA($C$2:$Q$2)</f>
         <v>1.1546319456101628E-14</v>
       </c>
     </row>
@@ -9734,63 +9720,63 @@
         <v>0</v>
       </c>
       <c r="D20" s="58">
-        <f t="shared" ref="D20:R20" si="2">1-D17/$C$17</f>
+        <f t="shared" ref="D20:R20" si="1">1-D17/$C$17</f>
         <v>0</v>
       </c>
       <c r="E20" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.1428571428571429</v>
       </c>
       <c r="F20" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.18367346938775508</v>
       </c>
       <c r="G20" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.32653061224489799</v>
       </c>
       <c r="H20" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.32653061224489799</v>
       </c>
       <c r="I20" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.40816326530612246</v>
       </c>
       <c r="J20" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.51020408163265307</v>
       </c>
       <c r="K20" s="58" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="L20" s="58" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="M20" s="58" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="N20" s="58" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="O20" s="58" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="P20" s="58" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q20" s="58" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="R20" s="58" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -11096,10 +11082,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B13:B15 E13:G13 B3:B11 A3:A15 C6:D8 D14:R15 D3:R12 G4:J15">
-    <cfRule type="expression" dxfId="27" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="37" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="38" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Commentaires + Maj BackLog 24/05/2013
</commit_message>
<xml_diff>
--- a/doc/Backlog [ACONIT].xlsx
+++ b/doc/Backlog [ACONIT].xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10155" yWindow="0" windowWidth="11490" windowHeight="10065" tabRatio="900" activeTab="2"/>
+    <workbookView xWindow="10155" yWindow="0" windowWidth="11475" windowHeight="10065" tabRatio="900" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="20" r:id="rId1"/>
@@ -1715,7 +1715,35 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vérification" xfId="42" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="36">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2048,7 +2076,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225353"/>
+          <c:x val="0.37032576667225386"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2066,9 +2094,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.1574212893553246"/>
+          <c:y val="0.15742128935532476"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192392"/>
+          <c:h val="0.70464767616192414"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2378,11 +2406,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="100456320"/>
-        <c:axId val="100548608"/>
+        <c:axId val="99538816"/>
+        <c:axId val="100941824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100456320"/>
+        <c:axId val="99538816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2414,7 +2442,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100548608"/>
+        <c:crossAx val="100941824"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2422,7 +2450,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100548608"/>
+        <c:axId val="100941824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2464,548 +2492,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100456320"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.82639198178585549"/>
-          <c:y val="3.2983508245877091E-2"/>
-          <c:w val="0.11675295106908352"/>
-          <c:h val="9.145427286356822E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="3175">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1445" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:ea typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
-    </a:solidFill>
-    <a:ln w="3175">
-      <a:solidFill>
-        <a:srgbClr val="000000"/>
-      </a:solidFill>
-      <a:prstDash val="solid"/>
-    </a:ln>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr sz="1575" b="0" i="0" u="none" strike="noStrike" baseline="0">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:latin typeface="Arial"/>
-          <a:ea typeface="Arial"/>
-          <a:cs typeface="Arial"/>
-        </a:defRPr>
-      </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000189" footer="0.49212598450000189"/>
-    <c:pageSetup paperSize="9" orientation="landscape"/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="fr-FR"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1900" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-                <a:ea typeface="Arial"/>
-                <a:cs typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="fr-FR"/>
-              <a:t>Suivi charge Iteration 2</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.37032576667225386"/>
-          <c:y val="2.6986506746626688E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="25400">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532476"/>
-          <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192414"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Iteration 2'!$B$17</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Iteration </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="12700">
-              <a:solidFill>
-                <a:srgbClr val="000080"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="000080"/>
-              </a:solidFill>
-              <a:ln>
-                <a:solidFill>
-                  <a:srgbClr val="000080"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Iteration 2'!$C$2:$R$2</c:f>
-              <c:numCache>
-                <c:formatCode>[$-40C]d\-mmm;@</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>41407</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41408</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41409</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>41410</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>41411</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>41414</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>41415</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>41416</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>41417</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>41418</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>41421</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41422</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41423</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41424</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41425</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>41428</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Iteration 2'!$C$17:$R$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Iteration 2'!$B$19</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>REF</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="12700">
-              <a:solidFill>
-                <a:srgbClr val="FF00FF"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FF00FF"/>
-              </a:solidFill>
-              <a:ln>
-                <a:solidFill>
-                  <a:srgbClr val="FF00FF"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Iteration 2'!$C$2:$R$2</c:f>
-              <c:numCache>
-                <c:formatCode>[$-40C]d\-mmm;@</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>41407</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41408</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41409</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>41410</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>41411</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>41414</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>41415</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>41416</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>41417</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>41418</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>41421</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41422</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41423</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41424</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41425</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>41428</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Iteration 2'!$C$19:$R$19</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>45.733333333333334</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42.466666666666669</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>39.200000000000003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>35.933333333333337</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.666666666666671</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>29.400000000000006</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>26.13333333333334</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>22.866666666666674</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>19.600000000000009</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>16.333333333333343</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>13.066666666666677</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>9.8000000000000114</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6.5333333333333448</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.2666666666666782</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.1546319456101628E-14</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="104309504"/>
-        <c:axId val="104311424"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="104309504"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="[$-40C]d\-mmm;@" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="3175">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:prstDash val="solid"/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="0" vert="horz"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1575" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-                <a:ea typeface="Arial"/>
-                <a:cs typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="104311424"/>
-        <c:crosses val="autoZero"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:tickLblSkip val="1"/>
-        <c:tickMarkSkip val="1"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="104311424"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="3175">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="3175">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:prstDash val="solid"/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="0" vert="horz"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1575" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-                <a:ea typeface="Arial"/>
-                <a:cs typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="104309504"/>
+        <c:crossAx val="99538816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3099,7 +2586,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="fr-FR"/>
   <c:chart>
@@ -3121,7 +2608,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-FR"/>
-              <a:t>Suivi charge Iteration 3</a:t>
+              <a:t>Suivi charge Iteration 2</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3160,7 +2647,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Iteration 3'!$B$12</c:f>
+              <c:f>'Iteration 2'!$B$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3194,96 +2681,96 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Iteration 3'!$C$2:$R$2</c:f>
+              <c:f>'Iteration 2'!$C$2:$R$2</c:f>
               <c:numCache>
                 <c:formatCode>[$-40C]d\-mmm;@</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
+                  <c:v>41407</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41408</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41409</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41410</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41411</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41414</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41415</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41416</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41417</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41418</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>41421</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="11">
                   <c:v>41422</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="12">
                   <c:v>41423</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="13">
                   <c:v>41424</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="14">
                   <c:v>41425</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="15">
                   <c:v>41428</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>41429</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>41430</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>41431</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>41432</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>41435</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41436</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41437</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41438</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41439</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>41442</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Iteration 3'!$C$12:$R$12</c:f>
+              <c:f>'Iteration 2'!$C$17:$R$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>52</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>#N/A</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>#N/A</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>#N/A</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>#N/A</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>#N/A</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>#N/A</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>#N/A</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>#N/A</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>#N/A</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>#N/A</c:v>
@@ -3312,7 +2799,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Iteration 3'!$B$14</c:f>
+              <c:f>'Iteration 2'!$B$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3346,125 +2833,125 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Iteration 3'!$C$2:$R$2</c:f>
+              <c:f>'Iteration 2'!$C$2:$R$2</c:f>
               <c:numCache>
                 <c:formatCode>[$-40C]d\-mmm;@</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
+                  <c:v>41407</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41408</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41409</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41410</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41411</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41414</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41415</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41416</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41417</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41418</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>41421</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="11">
                   <c:v>41422</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="12">
                   <c:v>41423</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="13">
                   <c:v>41424</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="14">
                   <c:v>41425</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="15">
                   <c:v>41428</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>41429</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>41430</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>41431</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>41432</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>41435</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41436</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41437</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41438</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41439</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>41442</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Iteration 3'!$C$14:$R$14</c:f>
+              <c:f>'Iteration 2'!$C$19:$R$19</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>52</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48.533333333333331</c:v>
+                  <c:v>45.733333333333334</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45.066666666666663</c:v>
+                  <c:v>42.466666666666669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41.599999999999994</c:v>
+                  <c:v>39.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38.133333333333326</c:v>
+                  <c:v>35.933333333333337</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34.666666666666657</c:v>
+                  <c:v>32.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31.199999999999989</c:v>
+                  <c:v>29.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27.73333333333332</c:v>
+                  <c:v>26.13333333333334</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>24.266666666666652</c:v>
+                  <c:v>22.866666666666674</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20.799999999999983</c:v>
+                  <c:v>19.600000000000009</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>17.333333333333314</c:v>
+                  <c:v>16.333333333333343</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13.866666666666648</c:v>
+                  <c:v>13.066666666666677</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10.399999999999981</c:v>
+                  <c:v>9.8000000000000114</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.933333333333314</c:v>
+                  <c:v>6.5333333333333448</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.4666666666666472</c:v>
+                  <c:v>3.2666666666666782</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-1.9539925233402755E-14</c:v>
+                  <c:v>1.1546319456101628E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="104385536"/>
-        <c:axId val="104387712"/>
+        <c:axId val="101294848"/>
+        <c:axId val="101296768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="104385536"/>
+        <c:axId val="101294848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3496,7 +2983,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="104387712"/>
+        <c:crossAx val="101296768"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3504,7 +2991,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104387712"/>
+        <c:axId val="101296768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3546,7 +3033,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="104385536"/>
+        <c:crossAx val="101294848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3640,7 +3127,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="fr-FR"/>
   <c:chart>
@@ -3662,7 +3149,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-FR"/>
-              <a:t>Suivi charge Iteration 4</a:t>
+              <a:t>Suivi charge Iteration 3</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3701,7 +3188,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Iteration 4'!$B$8</c:f>
+              <c:f>'Iteration 3'!$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3735,69 +3222,69 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Iteration 4'!$C$2:$R$2</c:f>
+              <c:f>'Iteration 3'!$C$2:$R$2</c:f>
               <c:numCache>
                 <c:formatCode>[$-40C]d\-mmm;@</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
+                  <c:v>41421</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41422</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41423</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41424</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41425</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41428</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41429</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41430</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41431</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41432</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41435</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41436</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41437</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41438</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41439</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>41442</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41443</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41444</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>41445</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>41446</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>41449</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>41450</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>41451</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>41452</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>41453</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>41456</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41457</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41458</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41459</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41460</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>41463</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Iteration 4'!$C$8:$R$8</c:f>
+              <c:f>'Iteration 3'!$C$12:$R$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>28</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
@@ -3853,7 +3340,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Iteration 4'!$B$10</c:f>
+              <c:f>'Iteration 3'!$B$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3887,125 +3374,125 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Iteration 4'!$C$2:$R$2</c:f>
+              <c:f>'Iteration 3'!$C$2:$R$2</c:f>
               <c:numCache>
                 <c:formatCode>[$-40C]d\-mmm;@</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
+                  <c:v>41421</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41422</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41423</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41424</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41425</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41428</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41429</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41430</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41431</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41432</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41435</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41436</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41437</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41438</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41439</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>41442</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41443</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41444</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>41445</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>41446</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>41449</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>41450</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>41451</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>41452</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>41453</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>41456</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41457</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41458</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41459</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41460</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>41463</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Iteration 4'!$C$10:$R$10</c:f>
+              <c:f>'Iteration 3'!$C$14:$R$14</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>28</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.133333333333333</c:v>
+                  <c:v>48.533333333333331</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.266666666666666</c:v>
+                  <c:v>45.066666666666663</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.4</c:v>
+                  <c:v>41.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.533333333333331</c:v>
+                  <c:v>38.133333333333326</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18.666666666666664</c:v>
+                  <c:v>34.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16.799999999999997</c:v>
+                  <c:v>31.199999999999989</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.93333333333333</c:v>
+                  <c:v>27.73333333333332</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13.066666666666663</c:v>
+                  <c:v>24.266666666666652</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11.199999999999996</c:v>
+                  <c:v>20.799999999999983</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.3333333333333286</c:v>
+                  <c:v>17.333333333333314</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.4666666666666615</c:v>
+                  <c:v>13.866666666666648</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.5999999999999943</c:v>
+                  <c:v>10.399999999999981</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.7333333333333276</c:v>
+                  <c:v>6.933333333333314</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.8666666666666609</c:v>
+                  <c:v>3.4666666666666472</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-5.773159728050814E-15</c:v>
+                  <c:v>-1.9539925233402755E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="104171008"/>
-        <c:axId val="104172928"/>
+        <c:axId val="101370880"/>
+        <c:axId val="101373056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="104171008"/>
+        <c:axId val="101370880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4037,7 +3524,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="104172928"/>
+        <c:crossAx val="101373056"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -4045,7 +3532,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104172928"/>
+        <c:axId val="101373056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4087,7 +3574,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="104171008"/>
+        <c:crossAx val="101370880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4176,6 +3663,547 @@
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
     <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000222" footer="0.49212598450000222"/>
+    <c:pageSetup paperSize="9" orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="fr-FR"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1900" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Suivi charge Iteration 4</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.3703257666722547"/>
+          <c:y val="2.6986506746626688E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.5640078243859845E-2"/>
+          <c:y val="0.15742128935532515"/>
+          <c:w val="0.92946294640153049"/>
+          <c:h val="0.70464767616192503"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Iteration 4'!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Iteration </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:srgbClr val="000080"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="000080"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="000080"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Iteration 4'!$C$2:$R$2</c:f>
+              <c:numCache>
+                <c:formatCode>[$-40C]d\-mmm;@</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>41442</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41443</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41444</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41445</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41446</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41449</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41450</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41451</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41452</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41453</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41456</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41457</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41458</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41459</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41460</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41463</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Iteration 4'!$C$8:$R$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Iteration 4'!$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>REF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:srgbClr val="FF00FF"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF00FF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="FF00FF"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Iteration 4'!$C$2:$R$2</c:f>
+              <c:numCache>
+                <c:formatCode>[$-40C]d\-mmm;@</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>41442</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41443</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41444</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41445</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41446</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41449</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41450</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41451</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41452</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41453</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41456</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41457</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41458</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41459</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41460</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41463</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Iteration 4'!$C$10:$R$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.133333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.266666666666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.533333333333331</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.93333333333333</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.066666666666663</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.3333333333333286</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.4666666666666615</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.5999999999999943</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.7333333333333276</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.8666666666666609</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-5.773159728050814E-15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="101160448"/>
+        <c:axId val="101162368"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="101160448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="[$-40C]d\-mmm;@" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="3175">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1575" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="101162368"/>
+        <c:crosses val="autoZero"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="101162368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="3175">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="3175">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1575" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="101160448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.82639198178585549"/>
+          <c:y val="3.2983508245877091E-2"/>
+          <c:w val="0.11675295106908352"/>
+          <c:h val="9.145427286356822E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="3175">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1445" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:ea typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln w="3175">
+      <a:solidFill>
+        <a:srgbClr val="000000"/>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1575" b="0" i="0" u="none" strike="noStrike" baseline="0">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Arial"/>
+          <a:ea typeface="Arial"/>
+          <a:cs typeface="Arial"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter alignWithMargins="0"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000233" footer="0.49212598450000233"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -4623,7 +4651,7 @@
       <pane xSplit="4" ySplit="5" topLeftCell="E21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
+      <selection pane="bottomRight" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -6048,10 +6076,10 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A54:A55 B48:C48 D49:E51 H48:K48 A46:A49 B37:E37 D15 D38:E38 D41 B36:C37 H36:K37 E36:E37 A35:A43 D26 B28:C31 A13:A22 H28:K31 D20:E21 E25:E26 A25:A31 D28 D30 E28:E31 B12:E12 D13:E13 B13:C17 H12:K17 E13:E15 E17:E19">
-    <cfRule type="expression" dxfId="31" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="49" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="50" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8585,18 +8613,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11 A3:B11 F3:G7 H3:R11">
-    <cfRule type="expression" dxfId="29" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="53" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="54" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B10 A3:A7 A11:B11">
-    <cfRule type="expression" dxfId="27" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="31" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="32" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8612,7 +8640,7 @@
   <dimension ref="A1:DP85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -8854,8 +8882,12 @@
       <c r="J4" s="167">
         <v>0</v>
       </c>
-      <c r="K4" s="167"/>
-      <c r="L4" s="167"/>
+      <c r="K4" s="167">
+        <v>0</v>
+      </c>
+      <c r="L4" s="167">
+        <v>0</v>
+      </c>
       <c r="M4" s="167"/>
       <c r="N4" s="167"/>
       <c r="O4" s="167"/>
@@ -8892,8 +8924,12 @@
       <c r="J5" s="167">
         <v>0</v>
       </c>
-      <c r="K5" s="167"/>
-      <c r="L5" s="167"/>
+      <c r="K5" s="167">
+        <v>0</v>
+      </c>
+      <c r="L5" s="167">
+        <v>0</v>
+      </c>
       <c r="M5" s="167"/>
       <c r="N5" s="167"/>
       <c r="O5" s="167"/>
@@ -8930,8 +8966,12 @@
       <c r="J6" s="156">
         <v>0</v>
       </c>
-      <c r="K6" s="156"/>
-      <c r="L6" s="156"/>
+      <c r="K6" s="156">
+        <v>0</v>
+      </c>
+      <c r="L6" s="156">
+        <v>0</v>
+      </c>
       <c r="M6" s="156"/>
       <c r="N6" s="156"/>
       <c r="O6" s="156"/>
@@ -8968,8 +9008,12 @@
       <c r="J7" s="156">
         <v>0</v>
       </c>
-      <c r="K7" s="156"/>
-      <c r="L7" s="156"/>
+      <c r="K7" s="156">
+        <v>0</v>
+      </c>
+      <c r="L7" s="156">
+        <v>0</v>
+      </c>
       <c r="M7" s="156"/>
       <c r="N7" s="156"/>
       <c r="O7" s="156"/>
@@ -9006,8 +9050,12 @@
       <c r="J8" s="167">
         <v>0</v>
       </c>
-      <c r="K8" s="156"/>
-      <c r="L8" s="156"/>
+      <c r="K8" s="167">
+        <v>0</v>
+      </c>
+      <c r="L8" s="167">
+        <v>0</v>
+      </c>
       <c r="M8" s="156"/>
       <c r="N8" s="156"/>
       <c r="O8" s="156"/>
@@ -9043,11 +9091,15 @@
       <c r="I9" s="153">
         <v>2</v>
       </c>
-      <c r="J9" s="72">
+      <c r="J9" s="153">
         <v>1</v>
       </c>
-      <c r="K9" s="156"/>
-      <c r="L9" s="156"/>
+      <c r="K9" s="72">
+        <v>1</v>
+      </c>
+      <c r="L9" s="72">
+        <v>1</v>
+      </c>
       <c r="M9" s="156"/>
       <c r="N9" s="156"/>
       <c r="O9" s="156"/>
@@ -9083,11 +9135,15 @@
       <c r="I10" s="153">
         <v>3</v>
       </c>
-      <c r="J10" s="72">
+      <c r="J10" s="153">
         <v>3</v>
       </c>
-      <c r="K10" s="156"/>
-      <c r="L10" s="156"/>
+      <c r="K10" s="153">
+        <v>2</v>
+      </c>
+      <c r="L10" s="72">
+        <v>1</v>
+      </c>
       <c r="M10" s="156"/>
       <c r="N10" s="156"/>
       <c r="O10" s="156"/>
@@ -9123,11 +9179,15 @@
       <c r="I11" s="153">
         <v>6</v>
       </c>
-      <c r="J11" s="72">
+      <c r="J11" s="153">
         <v>3</v>
       </c>
-      <c r="K11" s="156"/>
-      <c r="L11" s="156"/>
+      <c r="K11" s="72">
+        <v>2</v>
+      </c>
+      <c r="L11" s="72">
+        <v>1</v>
+      </c>
       <c r="M11" s="156"/>
       <c r="N11" s="156"/>
       <c r="O11" s="156"/>
@@ -9148,8 +9208,8 @@
       <c r="H12" s="158"/>
       <c r="I12" s="91"/>
       <c r="J12" s="91"/>
-      <c r="K12" s="169"/>
-      <c r="L12" s="169"/>
+      <c r="K12" s="91"/>
+      <c r="L12" s="91"/>
       <c r="M12" s="169"/>
       <c r="N12" s="169"/>
       <c r="O12" s="169"/>
@@ -9185,11 +9245,15 @@
       <c r="I13" s="153">
         <v>6</v>
       </c>
-      <c r="J13" s="72">
+      <c r="J13" s="153">
         <v>5</v>
       </c>
-      <c r="K13" s="170"/>
-      <c r="L13" s="170"/>
+      <c r="K13" s="72">
+        <v>1</v>
+      </c>
+      <c r="L13" s="72">
+        <v>1</v>
+      </c>
       <c r="M13" s="170"/>
       <c r="N13" s="170"/>
       <c r="O13" s="170"/>
@@ -9228,8 +9292,12 @@
       <c r="J14" s="72">
         <v>6</v>
       </c>
-      <c r="K14" s="155"/>
-      <c r="L14" s="155"/>
+      <c r="K14" s="72">
+        <v>6</v>
+      </c>
+      <c r="L14" s="72">
+        <v>6</v>
+      </c>
       <c r="M14" s="155"/>
       <c r="N14" s="155"/>
       <c r="O14" s="155"/>
@@ -9268,8 +9336,12 @@
       <c r="J15" s="72">
         <v>6</v>
       </c>
-      <c r="K15" s="155"/>
-      <c r="L15" s="155"/>
+      <c r="K15" s="72">
+        <v>6</v>
+      </c>
+      <c r="L15" s="72">
+        <v>6</v>
+      </c>
       <c r="M15" s="155"/>
       <c r="N15" s="155"/>
       <c r="O15" s="155"/>
@@ -9336,13 +9408,13 @@
         <f t="array" ref="J17">IF(ISBLANK(J4:J15), NA(), SUM(J4:J15))</f>
         <v>24</v>
       </c>
-      <c r="K17" s="38" t="e">
+      <c r="K17" s="38">
         <f t="array" ref="K17">IF(ISBLANK(K4:K15), NA(), SUM(K4:K15))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L17" s="38" t="e">
+        <v>18</v>
+      </c>
+      <c r="L17" s="38">
         <f t="array" ref="L17">IF(ISBLANK(L4:L15), NA(), SUM(L4:L15))</f>
-        <v>#N/A</v>
+        <v>16</v>
       </c>
       <c r="M17" s="38" t="e">
         <f t="array" ref="M17">IF(ISBLANK(M4:M15), NA(), SUM(M4:M15))</f>
@@ -9505,13 +9577,13 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="K18" s="38" t="e">
+      <c r="K18" s="38">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="L18" s="38" t="e">
+        <v>6</v>
+      </c>
+      <c r="L18" s="38">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>2</v>
       </c>
       <c r="M18" s="38" t="e">
         <f t="shared" si="0"/>
@@ -9650,63 +9722,63 @@
         <v>49</v>
       </c>
       <c r="D19" s="46">
-        <f>C19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" ref="D19:R19" si="1">C19-$C$17/COUNTA($C$2:$Q$2)</f>
         <v>45.733333333333334</v>
       </c>
       <c r="E19" s="46">
-        <f>D19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>42.466666666666669</v>
       </c>
       <c r="F19" s="46">
-        <f>E19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>39.200000000000003</v>
       </c>
       <c r="G19" s="46">
-        <f>F19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>35.933333333333337</v>
       </c>
       <c r="H19" s="46">
-        <f>G19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>32.666666666666671</v>
       </c>
       <c r="I19" s="46">
-        <f>H19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>29.400000000000006</v>
       </c>
       <c r="J19" s="46">
-        <f>I19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>26.13333333333334</v>
       </c>
       <c r="K19" s="46">
-        <f>J19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>22.866666666666674</v>
       </c>
       <c r="L19" s="46">
-        <f>K19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>19.600000000000009</v>
       </c>
       <c r="M19" s="46">
-        <f>L19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>16.333333333333343</v>
       </c>
       <c r="N19" s="46">
-        <f>M19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>13.066666666666677</v>
       </c>
       <c r="O19" s="46">
-        <f>N19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>9.8000000000000114</v>
       </c>
       <c r="P19" s="46">
-        <f>O19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>6.5333333333333448</v>
       </c>
       <c r="Q19" s="46">
-        <f>P19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>3.2666666666666782</v>
       </c>
       <c r="R19" s="46">
-        <f>Q19-$C$17/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="1"/>
         <v>1.1546319456101628E-14</v>
       </c>
     </row>
@@ -9720,63 +9792,63 @@
         <v>0</v>
       </c>
       <c r="D20" s="58">
-        <f t="shared" ref="D20:R20" si="1">1-D17/$C$17</f>
+        <f t="shared" ref="D20:R20" si="2">1-D17/$C$17</f>
         <v>0</v>
       </c>
       <c r="E20" s="58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1428571428571429</v>
       </c>
       <c r="F20" s="58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.18367346938775508</v>
       </c>
       <c r="G20" s="58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.32653061224489799</v>
       </c>
       <c r="H20" s="58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.32653061224489799</v>
       </c>
       <c r="I20" s="58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.40816326530612246</v>
       </c>
       <c r="J20" s="58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.51020408163265307</v>
       </c>
-      <c r="K20" s="58" t="e">
-        <f t="shared" si="1"/>
+      <c r="K20" s="58">
+        <f t="shared" si="2"/>
+        <v>0.63265306122448983</v>
+      </c>
+      <c r="L20" s="58">
+        <f t="shared" si="2"/>
+        <v>0.67346938775510212</v>
+      </c>
+      <c r="M20" s="58" t="e">
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="L20" s="58" t="e">
-        <f t="shared" si="1"/>
+      <c r="N20" s="58" t="e">
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="M20" s="58" t="e">
-        <f t="shared" si="1"/>
+      <c r="O20" s="58" t="e">
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="N20" s="58" t="e">
-        <f t="shared" si="1"/>
+      <c r="P20" s="58" t="e">
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="O20" s="58" t="e">
-        <f t="shared" si="1"/>
+      <c r="Q20" s="58" t="e">
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="P20" s="58" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="Q20" s="58" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
       <c r="R20" s="58" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -11081,11 +11153,11 @@
       <c r="R85" s="38"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B13:B15 E13:G13 B3:B11 A3:A15 C6:D8 D14:R15 D3:R12 G4:J15">
-    <cfRule type="expression" dxfId="1" priority="37" stopIfTrue="1">
+  <conditionalFormatting sqref="B13:B15 E13:G13 B3:B11 A3:A15 C6:D8 D14:R15 D3:R12 G4:L15">
+    <cfRule type="expression" dxfId="29" priority="37" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="38" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13080,50 +13152,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:R9 A3:A9 B3 B5:B6 B8:B9">
-    <cfRule type="expression" dxfId="25" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="27" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="28" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9 A4:A7 B3 B5:B6 B8:B9">
-    <cfRule type="expression" dxfId="23" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="25" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="26" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5 A7">
-    <cfRule type="expression" dxfId="21" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="23" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="24" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3 B5:B6 B8:B10">
-    <cfRule type="expression" dxfId="19" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="5" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="6" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4 A7">
-    <cfRule type="expression" dxfId="17" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B10 B3 B5:B6">
-    <cfRule type="expression" dxfId="15" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="1" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="2" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15243,50 +15315,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:B6 D3:R6">
-    <cfRule type="expression" dxfId="13" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="25" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="26" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B6 A4:B6">
-    <cfRule type="expression" dxfId="11" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="23" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="24" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="expression" dxfId="9" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="21" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="22" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B5">
-    <cfRule type="expression" dxfId="7" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="5" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="6" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A7">
-    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B5">
-    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
correction fixtures : nouvelle scène
</commit_message>
<xml_diff>
--- a/doc/Backlog [ACONIT].xlsx
+++ b/doc/Backlog [ACONIT].xlsx
@@ -39,10 +39,10 @@
   </definedNames>
   <calcPr calcId="125725"/>
   <customWorkbookViews>
+    <customWorkbookView name="Yoann Regardin - Affichage personnalisé" guid="{29B12ED2-AD48-4E1C-B971-77E4D76C1B5F}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="609" activeSheetId="2"/>
+    <customWorkbookView name="uvba7442 - Affichage personnalisé" guid="{38566435-C99E-4958-9169-0C5C493EE97D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1213" windowHeight="665" activeSheetId="1"/>
+    <customWorkbookView name="Didier Lassissi - Affichage personnalisé" guid="{5E22A59B-ECE7-4B50-9619-81A99F53295A}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1064" windowHeight="552" activeSheetId="1"/>
     <customWorkbookView name="Bernard Notarianni - Affichage personnalisé" guid="{178C21D0-B00A-4B0E-B009-71AAC80909BC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="785" activeSheetId="1"/>
-    <customWorkbookView name="Didier Lassissi - Affichage personnalisé" guid="{5E22A59B-ECE7-4B50-9619-81A99F53295A}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1064" windowHeight="552" activeSheetId="1"/>
-    <customWorkbookView name="uvba7442 - Affichage personnalisé" guid="{38566435-C99E-4958-9169-0C5C493EE97D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1213" windowHeight="665" activeSheetId="1"/>
-    <customWorkbookView name="Yoann Regardin - Affichage personnalisé" guid="{29B12ED2-AD48-4E1C-B971-77E4D76C1B5F}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="609" activeSheetId="2"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
@@ -1967,7 +1967,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.3703257666722547"/>
+          <c:x val="0.37032576667225486"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -1985,9 +1985,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532515"/>
+          <c:y val="0.15742128935532523"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192503"/>
+          <c:h val="0.70464767616192514"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2297,11 +2297,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="100215424"/>
-        <c:axId val="100238080"/>
+        <c:axId val="108517632"/>
+        <c:axId val="108740992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100215424"/>
+        <c:axId val="108517632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2333,7 +2333,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100238080"/>
+        <c:crossAx val="108740992"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2341,7 +2341,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100238080"/>
+        <c:axId val="108740992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2383,7 +2383,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100215424"/>
+        <c:crossAx val="108517632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2471,7 +2471,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000233" footer="0.49212598450000233"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000239" footer="0.49212598450000239"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2508,7 +2508,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225497"/>
+          <c:x val="0.37032576667225509"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2526,9 +2526,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532529"/>
+          <c:y val="0.15742128935532534"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192525"/>
+          <c:h val="0.70464767616192536"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2838,11 +2838,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="100140544"/>
-        <c:axId val="100142464"/>
+        <c:axId val="110269568"/>
+        <c:axId val="110271488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100140544"/>
+        <c:axId val="110269568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2874,7 +2874,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100142464"/>
+        <c:crossAx val="110271488"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2882,7 +2882,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100142464"/>
+        <c:axId val="110271488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2924,7 +2924,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100140544"/>
+        <c:crossAx val="110269568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3012,7 +3012,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000244" footer="0.49212598450000244"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.4921259845000025" footer="0.4921259845000025"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3049,7 +3049,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225525"/>
+          <c:x val="0.37032576667225542"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3067,9 +3067,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.1574212893553254"/>
+          <c:y val="0.15742128935532546"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192558"/>
+          <c:h val="0.70464767616192581"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3187,10 +3187,10 @@
                   <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>#N/A</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>#N/A</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>#N/A</c:v>
@@ -3379,11 +3379,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="100601856"/>
-        <c:axId val="100603776"/>
+        <c:axId val="110329216"/>
+        <c:axId val="110351872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100601856"/>
+        <c:axId val="110329216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3415,7 +3415,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100603776"/>
+        <c:crossAx val="110351872"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3423,7 +3423,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100603776"/>
+        <c:axId val="110351872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3465,7 +3465,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100601856"/>
+        <c:crossAx val="110329216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3553,7 +3553,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000256" footer="0.49212598450000256"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000261" footer="0.49212598450000261"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3590,7 +3590,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225553"/>
+          <c:x val="0.3703257666722557"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3608,9 +3608,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532551"/>
+          <c:y val="0.15742128935532557"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192592"/>
+          <c:h val="0.70464767616192603"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3920,11 +3920,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="100763904"/>
-        <c:axId val="100786560"/>
+        <c:axId val="110196608"/>
+        <c:axId val="110206976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100763904"/>
+        <c:axId val="110196608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3956,7 +3956,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100786560"/>
+        <c:crossAx val="110206976"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3964,7 +3964,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100786560"/>
+        <c:axId val="110206976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4006,7 +4006,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100763904"/>
+        <c:crossAx val="110196608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4094,7 +4094,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000267" footer="0.49212598450000267"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000272" footer="0.49212598450000272"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -11114,7 +11114,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:DP80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
@@ -11340,11 +11342,15 @@
       <c r="E4" s="72">
         <v>1</v>
       </c>
-      <c r="F4" s="72">
+      <c r="F4" s="145">
         <v>1</v>
       </c>
-      <c r="G4" s="95"/>
-      <c r="H4" s="95"/>
+      <c r="G4" s="72">
+        <v>0</v>
+      </c>
+      <c r="H4" s="72">
+        <v>0</v>
+      </c>
       <c r="I4" s="95"/>
       <c r="J4" s="95"/>
       <c r="K4" s="95"/>
@@ -11370,11 +11376,15 @@
       <c r="E5" s="72">
         <v>1</v>
       </c>
-      <c r="F5" s="72">
+      <c r="F5" s="145">
         <v>1</v>
       </c>
-      <c r="G5" s="95"/>
-      <c r="H5" s="95"/>
+      <c r="G5" s="72">
+        <v>0</v>
+      </c>
+      <c r="H5" s="72">
+        <v>0</v>
+      </c>
       <c r="I5" s="95"/>
       <c r="J5" s="95"/>
       <c r="K5" s="95"/>
@@ -11403,8 +11413,12 @@
       <c r="F6" s="72">
         <v>3</v>
       </c>
-      <c r="G6" s="95"/>
-      <c r="H6" s="95"/>
+      <c r="G6" s="145">
+        <v>3</v>
+      </c>
+      <c r="H6" s="72">
+        <v>2</v>
+      </c>
       <c r="I6" s="95"/>
       <c r="J6" s="95"/>
       <c r="K6" s="95"/>
@@ -11433,8 +11447,12 @@
       <c r="F7" s="72">
         <v>5</v>
       </c>
-      <c r="G7" s="95"/>
-      <c r="H7" s="95"/>
+      <c r="G7" s="72">
+        <v>5</v>
+      </c>
+      <c r="H7" s="72">
+        <v>5</v>
+      </c>
       <c r="I7" s="95"/>
       <c r="J7" s="95"/>
       <c r="K7" s="95"/>
@@ -11455,8 +11473,8 @@
       <c r="D8" s="91"/>
       <c r="E8" s="91"/>
       <c r="F8" s="91"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
+      <c r="G8" s="91"/>
+      <c r="H8" s="91"/>
       <c r="I8" s="93"/>
       <c r="J8" s="93"/>
       <c r="K8" s="93"/>
@@ -11484,11 +11502,15 @@
       <c r="E9" s="147">
         <v>5</v>
       </c>
-      <c r="F9" s="147">
+      <c r="F9" s="145">
         <v>5</v>
       </c>
-      <c r="G9" s="95"/>
-      <c r="H9" s="95"/>
+      <c r="G9" s="145">
+        <v>3</v>
+      </c>
+      <c r="H9" s="147">
+        <v>1</v>
+      </c>
       <c r="I9" s="95"/>
       <c r="J9" s="95"/>
       <c r="K9" s="95"/>
@@ -11509,8 +11531,8 @@
       <c r="D10" s="91"/>
       <c r="E10" s="91"/>
       <c r="F10" s="91"/>
-      <c r="G10" s="95"/>
-      <c r="H10" s="95"/>
+      <c r="G10" s="91"/>
+      <c r="H10" s="91"/>
       <c r="I10" s="95"/>
       <c r="J10" s="95"/>
       <c r="K10" s="95"/>
@@ -11541,8 +11563,12 @@
       <c r="F11" s="72">
         <v>20</v>
       </c>
-      <c r="G11" s="92"/>
-      <c r="H11" s="92"/>
+      <c r="G11" s="145">
+        <v>20</v>
+      </c>
+      <c r="H11" s="72">
+        <v>16</v>
+      </c>
       <c r="I11" s="92"/>
       <c r="J11" s="92"/>
       <c r="K11" s="92"/>
@@ -11563,8 +11589,8 @@
       <c r="D12" s="91"/>
       <c r="E12" s="91"/>
       <c r="F12" s="91"/>
-      <c r="G12" s="94"/>
-      <c r="H12" s="94"/>
+      <c r="G12" s="91"/>
+      <c r="H12" s="91"/>
       <c r="I12" s="94"/>
       <c r="J12" s="94"/>
       <c r="K12" s="94"/>
@@ -11595,8 +11621,12 @@
       <c r="F13" s="72">
         <v>10</v>
       </c>
-      <c r="G13" s="94"/>
-      <c r="H13" s="94"/>
+      <c r="G13" s="72">
+        <v>10</v>
+      </c>
+      <c r="H13" s="72">
+        <v>10</v>
+      </c>
       <c r="I13" s="94"/>
       <c r="J13" s="94"/>
       <c r="K13" s="94"/>
@@ -11621,7 +11651,7 @@
         <v>52</v>
       </c>
       <c r="D15" s="38">
-        <f t="shared" ref="D15:R15" si="0">IF(ISBLANK(D4:D13), NA(), SUM(D3:D13))</f>
+        <f t="shared" ref="D15:E15" si="0">IF(ISBLANK(D4:D13), NA(), SUM(D3:D13))</f>
         <v>47</v>
       </c>
       <c r="E15" s="38">
@@ -11632,13 +11662,13 @@
         <f t="array" ref="F15">IF(ISBLANK(F4:F13), NA(), SUM(F3:F13))</f>
         <v>45</v>
       </c>
-      <c r="G15" s="38" t="e">
+      <c r="G15" s="38">
         <f t="array" ref="G15">IF(ISBLANK(G4:G13), NA(), SUM(G3:G13))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H15" s="38" t="e">
+        <v>41</v>
+      </c>
+      <c r="H15" s="38">
         <f t="array" ref="H15">IF(ISBLANK(H4:H13), NA(), SUM(H3:H13))</f>
-        <v>#N/A</v>
+        <v>34</v>
       </c>
       <c r="I15" s="38" t="e">
         <f t="array" ref="I15">IF(ISBLANK(I4:I13), NA(), SUM(I3:I13))</f>
@@ -11699,13 +11729,13 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G16" s="38" t="e">
+      <c r="G16" s="38">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H16" s="38" t="e">
+        <v>4</v>
+      </c>
+      <c r="H16" s="38">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>7</v>
       </c>
       <c r="I16" s="38" t="e">
         <f t="shared" si="1"/>
@@ -11758,63 +11788,63 @@
         <v>52</v>
       </c>
       <c r="D17" s="46">
-        <f>C17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" ref="D17:R17" si="2">C17-$C$15/COUNTA($C$2:$Q$2)</f>
         <v>48.533333333333331</v>
       </c>
       <c r="E17" s="46">
-        <f>D17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>45.066666666666663</v>
       </c>
       <c r="F17" s="46">
-        <f>E17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>41.599999999999994</v>
       </c>
       <c r="G17" s="46">
-        <f>F17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>38.133333333333326</v>
       </c>
       <c r="H17" s="46">
-        <f>G17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>34.666666666666657</v>
       </c>
       <c r="I17" s="46">
-        <f>H17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>31.199999999999989</v>
       </c>
       <c r="J17" s="46">
-        <f>I17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>27.73333333333332</v>
       </c>
       <c r="K17" s="46">
-        <f>J17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>24.266666666666652</v>
       </c>
       <c r="L17" s="46">
-        <f>K17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>20.799999999999983</v>
       </c>
       <c r="M17" s="46">
-        <f>L17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>17.333333333333314</v>
       </c>
       <c r="N17" s="46">
-        <f>M17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>13.866666666666648</v>
       </c>
       <c r="O17" s="46">
-        <f>N17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>10.399999999999981</v>
       </c>
       <c r="P17" s="46">
-        <f>O17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>6.933333333333314</v>
       </c>
       <c r="Q17" s="46">
-        <f>P17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>3.4666666666666472</v>
       </c>
       <c r="R17" s="52">
-        <f>Q17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>-1.9539925233402755E-14</v>
       </c>
     </row>
@@ -11824,67 +11854,67 @@
         <v>40</v>
       </c>
       <c r="C18" s="58">
-        <f t="shared" ref="C18:R18" si="2">1-C15/$C$15</f>
+        <f t="shared" ref="C18:R18" si="3">1-C15/$C$15</f>
         <v>0</v>
       </c>
       <c r="D18" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.6153846153846145E-2</v>
       </c>
       <c r="E18" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.13461538461538458</v>
       </c>
       <c r="F18" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.13461538461538458</v>
       </c>
-      <c r="G18" s="58" t="e">
-        <f t="shared" si="2"/>
+      <c r="G18" s="58">
+        <f t="shared" si="3"/>
+        <v>0.21153846153846156</v>
+      </c>
+      <c r="H18" s="58">
+        <f t="shared" si="3"/>
+        <v>0.34615384615384615</v>
+      </c>
+      <c r="I18" s="58" t="e">
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="H18" s="58" t="e">
-        <f t="shared" si="2"/>
+      <c r="J18" s="58" t="e">
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="I18" s="58" t="e">
-        <f t="shared" si="2"/>
+      <c r="K18" s="58" t="e">
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="J18" s="58" t="e">
-        <f t="shared" si="2"/>
+      <c r="L18" s="58" t="e">
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="K18" s="58" t="e">
-        <f t="shared" si="2"/>
+      <c r="M18" s="58" t="e">
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="L18" s="58" t="e">
-        <f t="shared" si="2"/>
+      <c r="N18" s="58" t="e">
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M18" s="58" t="e">
-        <f t="shared" si="2"/>
+      <c r="O18" s="58" t="e">
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="N18" s="58" t="e">
-        <f t="shared" si="2"/>
+      <c r="P18" s="58" t="e">
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="O18" s="58" t="e">
-        <f t="shared" si="2"/>
+      <c r="Q18" s="58" t="e">
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="P18" s="58" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="Q18" s="58" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
       <c r="R18" s="58" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -13095,19 +13125,19 @@
       <c r="R80" s="38"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B9:B10 A3:A13 B12:B13 B3:B7 G3:R13">
-    <cfRule type="expression" dxfId="3" priority="31" stopIfTrue="1">
+  <conditionalFormatting sqref="B9:B10 A3:A13 B12:B13 B3:B7 I3:R13 G3:H3">
+    <cfRule type="expression" dxfId="15" priority="31" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="32" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B13 A12 A9:A10">
-    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15227,50 +15257,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:B6 D3:R6">
-    <cfRule type="expression" dxfId="15" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="25" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="26" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B6 A4:B6">
-    <cfRule type="expression" dxfId="13" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="23" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="24" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="expression" dxfId="11" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="21" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="22" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B5">
-    <cfRule type="expression" dxfId="9" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A7">
-    <cfRule type="expression" dxfId="7" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B5">
-    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Graphe du parcours + Maj BackLog 12/06/2013
</commit_message>
<xml_diff>
--- a/doc/Backlog [ACONIT].xlsx
+++ b/doc/Backlog [ACONIT].xlsx
@@ -33,7 +33,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Product backlog'!$5:$5</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Iteration 1'!$R$12:$Z$22</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Iteration 2'!$R$16:$Z$25</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'Iteration 3'!$R$14:$Z$20</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Iteration 3'!$R$15:$Z$21</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'Iteration 4'!$R$7:$Z$16</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Product backlog'!#REF!</definedName>
   </definedNames>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="115">
   <si>
     <t>Itération</t>
   </si>
@@ -415,6 +415,9 @@
   </si>
   <si>
     <t xml:space="preserve">        - Gestion de plusieurs sous-parcours</t>
+  </si>
+  <si>
+    <t>Visualisation graphique</t>
   </si>
 </sst>
 </file>
@@ -1153,7 +1156,7 @@
     <xf numFmtId="0" fontId="26" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="5" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1643,6 +1646,7 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" xfId="43" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20 % - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1690,7 +1694,21 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vérification" xfId="42" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="26">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3079,7 +3097,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Iteration 3'!$B$15</c:f>
+              <c:f>'Iteration 3'!$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3170,7 +3188,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Iteration 3'!$C$15:$R$15</c:f>
+              <c:f>'Iteration 3'!$C$16:$R$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -3190,10 +3208,10 @@
                   <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>#N/A</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>#N/A</c:v>
@@ -3231,7 +3249,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Iteration 3'!$B$17</c:f>
+              <c:f>'Iteration 3'!$B$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3322,7 +3340,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Iteration 3'!$C$17:$R$17</c:f>
+              <c:f>'Iteration 3'!$C$18:$R$18</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="16"/>
@@ -4180,13 +4198,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>112059</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>65444</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>11204</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>62002</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4542,7 +4560,7 @@
       <pane xSplit="4" ySplit="5" topLeftCell="E30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D39" sqref="D39"/>
+      <selection pane="bottomRight" activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -5888,10 +5906,10 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A51:A52 B46:C46 D47:E48 H46:K46 A44:A47 D40 B37:E37 D15 D38:E38 B36:C37 H36:K37 E36:E37 A35:A41 D26 B28:C31 A13:A22 H28:K31 D20:E21 E25:E26 A25:A31 D28 E28:E31 B12:E12 D13:E13 B13:C17 H12:K17 E13:E15 E17:E19 D30:D31">
-    <cfRule type="expression" dxfId="23" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="53" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="54" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8425,18 +8443,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11 A3:B11 F3:G7 H3:R11">
-    <cfRule type="expression" dxfId="21" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="53" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="54" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B10 A3:A7 A11:B11">
-    <cfRule type="expression" dxfId="19" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="31" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="32" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11096,10 +11114,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B13:B15 E13:G13 D14:R15 B3:B11 A3:A15 C6:D8 G9:M15 D3:R12 N4:R15">
-    <cfRule type="expression" dxfId="17" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="37" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="38" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11112,10 +11130,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DP80"/>
+  <dimension ref="A1:DP81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -11351,7 +11369,9 @@
       <c r="H4" s="72">
         <v>0</v>
       </c>
-      <c r="I4" s="95"/>
+      <c r="I4" s="72">
+        <v>0</v>
+      </c>
       <c r="J4" s="95"/>
       <c r="K4" s="95"/>
       <c r="L4" s="95"/>
@@ -11385,7 +11405,9 @@
       <c r="H5" s="72">
         <v>0</v>
       </c>
-      <c r="I5" s="95"/>
+      <c r="I5" s="72">
+        <v>0</v>
+      </c>
       <c r="J5" s="95"/>
       <c r="K5" s="95"/>
       <c r="L5" s="95"/>
@@ -11416,10 +11438,12 @@
       <c r="G6" s="145">
         <v>3</v>
       </c>
-      <c r="H6" s="72">
+      <c r="H6" s="145">
+        <v>3</v>
+      </c>
+      <c r="I6" s="72">
         <v>2</v>
       </c>
-      <c r="I6" s="95"/>
       <c r="J6" s="95"/>
       <c r="K6" s="95"/>
       <c r="L6" s="95"/>
@@ -11453,7 +11477,9 @@
       <c r="H7" s="72">
         <v>5</v>
       </c>
-      <c r="I7" s="95"/>
+      <c r="I7" s="72">
+        <v>5</v>
+      </c>
       <c r="J7" s="95"/>
       <c r="K7" s="95"/>
       <c r="L7" s="95"/>
@@ -11475,7 +11501,7 @@
       <c r="F8" s="91"/>
       <c r="G8" s="91"/>
       <c r="H8" s="91"/>
-      <c r="I8" s="93"/>
+      <c r="I8" s="91"/>
       <c r="J8" s="93"/>
       <c r="K8" s="93"/>
       <c r="L8" s="93"/>
@@ -11494,24 +11520,26 @@
         <v>23</v>
       </c>
       <c r="C9" s="145">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D9" s="145">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E9" s="147">
-        <v>5</v>
-      </c>
-      <c r="F9" s="145">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="F9" s="147">
+        <v>1</v>
       </c>
       <c r="G9" s="147">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H9" s="147">
-        <v>5</v>
-      </c>
-      <c r="I9" s="95"/>
+        <v>1</v>
+      </c>
+      <c r="I9" s="147">
+        <v>1</v>
+      </c>
       <c r="J9" s="95"/>
       <c r="K9" s="95"/>
       <c r="L9" s="95"/>
@@ -11533,7 +11561,7 @@
       <c r="F10" s="91"/>
       <c r="G10" s="91"/>
       <c r="H10" s="91"/>
-      <c r="I10" s="95"/>
+      <c r="I10" s="91"/>
       <c r="J10" s="95"/>
       <c r="K10" s="95"/>
       <c r="L10" s="95"/>
@@ -11544,90 +11572,92 @@
       <c r="Q10" s="95"/>
       <c r="R10" s="48"/>
     </row>
-    <row r="11" spans="1:120" ht="24.95" customHeight="1">
-      <c r="A11" s="70" t="s">
+    <row r="11" spans="1:120" s="169" customFormat="1" ht="24.95" customHeight="1">
+      <c r="A11" s="151" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="147"/>
+      <c r="C11" s="147">
+        <v>4</v>
+      </c>
+      <c r="D11" s="147">
+        <v>4</v>
+      </c>
+      <c r="E11" s="147">
+        <v>4</v>
+      </c>
+      <c r="F11" s="147">
+        <v>4</v>
+      </c>
+      <c r="G11" s="147">
+        <v>4</v>
+      </c>
+      <c r="H11" s="145">
+        <v>4</v>
+      </c>
+      <c r="I11" s="147">
+        <v>3</v>
+      </c>
+      <c r="J11" s="95"/>
+      <c r="K11" s="95"/>
+      <c r="L11" s="95"/>
+      <c r="M11" s="95"/>
+      <c r="N11" s="95"/>
+      <c r="O11" s="95"/>
+      <c r="P11" s="95"/>
+      <c r="Q11" s="95"/>
+      <c r="R11" s="95"/>
+    </row>
+    <row r="12" spans="1:120" ht="24.95" customHeight="1">
+      <c r="A12" s="70" t="s">
         <v>103</v>
       </c>
-      <c r="B11" s="75">
+      <c r="B12" s="75">
         <v>27</v>
       </c>
-      <c r="C11" s="72">
+      <c r="C12" s="72">
         <v>20</v>
       </c>
-      <c r="D11" s="72">
+      <c r="D12" s="72">
         <v>20</v>
       </c>
-      <c r="E11" s="72">
+      <c r="E12" s="72">
         <v>20</v>
       </c>
-      <c r="F11" s="72">
+      <c r="F12" s="72">
         <v>20</v>
       </c>
-      <c r="G11" s="145">
+      <c r="G12" s="145">
         <v>20</v>
       </c>
-      <c r="H11" s="72">
+      <c r="H12" s="145">
         <v>16</v>
       </c>
-      <c r="I11" s="92"/>
-      <c r="J11" s="92"/>
-      <c r="K11" s="92"/>
-      <c r="L11" s="92"/>
-      <c r="M11" s="92"/>
-      <c r="N11" s="92"/>
-      <c r="O11" s="92"/>
-      <c r="P11" s="92"/>
-      <c r="Q11" s="92"/>
-      <c r="R11" s="49"/>
-    </row>
-    <row r="12" spans="1:120" ht="24.95" customHeight="1">
-      <c r="A12" s="89" t="s">
+      <c r="I12" s="72">
+        <v>13</v>
+      </c>
+      <c r="J12" s="92"/>
+      <c r="K12" s="92"/>
+      <c r="L12" s="92"/>
+      <c r="M12" s="92"/>
+      <c r="N12" s="92"/>
+      <c r="O12" s="92"/>
+      <c r="P12" s="92"/>
+      <c r="Q12" s="92"/>
+      <c r="R12" s="49"/>
+    </row>
+    <row r="13" spans="1:120" ht="24.95" customHeight="1">
+      <c r="A13" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="75"/>
-      <c r="C12" s="91"/>
-      <c r="D12" s="91"/>
-      <c r="E12" s="91"/>
-      <c r="F12" s="91"/>
-      <c r="G12" s="91"/>
-      <c r="H12" s="91"/>
-      <c r="I12" s="94"/>
-      <c r="J12" s="94"/>
-      <c r="K12" s="94"/>
-      <c r="L12" s="94"/>
-      <c r="M12" s="94"/>
-      <c r="N12" s="94"/>
-      <c r="O12" s="94"/>
-      <c r="P12" s="94"/>
-      <c r="Q12" s="94"/>
-      <c r="R12" s="49"/>
-    </row>
-    <row r="13" spans="1:120" ht="24.95" customHeight="1">
-      <c r="A13" s="82" t="s">
-        <v>104</v>
-      </c>
-      <c r="B13" s="75">
-        <v>30</v>
-      </c>
-      <c r="C13" s="72">
-        <v>10</v>
-      </c>
-      <c r="D13" s="72">
-        <v>10</v>
-      </c>
-      <c r="E13" s="72">
-        <v>10</v>
-      </c>
-      <c r="F13" s="72">
-        <v>10</v>
-      </c>
-      <c r="G13" s="72">
-        <v>10</v>
-      </c>
-      <c r="H13" s="72">
-        <v>10</v>
-      </c>
-      <c r="I13" s="94"/>
+      <c r="B13" s="75"/>
+      <c r="C13" s="91"/>
+      <c r="D13" s="91"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="91"/>
+      <c r="G13" s="91"/>
+      <c r="H13" s="91"/>
+      <c r="I13" s="91"/>
       <c r="J13" s="94"/>
       <c r="K13" s="94"/>
       <c r="L13" s="94"/>
@@ -11638,311 +11668,329 @@
       <c r="Q13" s="94"/>
       <c r="R13" s="49"/>
     </row>
-    <row r="14" spans="1:120">
-      <c r="A14" s="38"/>
-    </row>
-    <row r="15" spans="1:120" s="56" customFormat="1">
-      <c r="A15" s="55"/>
-      <c r="B15" s="43" t="s">
+    <row r="14" spans="1:120" ht="24.95" customHeight="1">
+      <c r="A14" s="82" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="75">
+        <v>30</v>
+      </c>
+      <c r="C14" s="72">
+        <v>10</v>
+      </c>
+      <c r="D14" s="72">
+        <v>10</v>
+      </c>
+      <c r="E14" s="72">
+        <v>10</v>
+      </c>
+      <c r="F14" s="72">
+        <v>10</v>
+      </c>
+      <c r="G14" s="72">
+        <v>10</v>
+      </c>
+      <c r="H14" s="72">
+        <v>10</v>
+      </c>
+      <c r="I14" s="72">
+        <v>10</v>
+      </c>
+      <c r="J14" s="94"/>
+      <c r="K14" s="94"/>
+      <c r="L14" s="94"/>
+      <c r="M14" s="94"/>
+      <c r="N14" s="94"/>
+      <c r="O14" s="94"/>
+      <c r="P14" s="94"/>
+      <c r="Q14" s="94"/>
+      <c r="R14" s="49"/>
+    </row>
+    <row r="15" spans="1:120">
+      <c r="A15" s="38"/>
+    </row>
+    <row r="16" spans="1:120" s="56" customFormat="1">
+      <c r="A16" s="55"/>
+      <c r="B16" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="38">
-        <f>IF(ISBLANK(C4:C13), NA(), SUM(C3:C13))</f>
+      <c r="C16" s="38">
+        <f>IF(ISBLANK(C4:C14), NA(), SUM(C3:C14))</f>
         <v>52</v>
       </c>
-      <c r="D15" s="38">
-        <f t="shared" ref="D15:E15" si="0">IF(ISBLANK(D4:D13), NA(), SUM(D3:D13))</f>
+      <c r="D16" s="38">
+        <f t="shared" ref="D16:E16" si="0">IF(ISBLANK(D4:D14), NA(), SUM(D3:D14))</f>
         <v>47</v>
       </c>
-      <c r="E15" s="38">
+      <c r="E16" s="38">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="F15" s="38">
-        <f t="array" ref="F15">IF(ISBLANK(F4:F13), NA(), SUM(F3:F13))</f>
+      <c r="F16" s="38">
+        <f t="array" ref="F16">IF(ISBLANK(F4:F14), NA(), SUM(F3:F14))</f>
         <v>45</v>
       </c>
-      <c r="G15" s="38">
-        <f t="array" ref="G15">IF(ISBLANK(G4:G13), NA(), SUM(G3:G13))</f>
+      <c r="G16" s="38">
+        <f t="array" ref="G16">IF(ISBLANK(G4:G14), NA(), SUM(G3:G14))</f>
         <v>43</v>
       </c>
-      <c r="H15" s="38">
-        <f t="array" ref="H15">IF(ISBLANK(H4:H13), NA(), SUM(H3:H13))</f>
+      <c r="H16" s="38">
+        <f t="array" ref="H16">IF(ISBLANK(H4:H14), NA(), SUM(H3:H14))</f>
+        <v>39</v>
+      </c>
+      <c r="I16" s="38">
+        <f t="array" ref="I16">IF(ISBLANK(I4:I14), NA(), SUM(I3:I14))</f>
+        <v>34</v>
+      </c>
+      <c r="J16" s="38" t="e">
+        <f t="array" ref="J16">IF(ISBLANK(J4:J14), NA(), SUM(J3:J14))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K16" s="38" t="e">
+        <f t="array" ref="K16">IF(ISBLANK(K4:K14), NA(), SUM(K3:K14))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L16" s="38" t="e">
+        <f t="array" ref="L16">IF(ISBLANK(L4:L14), NA(), SUM(L3:L14))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M16" s="38" t="e">
+        <f t="array" ref="M16">IF(ISBLANK(M4:M14), NA(), SUM(M3:M14))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N16" s="38" t="e">
+        <f t="array" ref="N16">IF(ISBLANK(N4:N14), NA(), SUM(N3:N14))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O16" s="38" t="e">
+        <f t="array" ref="O16">IF(ISBLANK(O4:O14), NA(), SUM(O3:O14))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P16" s="38" t="e">
+        <f t="array" ref="P16">IF(ISBLANK(P4:P14), NA(), SUM(P3:P14))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q16" s="38" t="e">
+        <f t="array" ref="Q16">IF(ISBLANK(Q4:Q14), NA(), SUM(Q3:Q14))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R16" s="38" t="e">
+        <f t="array" ref="R16">IF(ISBLANK(R4:R14), NA(), SUM(R3:R14))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="25.5">
+      <c r="A17" s="38"/>
+      <c r="B17" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="I15" s="38" t="e">
-        <f t="array" ref="I15">IF(ISBLANK(I4:I13), NA(), SUM(I3:I13))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J15" s="38" t="e">
-        <f t="array" ref="J15">IF(ISBLANK(J4:J13), NA(), SUM(J3:J13))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K15" s="38" t="e">
-        <f t="array" ref="K15">IF(ISBLANK(K4:K13), NA(), SUM(K3:K13))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L15" s="38" t="e">
-        <f t="array" ref="L15">IF(ISBLANK(L4:L13), NA(), SUM(L3:L13))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M15" s="38" t="e">
-        <f t="array" ref="M15">IF(ISBLANK(M4:M13), NA(), SUM(M3:M13))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N15" s="38" t="e">
-        <f t="array" ref="N15">IF(ISBLANK(N4:N13), NA(), SUM(N3:N13))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O15" s="38" t="e">
-        <f t="array" ref="O15">IF(ISBLANK(O4:O13), NA(), SUM(O3:O13))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P15" s="38" t="e">
-        <f t="array" ref="P15">IF(ISBLANK(P4:P13), NA(), SUM(P3:P13))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q15" s="38" t="e">
-        <f t="array" ref="Q15">IF(ISBLANK(Q4:Q13), NA(), SUM(Q3:Q13))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R15" s="38" t="e">
-        <f t="array" ref="R15">IF(ISBLANK(R4:R13), NA(), SUM(R3:R13))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="16" spans="1:120" ht="25.5">
-      <c r="A16" s="38"/>
-      <c r="B16" s="43" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38">
-        <f t="shared" ref="D16:R16" si="1">C15-D15</f>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38">
+        <f t="shared" ref="D17:R17" si="1">C16-D16</f>
         <v>5</v>
       </c>
-      <c r="E16" s="38">
+      <c r="E17" s="38">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F16" s="38">
+      <c r="F17" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G16" s="38">
+      <c r="G17" s="38">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="H16" s="38">
+      <c r="H17" s="38">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I17" s="38">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="I16" s="38" t="e">
+      <c r="J17" s="38" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="J16" s="38" t="e">
+      <c r="K17" s="38" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="K16" s="38" t="e">
+      <c r="L17" s="38" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="L16" s="38" t="e">
+      <c r="M17" s="38" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="M16" s="38" t="e">
+      <c r="N17" s="38" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N16" s="38" t="e">
+      <c r="O17" s="38" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="O16" s="38" t="e">
+      <c r="P17" s="38" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="P16" s="38" t="e">
+      <c r="Q17" s="38" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="Q16" s="38" t="e">
+      <c r="R17" s="51" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="R16" s="51" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18">
-      <c r="A17" s="38"/>
-      <c r="B17" s="44" t="s">
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" s="38"/>
+      <c r="B18" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="45">
-        <f>C15</f>
+      <c r="C18" s="45">
+        <f>C16</f>
         <v>52</v>
       </c>
-      <c r="D17" s="46">
-        <f t="shared" ref="D17:R17" si="2">C17-$C$15/COUNTA($C$2:$Q$2)</f>
+      <c r="D18" s="46">
+        <f t="shared" ref="D18:R18" si="2">C18-$C$16/COUNTA($C$2:$Q$2)</f>
         <v>48.533333333333331</v>
       </c>
-      <c r="E17" s="46">
+      <c r="E18" s="46">
         <f t="shared" si="2"/>
         <v>45.066666666666663</v>
       </c>
-      <c r="F17" s="46">
+      <c r="F18" s="46">
         <f t="shared" si="2"/>
         <v>41.599999999999994</v>
       </c>
-      <c r="G17" s="46">
+      <c r="G18" s="46">
         <f t="shared" si="2"/>
         <v>38.133333333333326</v>
       </c>
-      <c r="H17" s="46">
+      <c r="H18" s="46">
         <f t="shared" si="2"/>
         <v>34.666666666666657</v>
       </c>
-      <c r="I17" s="46">
+      <c r="I18" s="46">
         <f t="shared" si="2"/>
         <v>31.199999999999989</v>
       </c>
-      <c r="J17" s="46">
+      <c r="J18" s="46">
         <f t="shared" si="2"/>
         <v>27.73333333333332</v>
       </c>
-      <c r="K17" s="46">
+      <c r="K18" s="46">
         <f t="shared" si="2"/>
         <v>24.266666666666652</v>
       </c>
-      <c r="L17" s="46">
+      <c r="L18" s="46">
         <f t="shared" si="2"/>
         <v>20.799999999999983</v>
       </c>
-      <c r="M17" s="46">
+      <c r="M18" s="46">
         <f t="shared" si="2"/>
         <v>17.333333333333314</v>
       </c>
-      <c r="N17" s="46">
+      <c r="N18" s="46">
         <f t="shared" si="2"/>
         <v>13.866666666666648</v>
       </c>
-      <c r="O17" s="46">
+      <c r="O18" s="46">
         <f t="shared" si="2"/>
         <v>10.399999999999981</v>
       </c>
-      <c r="P17" s="46">
+      <c r="P18" s="46">
         <f t="shared" si="2"/>
         <v>6.933333333333314</v>
       </c>
-      <c r="Q17" s="46">
+      <c r="Q18" s="46">
         <f t="shared" si="2"/>
         <v>3.4666666666666472</v>
       </c>
-      <c r="R17" s="52">
+      <c r="R18" s="52">
         <f t="shared" si="2"/>
         <v>-1.9539925233402755E-14</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
-      <c r="A18" s="38"/>
-      <c r="B18" s="57" t="s">
+    <row r="19" spans="1:18">
+      <c r="A19" s="38"/>
+      <c r="B19" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="58">
-        <f t="shared" ref="C18:R18" si="3">1-C15/$C$15</f>
-        <v>0</v>
-      </c>
-      <c r="D18" s="58">
+      <c r="C19" s="58">
+        <f t="shared" ref="C19:R19" si="3">1-C16/$C$16</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="58">
         <f t="shared" si="3"/>
         <v>9.6153846153846145E-2</v>
       </c>
-      <c r="E18" s="58">
+      <c r="E19" s="58">
         <f t="shared" si="3"/>
         <v>0.13461538461538458</v>
       </c>
-      <c r="F18" s="58">
+      <c r="F19" s="58">
         <f t="shared" si="3"/>
         <v>0.13461538461538458</v>
       </c>
-      <c r="G18" s="58">
+      <c r="G19" s="58">
         <f t="shared" si="3"/>
         <v>0.17307692307692313</v>
       </c>
-      <c r="H18" s="58">
+      <c r="H19" s="58">
         <f t="shared" si="3"/>
-        <v>0.26923076923076927</v>
-      </c>
-      <c r="I18" s="58" t="e">
+        <v>0.25</v>
+      </c>
+      <c r="I19" s="58">
+        <f t="shared" si="3"/>
+        <v>0.34615384615384615</v>
+      </c>
+      <c r="J19" s="58" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="J18" s="58" t="e">
+      <c r="K19" s="58" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="K18" s="58" t="e">
+      <c r="L19" s="58" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="L18" s="58" t="e">
+      <c r="M19" s="58" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M18" s="58" t="e">
+      <c r="N19" s="58" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="N18" s="58" t="e">
+      <c r="O19" s="58" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="O18" s="58" t="e">
+      <c r="P19" s="58" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="P18" s="58" t="e">
+      <c r="Q19" s="58" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="Q18" s="58" t="e">
+      <c r="R19" s="58" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="R18" s="58" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18">
-      <c r="A19" s="38"/>
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="38"/>
     </row>
     <row r="21" spans="1:18">
       <c r="A21" s="38"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38"/>
-      <c r="K21" s="38"/>
-      <c r="L21" s="38"/>
-      <c r="M21" s="38"/>
-      <c r="N21" s="38"/>
-      <c r="O21" s="38"/>
-      <c r="P21" s="38"/>
-      <c r="Q21" s="38"/>
-      <c r="R21" s="38"/>
     </row>
     <row r="22" spans="1:18">
       <c r="A22" s="38"/>
@@ -13124,20 +13172,40 @@
       <c r="Q80" s="38"/>
       <c r="R80" s="38"/>
     </row>
+    <row r="81" spans="1:18">
+      <c r="A81" s="38"/>
+      <c r="B81" s="38"/>
+      <c r="C81" s="38"/>
+      <c r="D81" s="38"/>
+      <c r="E81" s="38"/>
+      <c r="F81" s="38"/>
+      <c r="G81" s="38"/>
+      <c r="H81" s="38"/>
+      <c r="I81" s="38"/>
+      <c r="J81" s="38"/>
+      <c r="K81" s="38"/>
+      <c r="L81" s="38"/>
+      <c r="M81" s="38"/>
+      <c r="N81" s="38"/>
+      <c r="O81" s="38"/>
+      <c r="P81" s="38"/>
+      <c r="Q81" s="38"/>
+      <c r="R81" s="38"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B9:B10 A3:A13 B12:B13 B3:B7 I3:R13 G3:H3">
-    <cfRule type="expression" dxfId="15" priority="31" stopIfTrue="1">
+  <conditionalFormatting sqref="B9:B11 A3:A14 B13:B14 B3:B7 G3:I3 J3:R14 I3:I10 I12:I14">
+    <cfRule type="expression" dxfId="3" priority="31" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="32" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B13 A12 A9:A10">
-    <cfRule type="expression" dxfId="13" priority="3" stopIfTrue="1">
+  <conditionalFormatting sqref="B3:B14 A13 A9:A11">
+    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15257,50 +15325,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:B6 D3:R6">
-    <cfRule type="expression" dxfId="11" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="25" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="26" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B6 A4:B6">
-    <cfRule type="expression" dxfId="9" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="23" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="24" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="expression" dxfId="7" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="21" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="22" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B5">
-    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="5" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="6" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A7">
-    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B5">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="1" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
suppression d'un sous parcours
</commit_message>
<xml_diff>
--- a/doc/Backlog [ACONIT].xlsx
+++ b/doc/Backlog [ACONIT].xlsx
@@ -33,23 +33,23 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Product backlog'!$5:$5</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Iteration 1'!$R$12:$Z$22</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Iteration 2'!$R$16:$Z$25</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'Iteration 3'!$R$15:$Z$21</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Iteration 3'!$R$14:$Z$20</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'Iteration 4'!$R$7:$Z$16</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Product backlog'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <customWorkbookViews>
+    <customWorkbookView name="Bernard Notarianni - Affichage personnalisé" guid="{178C21D0-B00A-4B0E-B009-71AAC80909BC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="785" activeSheetId="1"/>
+    <customWorkbookView name="Didier Lassissi - Affichage personnalisé" guid="{5E22A59B-ECE7-4B50-9619-81A99F53295A}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1064" windowHeight="552" activeSheetId="1"/>
+    <customWorkbookView name="uvba7442 - Affichage personnalisé" guid="{38566435-C99E-4958-9169-0C5C493EE97D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1213" windowHeight="665" activeSheetId="1"/>
     <customWorkbookView name="Yoann Regardin - Affichage personnalisé" guid="{29B12ED2-AD48-4E1C-B971-77E4D76C1B5F}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="609" activeSheetId="2"/>
-    <customWorkbookView name="uvba7442 - Affichage personnalisé" guid="{38566435-C99E-4958-9169-0C5C493EE97D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1213" windowHeight="665" activeSheetId="1"/>
-    <customWorkbookView name="Didier Lassissi - Affichage personnalisé" guid="{5E22A59B-ECE7-4B50-9619-81A99F53295A}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1064" windowHeight="552" activeSheetId="1"/>
-    <customWorkbookView name="Bernard Notarianni - Affichage personnalisé" guid="{178C21D0-B00A-4B0E-B009-71AAC80909BC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="785" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="115">
   <si>
     <t>Itération</t>
   </si>
@@ -408,9 +408,6 @@
     <t>Système de log pour tracer toutes les actions</t>
   </si>
   <si>
-    <t>Champ coordonnées géographiques</t>
-  </si>
-  <si>
     <t xml:space="preserve">        - Gestion de plusieurs sous-parcours </t>
   </si>
   <si>
@@ -418,6 +415,9 @@
   </si>
   <si>
     <t>Visualisation graphique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        - Edition parcours avec transitions secondaires</t>
   </si>
 </sst>
 </file>
@@ -1985,7 +1985,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225509"/>
+          <c:x val="0.37032576667225525"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2003,9 +2003,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532534"/>
+          <c:y val="0.1574212893553254"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192536"/>
+          <c:h val="0.70464767616192558"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2315,11 +2315,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="100915456"/>
-        <c:axId val="101269888"/>
+        <c:axId val="105044224"/>
+        <c:axId val="105398656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100915456"/>
+        <c:axId val="105044224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2351,7 +2351,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101269888"/>
+        <c:crossAx val="105398656"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2359,7 +2359,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101269888"/>
+        <c:axId val="105398656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2401,7 +2401,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100915456"/>
+        <c:crossAx val="105044224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2489,7 +2489,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.4921259845000025" footer="0.4921259845000025"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000256" footer="0.49212598450000256"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2526,7 +2526,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225542"/>
+          <c:x val="0.37032576667225553"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2544,9 +2544,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532546"/>
+          <c:y val="0.15742128935532551"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192581"/>
+          <c:h val="0.70464767616192592"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2856,11 +2856,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="101622912"/>
-        <c:axId val="101624832"/>
+        <c:axId val="105739392"/>
+        <c:axId val="105741312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101622912"/>
+        <c:axId val="105739392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2892,7 +2892,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101624832"/>
+        <c:crossAx val="105741312"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2900,7 +2900,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101624832"/>
+        <c:axId val="105741312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2942,7 +2942,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101622912"/>
+        <c:crossAx val="105739392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3030,7 +3030,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000261" footer="0.49212598450000261"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000267" footer="0.49212598450000267"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3067,7 +3067,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.3703257666722557"/>
+          <c:x val="0.37032576667225586"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3085,9 +3085,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532557"/>
+          <c:y val="0.15742128935532565"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192603"/>
+          <c:h val="0.70464767616192614"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3097,7 +3097,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Iteration 3'!$B$16</c:f>
+              <c:f>'Iteration 3'!$B$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3188,45 +3188,45 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Iteration 3'!$C$16:$R$16</c:f>
+              <c:f>'Iteration 3'!$C$15:$R$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>52</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>47</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>39</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>#N/A</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>#N/A</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>#N/A</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>#N/A</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>#N/A</c:v>
@@ -3249,7 +3249,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Iteration 3'!$B$18</c:f>
+              <c:f>'Iteration 3'!$B$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3340,68 +3340,68 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Iteration 3'!$C$18:$R$18</c:f>
+              <c:f>'Iteration 3'!$C$17:$R$17</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>52</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48.533333333333331</c:v>
+                  <c:v>43.866666666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45.066666666666663</c:v>
+                  <c:v>40.733333333333334</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41.599999999999994</c:v>
+                  <c:v>37.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38.133333333333326</c:v>
+                  <c:v>34.466666666666669</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34.666666666666657</c:v>
+                  <c:v>31.333333333333336</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31.199999999999989</c:v>
+                  <c:v>28.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27.73333333333332</c:v>
+                  <c:v>25.06666666666667</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>24.266666666666652</c:v>
+                  <c:v>21.933333333333337</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20.799999999999983</c:v>
+                  <c:v>18.800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>17.333333333333314</c:v>
+                  <c:v>15.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13.866666666666648</c:v>
+                  <c:v>12.533333333333339</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10.399999999999981</c:v>
+                  <c:v>9.4000000000000057</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.933333333333314</c:v>
+                  <c:v>6.2666666666666728</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.4666666666666472</c:v>
+                  <c:v>3.1333333333333395</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-1.9539925233402755E-14</c:v>
+                  <c:v>6.2172489379008766E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="101686656"/>
-        <c:axId val="101705216"/>
+        <c:axId val="105667968"/>
+        <c:axId val="105682432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101686656"/>
+        <c:axId val="105667968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3433,7 +3433,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101705216"/>
+        <c:crossAx val="105682432"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3441,7 +3441,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101705216"/>
+        <c:axId val="105682432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3483,7 +3483,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101686656"/>
+        <c:crossAx val="105667968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3571,7 +3571,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000272" footer="0.49212598450000272"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000278" footer="0.49212598450000278"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3608,7 +3608,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225597"/>
+          <c:x val="0.37032576667225608"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3626,9 +3626,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532573"/>
+          <c:y val="0.15742128935532579"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192625"/>
+          <c:h val="0.70464767616192636"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3938,11 +3938,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="101746560"/>
-        <c:axId val="101756928"/>
+        <c:axId val="105863040"/>
+        <c:axId val="105873408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101746560"/>
+        <c:axId val="105863040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3974,7 +3974,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101756928"/>
+        <c:crossAx val="105873408"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3982,7 +3982,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101756928"/>
+        <c:axId val="105873408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4024,7 +4024,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101746560"/>
+        <c:crossAx val="105863040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4112,7 +4112,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000283" footer="0.49212598450000283"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000289" footer="0.49212598450000289"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -4198,13 +4198,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>112059</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>65444</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>11204</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>62002</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5442,7 +5442,7 @@
         <v>1</v>
       </c>
       <c r="D37" s="70" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E37" s="70"/>
       <c r="F37" s="72" t="s">
@@ -8469,7 +8469,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:DP85"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
@@ -11130,10 +11132,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DP81"/>
+  <dimension ref="A1:DP80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -11375,10 +11377,18 @@
       <c r="J4" s="72">
         <v>0</v>
       </c>
-      <c r="K4" s="95"/>
-      <c r="L4" s="95"/>
-      <c r="M4" s="95"/>
-      <c r="N4" s="95"/>
+      <c r="K4" s="72">
+        <v>0</v>
+      </c>
+      <c r="L4" s="72">
+        <v>0</v>
+      </c>
+      <c r="M4" s="72">
+        <v>0</v>
+      </c>
+      <c r="N4" s="72">
+        <v>0</v>
+      </c>
       <c r="O4" s="95"/>
       <c r="P4" s="95"/>
       <c r="Q4" s="95"/>
@@ -11413,10 +11423,18 @@
       <c r="J5" s="72">
         <v>0</v>
       </c>
-      <c r="K5" s="95"/>
-      <c r="L5" s="95"/>
-      <c r="M5" s="95"/>
-      <c r="N5" s="95"/>
+      <c r="K5" s="72">
+        <v>0</v>
+      </c>
+      <c r="L5" s="72">
+        <v>0</v>
+      </c>
+      <c r="M5" s="72">
+        <v>0</v>
+      </c>
+      <c r="N5" s="72">
+        <v>0</v>
+      </c>
       <c r="O5" s="95"/>
       <c r="P5" s="95"/>
       <c r="Q5" s="95"/>
@@ -11439,7 +11457,7 @@
       <c r="F6" s="72">
         <v>3</v>
       </c>
-      <c r="G6" s="145">
+      <c r="G6" s="147">
         <v>3</v>
       </c>
       <c r="H6" s="145">
@@ -11448,565 +11466,587 @@
       <c r="I6" s="145">
         <v>2</v>
       </c>
-      <c r="J6" s="72">
+      <c r="J6" s="145">
         <v>1</v>
       </c>
-      <c r="K6" s="95"/>
-      <c r="L6" s="95"/>
-      <c r="M6" s="95"/>
-      <c r="N6" s="95"/>
+      <c r="K6" s="145">
+        <v>1</v>
+      </c>
+      <c r="L6" s="145">
+        <v>1</v>
+      </c>
+      <c r="M6" s="145">
+        <v>1</v>
+      </c>
+      <c r="N6" s="145">
+        <v>1</v>
+      </c>
       <c r="O6" s="95"/>
       <c r="P6" s="95"/>
       <c r="Q6" s="95"/>
       <c r="R6" s="48"/>
     </row>
     <row r="7" spans="1:120" ht="24.95" customHeight="1">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="89" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="75"/>
+      <c r="C7" s="91"/>
+      <c r="D7" s="91"/>
+      <c r="E7" s="91"/>
+      <c r="F7" s="91"/>
+      <c r="G7" s="91"/>
+      <c r="H7" s="91"/>
+      <c r="I7" s="91"/>
+      <c r="J7" s="91"/>
+      <c r="K7" s="91"/>
+      <c r="L7" s="91"/>
+      <c r="M7" s="91"/>
+      <c r="N7" s="91"/>
+      <c r="O7" s="93"/>
+      <c r="P7" s="93"/>
+      <c r="Q7" s="93"/>
+      <c r="R7" s="48"/>
+    </row>
+    <row r="8" spans="1:120" ht="24.95" customHeight="1">
+      <c r="A8" s="70" t="s">
         <v>111</v>
       </c>
-      <c r="B7" s="75"/>
-      <c r="C7" s="72">
-        <v>5</v>
-      </c>
-      <c r="D7" s="72">
-        <v>5</v>
-      </c>
-      <c r="E7" s="72">
-        <v>5</v>
-      </c>
-      <c r="F7" s="72">
-        <v>5</v>
-      </c>
-      <c r="G7" s="72">
-        <v>5</v>
-      </c>
-      <c r="H7" s="72">
-        <v>5</v>
-      </c>
-      <c r="I7" s="72">
-        <v>5</v>
-      </c>
-      <c r="J7" s="72">
-        <v>5</v>
-      </c>
-      <c r="K7" s="95"/>
-      <c r="L7" s="95"/>
-      <c r="M7" s="95"/>
-      <c r="N7" s="95"/>
-      <c r="O7" s="95"/>
-      <c r="P7" s="95"/>
-      <c r="Q7" s="95"/>
-      <c r="R7" s="48"/>
-    </row>
-    <row r="8" spans="1:120" ht="24.95" customHeight="1">
-      <c r="A8" s="89" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="75"/>
-      <c r="C8" s="91"/>
-      <c r="D8" s="91"/>
-      <c r="E8" s="91"/>
-      <c r="F8" s="91"/>
-      <c r="G8" s="91"/>
-      <c r="H8" s="91"/>
-      <c r="I8" s="91"/>
-      <c r="J8" s="91"/>
-      <c r="K8" s="93"/>
-      <c r="L8" s="93"/>
-      <c r="M8" s="93"/>
-      <c r="N8" s="93"/>
-      <c r="O8" s="93"/>
-      <c r="P8" s="93"/>
-      <c r="Q8" s="93"/>
+      <c r="B8" s="75">
+        <v>23</v>
+      </c>
+      <c r="C8" s="145">
+        <v>8</v>
+      </c>
+      <c r="D8" s="145">
+        <v>3</v>
+      </c>
+      <c r="E8" s="145">
+        <v>1</v>
+      </c>
+      <c r="F8" s="145">
+        <v>1</v>
+      </c>
+      <c r="G8" s="147">
+        <v>0</v>
+      </c>
+      <c r="H8" s="147">
+        <v>0</v>
+      </c>
+      <c r="I8" s="147">
+        <v>0</v>
+      </c>
+      <c r="J8" s="147">
+        <v>0</v>
+      </c>
+      <c r="K8" s="147">
+        <v>0</v>
+      </c>
+      <c r="L8" s="147">
+        <v>0</v>
+      </c>
+      <c r="M8" s="147">
+        <v>0</v>
+      </c>
+      <c r="N8" s="147">
+        <v>0</v>
+      </c>
+      <c r="O8" s="95"/>
+      <c r="P8" s="95"/>
+      <c r="Q8" s="95"/>
       <c r="R8" s="48"/>
     </row>
     <row r="9" spans="1:120" ht="24.95" customHeight="1">
-      <c r="A9" s="70" t="s">
-        <v>112</v>
-      </c>
-      <c r="B9" s="75">
-        <v>23</v>
-      </c>
-      <c r="C9" s="145">
-        <v>8</v>
-      </c>
-      <c r="D9" s="145">
-        <v>3</v>
-      </c>
-      <c r="E9" s="147">
-        <v>1</v>
-      </c>
-      <c r="F9" s="147">
-        <v>1</v>
-      </c>
-      <c r="G9" s="147">
-        <v>1</v>
-      </c>
-      <c r="H9" s="147">
-        <v>1</v>
-      </c>
-      <c r="I9" s="147">
-        <v>1</v>
-      </c>
-      <c r="J9" s="147">
-        <v>1</v>
-      </c>
-      <c r="K9" s="95"/>
-      <c r="L9" s="95"/>
-      <c r="M9" s="95"/>
-      <c r="N9" s="95"/>
+      <c r="A9" s="89" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="75"/>
+      <c r="C9" s="91"/>
+      <c r="D9" s="91"/>
+      <c r="E9" s="91"/>
+      <c r="F9" s="91"/>
+      <c r="G9" s="91"/>
+      <c r="H9" s="91"/>
+      <c r="I9" s="91"/>
+      <c r="J9" s="91"/>
+      <c r="K9" s="91"/>
+      <c r="L9" s="91"/>
+      <c r="M9" s="91"/>
+      <c r="N9" s="91"/>
       <c r="O9" s="95"/>
       <c r="P9" s="95"/>
       <c r="Q9" s="95"/>
       <c r="R9" s="48"/>
     </row>
-    <row r="10" spans="1:120" ht="24.95" customHeight="1">
-      <c r="A10" s="89" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="75"/>
-      <c r="C10" s="91"/>
-      <c r="D10" s="91"/>
-      <c r="E10" s="91"/>
-      <c r="F10" s="91"/>
-      <c r="G10" s="91"/>
-      <c r="H10" s="91"/>
-      <c r="I10" s="91"/>
-      <c r="J10" s="91"/>
-      <c r="K10" s="95"/>
-      <c r="L10" s="95"/>
-      <c r="M10" s="95"/>
-      <c r="N10" s="95"/>
+    <row r="10" spans="1:120" s="161" customFormat="1" ht="24.95" customHeight="1">
+      <c r="A10" s="151" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="147"/>
+      <c r="C10" s="147">
+        <v>4</v>
+      </c>
+      <c r="D10" s="147">
+        <v>4</v>
+      </c>
+      <c r="E10" s="147">
+        <v>4</v>
+      </c>
+      <c r="F10" s="147">
+        <v>4</v>
+      </c>
+      <c r="G10" s="147">
+        <v>4</v>
+      </c>
+      <c r="H10" s="145">
+        <v>4</v>
+      </c>
+      <c r="I10" s="145">
+        <v>3</v>
+      </c>
+      <c r="J10" s="145">
+        <v>2</v>
+      </c>
+      <c r="K10" s="145">
+        <v>2</v>
+      </c>
+      <c r="L10" s="145">
+        <v>1</v>
+      </c>
+      <c r="M10" s="147">
+        <v>0</v>
+      </c>
+      <c r="N10" s="147">
+        <v>0</v>
+      </c>
       <c r="O10" s="95"/>
       <c r="P10" s="95"/>
       <c r="Q10" s="95"/>
-      <c r="R10" s="48"/>
-    </row>
-    <row r="11" spans="1:120" s="161" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A11" s="151" t="s">
+      <c r="R10" s="95"/>
+    </row>
+    <row r="11" spans="1:120" ht="24.95" customHeight="1">
+      <c r="A11" s="70" t="s">
         <v>114</v>
       </c>
-      <c r="B11" s="147"/>
-      <c r="C11" s="147">
-        <v>4</v>
-      </c>
-      <c r="D11" s="147">
-        <v>4</v>
-      </c>
-      <c r="E11" s="147">
-        <v>4</v>
-      </c>
-      <c r="F11" s="147">
-        <v>4</v>
-      </c>
-      <c r="G11" s="147">
-        <v>4</v>
+      <c r="B11" s="75">
+        <v>27</v>
+      </c>
+      <c r="C11" s="72">
+        <v>20</v>
+      </c>
+      <c r="D11" s="72">
+        <v>20</v>
+      </c>
+      <c r="E11" s="72">
+        <v>20</v>
+      </c>
+      <c r="F11" s="72">
+        <v>20</v>
+      </c>
+      <c r="G11" s="145">
+        <v>20</v>
       </c>
       <c r="H11" s="145">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="I11" s="145">
+        <v>13</v>
+      </c>
+      <c r="J11" s="145">
+        <v>11</v>
+      </c>
+      <c r="K11" s="145">
+        <v>9</v>
+      </c>
+      <c r="L11" s="145">
+        <v>5</v>
+      </c>
+      <c r="M11" s="145">
         <v>3</v>
       </c>
-      <c r="J11" s="145">
-        <v>2</v>
-      </c>
-      <c r="K11" s="95"/>
-      <c r="L11" s="95"/>
-      <c r="M11" s="95"/>
-      <c r="N11" s="95"/>
-      <c r="O11" s="95"/>
-      <c r="P11" s="95"/>
-      <c r="Q11" s="95"/>
-      <c r="R11" s="95"/>
+      <c r="N11" s="147">
+        <v>1</v>
+      </c>
+      <c r="O11" s="92"/>
+      <c r="P11" s="92"/>
+      <c r="Q11" s="92"/>
+      <c r="R11" s="49"/>
     </row>
     <row r="12" spans="1:120" ht="24.95" customHeight="1">
-      <c r="A12" s="70" t="s">
-        <v>103</v>
-      </c>
-      <c r="B12" s="75">
-        <v>27</v>
-      </c>
-      <c r="C12" s="72">
-        <v>20</v>
-      </c>
-      <c r="D12" s="72">
-        <v>20</v>
-      </c>
-      <c r="E12" s="72">
-        <v>20</v>
-      </c>
-      <c r="F12" s="72">
-        <v>20</v>
-      </c>
-      <c r="G12" s="145">
-        <v>20</v>
-      </c>
-      <c r="H12" s="145">
-        <v>16</v>
-      </c>
-      <c r="I12" s="145">
-        <v>13</v>
-      </c>
-      <c r="J12" s="145">
-        <v>11</v>
-      </c>
-      <c r="K12" s="92"/>
-      <c r="L12" s="92"/>
-      <c r="M12" s="92"/>
-      <c r="N12" s="92"/>
-      <c r="O12" s="92"/>
-      <c r="P12" s="92"/>
-      <c r="Q12" s="92"/>
+      <c r="A12" s="89" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="75"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="91"/>
+      <c r="E12" s="91"/>
+      <c r="F12" s="91"/>
+      <c r="G12" s="91"/>
+      <c r="H12" s="91"/>
+      <c r="I12" s="91"/>
+      <c r="J12" s="91"/>
+      <c r="K12" s="91"/>
+      <c r="L12" s="91"/>
+      <c r="M12" s="91"/>
+      <c r="N12" s="91"/>
+      <c r="O12" s="94"/>
+      <c r="P12" s="94"/>
+      <c r="Q12" s="94"/>
       <c r="R12" s="49"/>
     </row>
     <row r="13" spans="1:120" ht="24.95" customHeight="1">
-      <c r="A13" s="89" t="s">
-        <v>65</v>
-      </c>
-      <c r="B13" s="75"/>
-      <c r="C13" s="91"/>
-      <c r="D13" s="91"/>
-      <c r="E13" s="91"/>
-      <c r="F13" s="91"/>
-      <c r="G13" s="91"/>
-      <c r="H13" s="91"/>
-      <c r="I13" s="91"/>
-      <c r="J13" s="91"/>
-      <c r="K13" s="94"/>
-      <c r="L13" s="94"/>
-      <c r="M13" s="94"/>
-      <c r="N13" s="94"/>
+      <c r="A13" s="82" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="75">
+        <v>30</v>
+      </c>
+      <c r="C13" s="72">
+        <v>10</v>
+      </c>
+      <c r="D13" s="72">
+        <v>10</v>
+      </c>
+      <c r="E13" s="72">
+        <v>10</v>
+      </c>
+      <c r="F13" s="72">
+        <v>10</v>
+      </c>
+      <c r="G13" s="72">
+        <v>10</v>
+      </c>
+      <c r="H13" s="72">
+        <v>10</v>
+      </c>
+      <c r="I13" s="72">
+        <v>10</v>
+      </c>
+      <c r="J13" s="72">
+        <v>10</v>
+      </c>
+      <c r="K13" s="72">
+        <v>10</v>
+      </c>
+      <c r="L13" s="72">
+        <v>10</v>
+      </c>
+      <c r="M13" s="72">
+        <v>10</v>
+      </c>
+      <c r="N13" s="72">
+        <v>10</v>
+      </c>
       <c r="O13" s="94"/>
       <c r="P13" s="94"/>
       <c r="Q13" s="94"/>
       <c r="R13" s="49"/>
     </row>
-    <row r="14" spans="1:120" ht="24.95" customHeight="1">
-      <c r="A14" s="82" t="s">
-        <v>104</v>
-      </c>
-      <c r="B14" s="75">
-        <v>30</v>
-      </c>
-      <c r="C14" s="72">
-        <v>10</v>
-      </c>
-      <c r="D14" s="72">
-        <v>10</v>
-      </c>
-      <c r="E14" s="72">
-        <v>10</v>
-      </c>
-      <c r="F14" s="72">
-        <v>10</v>
-      </c>
-      <c r="G14" s="72">
-        <v>10</v>
-      </c>
-      <c r="H14" s="72">
-        <v>10</v>
-      </c>
-      <c r="I14" s="72">
-        <v>10</v>
-      </c>
-      <c r="J14" s="72">
-        <v>10</v>
-      </c>
-      <c r="K14" s="94"/>
-      <c r="L14" s="94"/>
-      <c r="M14" s="94"/>
-      <c r="N14" s="94"/>
-      <c r="O14" s="94"/>
-      <c r="P14" s="94"/>
-      <c r="Q14" s="94"/>
-      <c r="R14" s="49"/>
-    </row>
-    <row r="15" spans="1:120">
-      <c r="A15" s="38"/>
-    </row>
-    <row r="16" spans="1:120" s="56" customFormat="1">
-      <c r="A16" s="55"/>
+    <row r="14" spans="1:120">
+      <c r="A14" s="38"/>
+    </row>
+    <row r="15" spans="1:120" s="56" customFormat="1">
+      <c r="A15" s="55"/>
+      <c r="B15" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="38">
+        <f>IF(ISBLANK(C3:C13), NA(), SUM(C3:C13))</f>
+        <v>47</v>
+      </c>
+      <c r="D15" s="38">
+        <f t="shared" ref="D15:R15" si="0">IF(ISBLANK(D3:D13), NA(), SUM(D3:D13))</f>
+        <v>42</v>
+      </c>
+      <c r="E15" s="38">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="F15" s="38">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="G15" s="38">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="H15" s="38">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="I15" s="38">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="J15" s="38">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="K15" s="38">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="L15" s="38">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="M15" s="38">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="N15" s="38">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="O15" s="38" t="e">
+        <f t="array" ref="O15">IF(ISBLANK(O3:O13), NA(), SUM(O3:O13))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P15" s="38" t="e">
+        <f t="array" ref="P15">IF(ISBLANK(P3:P13), NA(), SUM(P3:P13))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q15" s="38" t="e">
+        <f t="array" ref="Q15">IF(ISBLANK(Q3:Q13), NA(), SUM(Q3:Q13))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R15" s="38" t="e">
+        <f t="array" ref="R15">IF(ISBLANK(R3:R13), NA(), SUM(R3:R13))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="16" spans="1:120" ht="25.5">
+      <c r="A16" s="38"/>
       <c r="B16" s="43" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="38">
-        <f>IF(ISBLANK(C4:C14), NA(), SUM(C3:C14))</f>
-        <v>52</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C16" s="38"/>
       <c r="D16" s="38">
-        <f t="shared" ref="D16:E16" si="0">IF(ISBLANK(D4:D14), NA(), SUM(D3:D14))</f>
-        <v>47</v>
+        <f t="shared" ref="D16:R16" si="1">C15-D15</f>
+        <v>5</v>
       </c>
       <c r="E16" s="38">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="F16" s="38">
-        <f t="array" ref="F16">IF(ISBLANK(F4:F14), NA(), SUM(F3:F14))</f>
-        <v>45</v>
-      </c>
-      <c r="G16" s="38">
-        <f t="array" ref="G16">IF(ISBLANK(G4:G14), NA(), SUM(G3:G14))</f>
-        <v>43</v>
-      </c>
-      <c r="H16" s="38">
-        <f t="array" ref="H16">IF(ISBLANK(H4:H14), NA(), SUM(H3:H14))</f>
-        <v>39</v>
-      </c>
-      <c r="I16" s="38">
-        <f t="array" ref="I16">IF(ISBLANK(I4:I14), NA(), SUM(I3:I14))</f>
-        <v>34</v>
-      </c>
-      <c r="J16" s="38">
-        <f t="array" ref="J16">IF(ISBLANK(J4:J14), NA(), SUM(J3:J14))</f>
-        <v>30</v>
-      </c>
-      <c r="K16" s="38" t="e">
-        <f t="array" ref="K16">IF(ISBLANK(K4:K14), NA(), SUM(K3:K14))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L16" s="38" t="e">
-        <f t="array" ref="L16">IF(ISBLANK(L4:L14), NA(), SUM(L3:L14))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M16" s="38" t="e">
-        <f t="array" ref="M16">IF(ISBLANK(M4:M14), NA(), SUM(M3:M14))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N16" s="38" t="e">
-        <f t="array" ref="N16">IF(ISBLANK(N4:N14), NA(), SUM(N3:N14))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O16" s="38" t="e">
-        <f t="array" ref="O16">IF(ISBLANK(O4:O14), NA(), SUM(O3:O14))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P16" s="38" t="e">
-        <f t="array" ref="P16">IF(ISBLANK(P4:P14), NA(), SUM(P3:P14))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q16" s="38" t="e">
-        <f t="array" ref="Q16">IF(ISBLANK(Q4:Q14), NA(), SUM(Q3:Q14))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R16" s="38" t="e">
-        <f t="array" ref="R16">IF(ISBLANK(R4:R14), NA(), SUM(R3:R14))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="25.5">
-      <c r="A17" s="38"/>
-      <c r="B17" s="43" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38">
-        <f t="shared" ref="D17:R17" si="1">C16-D16</f>
-        <v>5</v>
-      </c>
-      <c r="E17" s="38">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F17" s="38">
+      <c r="F16" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G17" s="38">
+      <c r="G16" s="38">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="H16" s="38">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I16" s="38">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J16" s="38">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K16" s="38">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="H17" s="38">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="I17" s="38">
+      <c r="L16" s="38">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="J17" s="38">
+      <c r="M16" s="38">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="K17" s="38" t="e">
+        <v>3</v>
+      </c>
+      <c r="N16" s="38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="O16" s="38" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="L17" s="38" t="e">
+      <c r="P16" s="38" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="M17" s="38" t="e">
+      <c r="Q16" s="38" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="N17" s="38" t="e">
+      <c r="R16" s="51" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="O17" s="38" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="P17" s="38" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="Q17" s="38" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R17" s="51" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" s="38"/>
+      <c r="B17" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="45">
+        <f>C15</f>
+        <v>47</v>
+      </c>
+      <c r="D17" s="46">
+        <f>C17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <v>43.866666666666667</v>
+      </c>
+      <c r="E17" s="46">
+        <f>D17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <v>40.733333333333334</v>
+      </c>
+      <c r="F17" s="46">
+        <f>E17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <v>37.6</v>
+      </c>
+      <c r="G17" s="46">
+        <f>F17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <v>34.466666666666669</v>
+      </c>
+      <c r="H17" s="46">
+        <f>G17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <v>31.333333333333336</v>
+      </c>
+      <c r="I17" s="46">
+        <f>H17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <v>28.200000000000003</v>
+      </c>
+      <c r="J17" s="46">
+        <f>I17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <v>25.06666666666667</v>
+      </c>
+      <c r="K17" s="46">
+        <f>J17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <v>21.933333333333337</v>
+      </c>
+      <c r="L17" s="46">
+        <f>K17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <v>18.800000000000004</v>
+      </c>
+      <c r="M17" s="46">
+        <f>L17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <v>15.666666666666671</v>
+      </c>
+      <c r="N17" s="46">
+        <f>M17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <v>12.533333333333339</v>
+      </c>
+      <c r="O17" s="46">
+        <f>N17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <v>9.4000000000000057</v>
+      </c>
+      <c r="P17" s="46">
+        <f>O17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <v>6.2666666666666728</v>
+      </c>
+      <c r="Q17" s="46">
+        <f>P17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <v>3.1333333333333395</v>
+      </c>
+      <c r="R17" s="52">
+        <f>Q17-$C$15/COUNTA($C$2:$Q$2)</f>
+        <v>6.2172489379008766E-15</v>
       </c>
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="38"/>
-      <c r="B18" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="45">
-        <f>C16</f>
-        <v>52</v>
-      </c>
-      <c r="D18" s="46">
-        <f t="shared" ref="D18:R18" si="2">C18-$C$16/COUNTA($C$2:$Q$2)</f>
-        <v>48.533333333333331</v>
-      </c>
-      <c r="E18" s="46">
+      <c r="B18" s="57" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="58">
+        <f t="shared" ref="C18:R18" si="2">1-C15/$C$15</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="58">
         <f t="shared" si="2"/>
-        <v>45.066666666666663</v>
-      </c>
-      <c r="F18" s="46">
+        <v>0.1063829787234043</v>
+      </c>
+      <c r="E18" s="58">
         <f t="shared" si="2"/>
-        <v>41.599999999999994</v>
-      </c>
-      <c r="G18" s="46">
+        <v>0.14893617021276595</v>
+      </c>
+      <c r="F18" s="58">
         <f t="shared" si="2"/>
-        <v>38.133333333333326</v>
-      </c>
-      <c r="H18" s="46">
+        <v>0.14893617021276595</v>
+      </c>
+      <c r="G18" s="58">
         <f t="shared" si="2"/>
-        <v>34.666666666666657</v>
-      </c>
-      <c r="I18" s="46">
+        <v>0.21276595744680848</v>
+      </c>
+      <c r="H18" s="58">
         <f t="shared" si="2"/>
-        <v>31.199999999999989</v>
-      </c>
-      <c r="J18" s="46">
+        <v>0.2978723404255319</v>
+      </c>
+      <c r="I18" s="58">
         <f t="shared" si="2"/>
-        <v>27.73333333333332</v>
-      </c>
-      <c r="K18" s="46">
+        <v>0.4042553191489362</v>
+      </c>
+      <c r="J18" s="58">
         <f t="shared" si="2"/>
-        <v>24.266666666666652</v>
-      </c>
-      <c r="L18" s="46">
+        <v>0.48936170212765961</v>
+      </c>
+      <c r="K18" s="58">
         <f t="shared" si="2"/>
-        <v>20.799999999999983</v>
-      </c>
-      <c r="M18" s="46">
+        <v>0.53191489361702127</v>
+      </c>
+      <c r="L18" s="58">
         <f t="shared" si="2"/>
-        <v>17.333333333333314</v>
-      </c>
-      <c r="N18" s="46">
+        <v>0.63829787234042556</v>
+      </c>
+      <c r="M18" s="58">
         <f t="shared" si="2"/>
-        <v>13.866666666666648</v>
-      </c>
-      <c r="O18" s="46">
+        <v>0.7021276595744681</v>
+      </c>
+      <c r="N18" s="58">
         <f t="shared" si="2"/>
-        <v>10.399999999999981</v>
-      </c>
-      <c r="P18" s="46">
+        <v>0.74468085106382986</v>
+      </c>
+      <c r="O18" s="58" t="e">
         <f t="shared" si="2"/>
-        <v>6.933333333333314</v>
-      </c>
-      <c r="Q18" s="46">
+        <v>#N/A</v>
+      </c>
+      <c r="P18" s="58" t="e">
         <f t="shared" si="2"/>
-        <v>3.4666666666666472</v>
-      </c>
-      <c r="R18" s="52">
+        <v>#N/A</v>
+      </c>
+      <c r="Q18" s="58" t="e">
         <f t="shared" si="2"/>
-        <v>-1.9539925233402755E-14</v>
+        <v>#N/A</v>
+      </c>
+      <c r="R18" s="58" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="38"/>
-      <c r="B19" s="57" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="58">
-        <f t="shared" ref="C19:R19" si="3">1-C16/$C$16</f>
-        <v>0</v>
-      </c>
-      <c r="D19" s="58">
-        <f t="shared" si="3"/>
-        <v>9.6153846153846145E-2</v>
-      </c>
-      <c r="E19" s="58">
-        <f t="shared" si="3"/>
-        <v>0.13461538461538458</v>
-      </c>
-      <c r="F19" s="58">
-        <f t="shared" si="3"/>
-        <v>0.13461538461538458</v>
-      </c>
-      <c r="G19" s="58">
-        <f t="shared" si="3"/>
-        <v>0.17307692307692313</v>
-      </c>
-      <c r="H19" s="58">
-        <f t="shared" si="3"/>
-        <v>0.25</v>
-      </c>
-      <c r="I19" s="58">
-        <f t="shared" si="3"/>
-        <v>0.34615384615384615</v>
-      </c>
-      <c r="J19" s="58">
-        <f t="shared" si="3"/>
-        <v>0.42307692307692313</v>
-      </c>
-      <c r="K19" s="58" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-      <c r="L19" s="58" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M19" s="58" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-      <c r="N19" s="58" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-      <c r="O19" s="58" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-      <c r="P19" s="58" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-      <c r="Q19" s="58" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R19" s="58" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="38"/>
     </row>
     <row r="21" spans="1:18">
       <c r="A21" s="38"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="38"/>
+      <c r="O21" s="38"/>
+      <c r="P21" s="38"/>
+      <c r="Q21" s="38"/>
+      <c r="R21" s="38"/>
     </row>
     <row r="22" spans="1:18">
       <c r="A22" s="38"/>
@@ -13188,40 +13228,20 @@
       <c r="Q80" s="38"/>
       <c r="R80" s="38"/>
     </row>
-    <row r="81" spans="1:18">
-      <c r="A81" s="38"/>
-      <c r="B81" s="38"/>
-      <c r="C81" s="38"/>
-      <c r="D81" s="38"/>
-      <c r="E81" s="38"/>
-      <c r="F81" s="38"/>
-      <c r="G81" s="38"/>
-      <c r="H81" s="38"/>
-      <c r="I81" s="38"/>
-      <c r="J81" s="38"/>
-      <c r="K81" s="38"/>
-      <c r="L81" s="38"/>
-      <c r="M81" s="38"/>
-      <c r="N81" s="38"/>
-      <c r="O81" s="38"/>
-      <c r="P81" s="38"/>
-      <c r="Q81" s="38"/>
-      <c r="R81" s="38"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B9:B11 A3:A14 B13:B14 B3:B7 G3:I3 I3:I10 J3:R14 I12:J14">
-    <cfRule type="expression" dxfId="17" priority="31" stopIfTrue="1">
+  <conditionalFormatting sqref="I11:J13 A3:B13 G3:I3 J9:N13 O3:R13 I3:N7 I9">
+    <cfRule type="expression" dxfId="3" priority="31" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="32" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B14 A13 A9:A11">
-    <cfRule type="expression" dxfId="15" priority="3" stopIfTrue="1">
+  <conditionalFormatting sqref="A12 A8:A10">
+    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15341,50 +15361,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:B6 D3:R6">
-    <cfRule type="expression" dxfId="13" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="25" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="26" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B6 A4:B6">
-    <cfRule type="expression" dxfId="11" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="23" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="24" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="expression" dxfId="9" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="21" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="22" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B5">
-    <cfRule type="expression" dxfId="7" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="5" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="6" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A7">
-    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B5">
-    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="1" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
maj fiche consulter artefact
</commit_message>
<xml_diff>
--- a/doc/Backlog [ACONIT].xlsx
+++ b/doc/Backlog [ACONIT].xlsx
@@ -39,10 +39,10 @@
   </definedNames>
   <calcPr calcId="125725"/>
   <customWorkbookViews>
+    <customWorkbookView name="Bernard Notarianni - Affichage personnalisé" guid="{178C21D0-B00A-4B0E-B009-71AAC80909BC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="785" activeSheetId="1"/>
+    <customWorkbookView name="Didier Lassissi - Affichage personnalisé" guid="{5E22A59B-ECE7-4B50-9619-81A99F53295A}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1064" windowHeight="552" activeSheetId="1"/>
+    <customWorkbookView name="uvba7442 - Affichage personnalisé" guid="{38566435-C99E-4958-9169-0C5C493EE97D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1213" windowHeight="665" activeSheetId="1"/>
     <customWorkbookView name="Yoann Regardin - Affichage personnalisé" guid="{29B12ED2-AD48-4E1C-B971-77E4D76C1B5F}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="609" activeSheetId="2"/>
-    <customWorkbookView name="uvba7442 - Affichage personnalisé" guid="{38566435-C99E-4958-9169-0C5C493EE97D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1213" windowHeight="665" activeSheetId="1"/>
-    <customWorkbookView name="Didier Lassissi - Affichage personnalisé" guid="{5E22A59B-ECE7-4B50-9619-81A99F53295A}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1064" windowHeight="552" activeSheetId="1"/>
-    <customWorkbookView name="Bernard Notarianni - Affichage personnalisé" guid="{178C21D0-B00A-4B0E-B009-71AAC80909BC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="785" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
@@ -1688,21 +1688,7 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vérification" xfId="42" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="51"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="22">
     <dxf>
       <fill>
         <patternFill>
@@ -1965,7 +1951,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225542"/>
+          <c:x val="0.37032576667225553"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -1983,9 +1969,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532546"/>
+          <c:y val="0.15742128935532551"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192581"/>
+          <c:h val="0.70464767616192592"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2295,11 +2281,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="103467264"/>
-        <c:axId val="103821696"/>
+        <c:axId val="113244416"/>
+        <c:axId val="113590656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103467264"/>
+        <c:axId val="113244416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2331,7 +2317,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="103821696"/>
+        <c:crossAx val="113590656"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2339,7 +2325,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103821696"/>
+        <c:axId val="113590656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2381,7 +2367,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="103467264"/>
+        <c:crossAx val="113244416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2469,7 +2455,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000261" footer="0.49212598450000261"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000267" footer="0.49212598450000267"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2506,7 +2492,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.3703257666722557"/>
+          <c:x val="0.37032576667225586"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2524,9 +2510,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532557"/>
+          <c:y val="0.15742128935532565"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192603"/>
+          <c:h val="0.70464767616192614"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2836,11 +2822,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="104178816"/>
-        <c:axId val="104180736"/>
+        <c:axId val="113939584"/>
+        <c:axId val="113941504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="104178816"/>
+        <c:axId val="113939584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2872,7 +2858,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="104180736"/>
+        <c:crossAx val="113941504"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2880,7 +2866,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104180736"/>
+        <c:axId val="113941504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2922,7 +2908,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="104178816"/>
+        <c:crossAx val="113939584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3010,7 +2996,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000272" footer="0.49212598450000272"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000278" footer="0.49212598450000278"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3047,7 +3033,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225597"/>
+          <c:x val="0.37032576667225608"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3065,9 +3051,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532573"/>
+          <c:y val="0.15742128935532579"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192625"/>
+          <c:h val="0.70464767616192636"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3377,11 +3363,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="104226176"/>
-        <c:axId val="104244736"/>
+        <c:axId val="113991040"/>
+        <c:axId val="114005504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="104226176"/>
+        <c:axId val="113991040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3413,7 +3399,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="104244736"/>
+        <c:crossAx val="114005504"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3421,7 +3407,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104244736"/>
+        <c:axId val="114005504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3463,7 +3449,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="104226176"/>
+        <c:crossAx val="113991040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3551,7 +3537,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000283" footer="0.49212598450000283"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000289" footer="0.49212598450000289"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3588,7 +3574,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.3703257666722562"/>
+          <c:x val="0.37032576667225636"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3606,9 +3592,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532584"/>
+          <c:y val="0.1574212893553259"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192658"/>
+          <c:h val="0.70464767616192681"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3918,11 +3904,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="104298368"/>
-        <c:axId val="104308736"/>
+        <c:axId val="114063232"/>
+        <c:axId val="114073600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="104298368"/>
+        <c:axId val="114063232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3954,7 +3940,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="104308736"/>
+        <c:crossAx val="114073600"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3962,7 +3948,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104308736"/>
+        <c:axId val="114073600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4004,7 +3990,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="104298368"/>
+        <c:crossAx val="114063232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4092,7 +4078,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000294" footer="0.49212598450000294"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.492125984500003" footer="0.492125984500003"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -5869,10 +5855,10 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A50:A51 B45:C45 D46:E47 H45:K45 A43:A46 B37:E37 D15 D38:E38 B36:C37 H36:K37 E36:E37 A35:A40 D26 B28:C31 A13:A22 H28:K31 D20:E21 E25:E26 A25:A31 D28 E28:E31 B12:E12 D13:E13 B13:C17 H12:K17 E13:E15 E17:E19 D30:D31">
-    <cfRule type="expression" dxfId="3" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="53" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="54" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8406,18 +8392,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11 A3:B11 F3:G7 H3:R11">
-    <cfRule type="expression" dxfId="23" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="53" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="54" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B10 A3:A7 A11:B11">
-    <cfRule type="expression" dxfId="21" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="31" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="32" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11079,10 +11065,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B13:B15 E13:G13 D14:R15 B3:B11 A3:A15 C6:D8 G9:M15 D3:R12 N4:R15">
-    <cfRule type="expression" dxfId="19" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="37" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="38" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11704,51 +11690,51 @@
         <v>37</v>
       </c>
       <c r="C14" s="38">
-        <f>IF(ISBLANK(C3:C12), NA(), SUM(C3:C12))</f>
+        <f t="shared" ref="C14:N14" si="0">IF(ISBLANK(C3:C12), NA(), SUM(C3:C12))</f>
         <v>47</v>
       </c>
       <c r="D14" s="38">
-        <f>IF(ISBLANK(D3:D12), NA(), SUM(D3:D12))</f>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="E14" s="38">
-        <f>IF(ISBLANK(E3:E12), NA(), SUM(E3:E12))</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="F14" s="38">
-        <f>IF(ISBLANK(F3:F12), NA(), SUM(F3:F12))</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="G14" s="38">
-        <f>IF(ISBLANK(G3:G12), NA(), SUM(G3:G12))</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="H14" s="38">
-        <f>IF(ISBLANK(H3:H12), NA(), SUM(H3:H12))</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="I14" s="38">
-        <f>IF(ISBLANK(I3:I12), NA(), SUM(I3:I12))</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="J14" s="38">
-        <f>IF(ISBLANK(J3:J12), NA(), SUM(J3:J12))</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="K14" s="38">
-        <f>IF(ISBLANK(K3:K12), NA(), SUM(K3:K12))</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="L14" s="38">
-        <f>IF(ISBLANK(L3:L12), NA(), SUM(L3:L12))</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="M14" s="38">
-        <f>IF(ISBLANK(M3:M12), NA(), SUM(M3:M12))</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="N14" s="38">
-        <f>IF(ISBLANK(N3:N12), NA(), SUM(N3:N12))</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="O14" s="38" t="e">
@@ -11775,63 +11761,63 @@
       </c>
       <c r="C15" s="38"/>
       <c r="D15" s="38">
-        <f t="shared" ref="D15:R15" si="0">C14-D14</f>
+        <f t="shared" ref="D15:R15" si="1">C14-D14</f>
         <v>5</v>
       </c>
       <c r="E15" s="38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="F15" s="38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G15" s="38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="H15" s="38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="I15" s="38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="J15" s="38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="K15" s="38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="L15" s="38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="M15" s="38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="N15" s="38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="O15" s="38" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="P15" s="38" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="Q15" s="38" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="R15" s="51" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -11845,63 +11831,63 @@
         <v>47</v>
       </c>
       <c r="D16" s="46">
-        <f>C16-$C$14/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" ref="D16:R16" si="2">C16-$C$14/COUNTA($C$2:$Q$2)</f>
         <v>43.866666666666667</v>
       </c>
       <c r="E16" s="46">
-        <f>D16-$C$14/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>40.733333333333334</v>
       </c>
       <c r="F16" s="46">
-        <f>E16-$C$14/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>37.6</v>
       </c>
       <c r="G16" s="46">
-        <f>F16-$C$14/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>34.466666666666669</v>
       </c>
       <c r="H16" s="46">
-        <f>G16-$C$14/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>31.333333333333336</v>
       </c>
       <c r="I16" s="46">
-        <f>H16-$C$14/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>28.200000000000003</v>
       </c>
       <c r="J16" s="46">
-        <f>I16-$C$14/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>25.06666666666667</v>
       </c>
       <c r="K16" s="46">
-        <f>J16-$C$14/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>21.933333333333337</v>
       </c>
       <c r="L16" s="46">
-        <f>K16-$C$14/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>18.800000000000004</v>
       </c>
       <c r="M16" s="46">
-        <f>L16-$C$14/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>15.666666666666671</v>
       </c>
       <c r="N16" s="46">
-        <f>M16-$C$14/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>12.533333333333339</v>
       </c>
       <c r="O16" s="46">
-        <f>N16-$C$14/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>9.4000000000000057</v>
       </c>
       <c r="P16" s="46">
-        <f>O16-$C$14/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>6.2666666666666728</v>
       </c>
       <c r="Q16" s="46">
-        <f>P16-$C$14/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>3.1333333333333395</v>
       </c>
       <c r="R16" s="52">
-        <f>Q16-$C$14/COUNTA($C$2:$Q$2)</f>
+        <f t="shared" si="2"/>
         <v>6.2172489379008766E-15</v>
       </c>
     </row>
@@ -11911,67 +11897,67 @@
         <v>40</v>
       </c>
       <c r="C17" s="58">
-        <f t="shared" ref="C17:R17" si="1">1-C14/$C$14</f>
+        <f t="shared" ref="C17:R17" si="3">1-C14/$C$14</f>
         <v>0</v>
       </c>
       <c r="D17" s="58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.1063829787234043</v>
       </c>
       <c r="E17" s="58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.14893617021276595</v>
       </c>
       <c r="F17" s="58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.14893617021276595</v>
       </c>
       <c r="G17" s="58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.21276595744680848</v>
       </c>
       <c r="H17" s="58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.2978723404255319</v>
       </c>
       <c r="I17" s="58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.4042553191489362</v>
       </c>
       <c r="J17" s="58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.48936170212765961</v>
       </c>
       <c r="K17" s="58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.53191489361702127</v>
       </c>
       <c r="L17" s="58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.63829787234042556</v>
       </c>
       <c r="M17" s="58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.7021276595744681</v>
       </c>
       <c r="N17" s="58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.74468085106382986</v>
       </c>
       <c r="O17" s="58" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="P17" s="58" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="Q17" s="58" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="R17" s="58" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -13183,10 +13169,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I11:J12 G3:I3 J9:N12 I9 O3:R12 I3:O7 A3:B12">
-    <cfRule type="expression" dxfId="1" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="31" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="32" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15306,50 +15292,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:B6 D3:R6">
-    <cfRule type="expression" dxfId="17" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="25" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="26" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B6 A4:B6">
-    <cfRule type="expression" dxfId="15" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="23" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="24" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="expression" dxfId="13" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="21" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="22" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B5">
-    <cfRule type="expression" dxfId="11" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A7">
-    <cfRule type="expression" dxfId="9" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B5">
-    <cfRule type="expression" dxfId="7" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Affichage du formulaire d'ajout d'un utilisateur
</commit_message>
<xml_diff>
--- a/doc/Backlog [ACONIT].xlsx
+++ b/doc/Backlog [ACONIT].xlsx
@@ -39,10 +39,10 @@
   </definedNames>
   <calcPr calcId="125725"/>
   <customWorkbookViews>
+    <customWorkbookView name="Bernard Notarianni - Affichage personnalisé" guid="{178C21D0-B00A-4B0E-B009-71AAC80909BC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="785" activeSheetId="1"/>
+    <customWorkbookView name="Didier Lassissi - Affichage personnalisé" guid="{5E22A59B-ECE7-4B50-9619-81A99F53295A}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1064" windowHeight="552" activeSheetId="1"/>
+    <customWorkbookView name="uvba7442 - Affichage personnalisé" guid="{38566435-C99E-4958-9169-0C5C493EE97D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1213" windowHeight="665" activeSheetId="1"/>
     <customWorkbookView name="Yoann Regardin - Affichage personnalisé" guid="{29B12ED2-AD48-4E1C-B971-77E4D76C1B5F}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="609" activeSheetId="2"/>
-    <customWorkbookView name="uvba7442 - Affichage personnalisé" guid="{38566435-C99E-4958-9169-0C5C493EE97D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1213" windowHeight="665" activeSheetId="1"/>
-    <customWorkbookView name="Didier Lassissi - Affichage personnalisé" guid="{5E22A59B-ECE7-4B50-9619-81A99F53295A}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1064" windowHeight="552" activeSheetId="1"/>
-    <customWorkbookView name="Bernard Notarianni - Affichage personnalisé" guid="{178C21D0-B00A-4B0E-B009-71AAC80909BC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="785" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
@@ -1965,7 +1965,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.3703257666722557"/>
+          <c:x val="0.37032576667225586"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -1983,9 +1983,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532557"/>
+          <c:y val="0.15742128935532565"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192603"/>
+          <c:h val="0.70464767616192614"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2295,11 +2295,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="95414528"/>
-        <c:axId val="95760768"/>
+        <c:axId val="108394752"/>
+        <c:axId val="108474752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95414528"/>
+        <c:axId val="108394752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2331,7 +2331,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95760768"/>
+        <c:crossAx val="108474752"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2339,7 +2339,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95760768"/>
+        <c:axId val="108474752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2381,7 +2381,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95414528"/>
+        <c:crossAx val="108394752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2469,7 +2469,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000272" footer="0.49212598450000272"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000278" footer="0.49212598450000278"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2506,7 +2506,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225597"/>
+          <c:x val="0.37032576667225608"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2524,9 +2524,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532573"/>
+          <c:y val="0.15742128935532579"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192625"/>
+          <c:h val="0.70464767616192636"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2836,11 +2836,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="95978624"/>
-        <c:axId val="95980544"/>
+        <c:axId val="111051904"/>
+        <c:axId val="111053824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95978624"/>
+        <c:axId val="111051904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2872,7 +2872,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95980544"/>
+        <c:crossAx val="111053824"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2880,7 +2880,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95980544"/>
+        <c:axId val="111053824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2922,7 +2922,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95978624"/>
+        <c:crossAx val="111051904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3010,7 +3010,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000283" footer="0.49212598450000283"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000289" footer="0.49212598450000289"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3047,7 +3047,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.3703257666722562"/>
+          <c:x val="0.37032576667225636"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3065,9 +3065,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532584"/>
+          <c:y val="0.1574212893553259"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192658"/>
+          <c:h val="0.70464767616192681"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3209,13 +3209,13 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -3377,11 +3377,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="96165248"/>
-        <c:axId val="96183808"/>
+        <c:axId val="111238528"/>
+        <c:axId val="111257088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96165248"/>
+        <c:axId val="111238528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3413,7 +3413,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96183808"/>
+        <c:crossAx val="111257088"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3421,7 +3421,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96183808"/>
+        <c:axId val="111257088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3463,7 +3463,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96165248"/>
+        <c:crossAx val="111238528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3551,7 +3551,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000294" footer="0.49212598450000294"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.492125984500003" footer="0.492125984500003"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3588,7 +3588,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225647"/>
+          <c:x val="0.37032576667225658"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3606,9 +3606,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532596"/>
+          <c:y val="0.15742128935532601"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192692"/>
+          <c:h val="0.70464767616192703"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3918,11 +3918,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="96233344"/>
-        <c:axId val="96243712"/>
+        <c:axId val="111306624"/>
+        <c:axId val="111312896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96233344"/>
+        <c:axId val="111306624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3954,7 +3954,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96243712"/>
+        <c:crossAx val="111312896"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3962,7 +3962,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96243712"/>
+        <c:axId val="111312896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4004,7 +4004,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96233344"/>
+        <c:crossAx val="111306624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4092,7 +4092,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000306" footer="0.49212598450000306"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000311" footer="0.49212598450000311"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -8432,7 +8432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:DP85"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -11098,7 +11098,7 @@
   <dimension ref="A1:DP79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -11358,7 +11358,9 @@
       <c r="P4" s="72">
         <v>0</v>
       </c>
-      <c r="Q4" s="95"/>
+      <c r="Q4" s="72">
+        <v>0</v>
+      </c>
       <c r="R4" s="48"/>
     </row>
     <row r="5" spans="1:120" ht="24.95" customHeight="1">
@@ -11408,7 +11410,9 @@
       <c r="P5" s="72">
         <v>0</v>
       </c>
-      <c r="Q5" s="95"/>
+      <c r="Q5" s="72">
+        <v>0</v>
+      </c>
       <c r="R5" s="48"/>
     </row>
     <row r="6" spans="1:120" ht="24.95" customHeight="1">
@@ -11458,7 +11462,9 @@
       <c r="P6" s="147">
         <v>0</v>
       </c>
-      <c r="Q6" s="95"/>
+      <c r="Q6" s="147">
+        <v>0</v>
+      </c>
       <c r="R6" s="48"/>
     </row>
     <row r="7" spans="1:120" ht="24.95" customHeight="1">
@@ -11480,7 +11486,7 @@
       <c r="N7" s="91"/>
       <c r="O7" s="91"/>
       <c r="P7" s="91"/>
-      <c r="Q7" s="93"/>
+      <c r="Q7" s="91"/>
       <c r="R7" s="48"/>
     </row>
     <row r="8" spans="1:120" ht="24.95" customHeight="1">
@@ -11532,7 +11538,9 @@
       <c r="P8" s="147">
         <v>0</v>
       </c>
-      <c r="Q8" s="95"/>
+      <c r="Q8" s="147">
+        <v>0</v>
+      </c>
       <c r="R8" s="48"/>
     </row>
     <row r="9" spans="1:120" ht="24.95" customHeight="1">
@@ -11554,7 +11562,7 @@
       <c r="N9" s="91"/>
       <c r="O9" s="91"/>
       <c r="P9" s="91"/>
-      <c r="Q9" s="95"/>
+      <c r="Q9" s="91"/>
       <c r="R9" s="48"/>
     </row>
     <row r="10" spans="1:120" s="161" customFormat="1" ht="24.95" customHeight="1">
@@ -11604,7 +11612,9 @@
       <c r="P10" s="147">
         <v>0</v>
       </c>
-      <c r="Q10" s="95"/>
+      <c r="Q10" s="147">
+        <v>0</v>
+      </c>
       <c r="R10" s="95"/>
     </row>
     <row r="11" spans="1:120" ht="24.95" customHeight="1">
@@ -11656,7 +11666,9 @@
       <c r="P11" s="147">
         <v>0</v>
       </c>
-      <c r="Q11" s="92"/>
+      <c r="Q11" s="147">
+        <v>0</v>
+      </c>
       <c r="R11" s="49"/>
     </row>
     <row r="12" spans="1:120" ht="24.95" customHeight="1">
@@ -11699,16 +11711,18 @@
       <c r="M12" s="72">
         <v>10</v>
       </c>
-      <c r="N12" s="72">
+      <c r="N12" s="145">
         <v>10</v>
       </c>
-      <c r="O12" s="72">
-        <v>10</v>
-      </c>
-      <c r="P12" s="72">
-        <v>10</v>
-      </c>
-      <c r="Q12" s="94"/>
+      <c r="O12" s="145">
+        <v>7</v>
+      </c>
+      <c r="P12" s="145">
+        <v>4</v>
+      </c>
+      <c r="Q12" s="145">
+        <v>2</v>
+      </c>
       <c r="R12" s="49"/>
     </row>
     <row r="13" spans="1:120">
@@ -11769,15 +11783,15 @@
       </c>
       <c r="O14" s="38">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P14" s="38">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="Q14" s="38">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R14" s="38">
         <f t="shared" si="0"/>
@@ -11836,19 +11850,19 @@
       </c>
       <c r="O15" s="38">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P15" s="38">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Q15" s="38">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="R15" s="51">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:120">
@@ -11976,15 +11990,15 @@
       </c>
       <c r="O17" s="58">
         <f t="shared" si="3"/>
-        <v>0.76595744680851063</v>
+        <v>0.82978723404255317</v>
       </c>
       <c r="P17" s="58">
         <f t="shared" si="3"/>
-        <v>0.78723404255319152</v>
+        <v>0.91489361702127658</v>
       </c>
       <c r="Q17" s="58">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.95744680851063835</v>
       </c>
       <c r="R17" s="58">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Etat pulic/brouillon terminé : factoring des actions sur les pages des scènes et des éléments
</commit_message>
<xml_diff>
--- a/doc/Backlog [ACONIT].xlsx
+++ b/doc/Backlog [ACONIT].xlsx
@@ -39,10 +39,10 @@
   </definedNames>
   <calcPr calcId="125725"/>
   <customWorkbookViews>
+    <customWorkbookView name="Yoann Regardin - Affichage personnalisé" guid="{29B12ED2-AD48-4E1C-B971-77E4D76C1B5F}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="609" activeSheetId="2"/>
+    <customWorkbookView name="uvba7442 - Affichage personnalisé" guid="{38566435-C99E-4958-9169-0C5C493EE97D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1213" windowHeight="665" activeSheetId="1"/>
+    <customWorkbookView name="Didier Lassissi - Affichage personnalisé" guid="{5E22A59B-ECE7-4B50-9619-81A99F53295A}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1064" windowHeight="552" activeSheetId="1"/>
     <customWorkbookView name="Bernard Notarianni - Affichage personnalisé" guid="{178C21D0-B00A-4B0E-B009-71AAC80909BC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="785" activeSheetId="1"/>
-    <customWorkbookView name="Didier Lassissi - Affichage personnalisé" guid="{5E22A59B-ECE7-4B50-9619-81A99F53295A}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1064" windowHeight="552" activeSheetId="1"/>
-    <customWorkbookView name="uvba7442 - Affichage personnalisé" guid="{38566435-C99E-4958-9169-0C5C493EE97D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1213" windowHeight="665" activeSheetId="1"/>
-    <customWorkbookView name="Yoann Regardin - Affichage personnalisé" guid="{29B12ED2-AD48-4E1C-B971-77E4D76C1B5F}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="609" activeSheetId="2"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
@@ -1993,7 +1993,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225608"/>
+          <c:x val="0.3703257666722562"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2011,9 +2011,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532579"/>
+          <c:y val="0.15742128935532584"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192636"/>
+          <c:h val="0.70464767616192658"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2323,11 +2323,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="107731200"/>
-        <c:axId val="108085632"/>
+        <c:axId val="105634048"/>
+        <c:axId val="107037056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="107731200"/>
+        <c:axId val="105634048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2359,7 +2359,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108085632"/>
+        <c:crossAx val="107037056"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2367,7 +2367,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108085632"/>
+        <c:axId val="107037056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2409,7 +2409,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="107731200"/>
+        <c:crossAx val="105634048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2497,7 +2497,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000289" footer="0.49212598450000289"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000294" footer="0.49212598450000294"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2534,7 +2534,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225636"/>
+          <c:x val="0.37032576667225647"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2552,9 +2552,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.1574212893553259"/>
+          <c:y val="0.15742128935532596"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192681"/>
+          <c:h val="0.70464767616192692"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2864,11 +2864,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="108434560"/>
-        <c:axId val="108436480"/>
+        <c:axId val="107385984"/>
+        <c:axId val="107387904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="108434560"/>
+        <c:axId val="107385984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2900,7 +2900,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108436480"/>
+        <c:crossAx val="107387904"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2908,7 +2908,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108436480"/>
+        <c:axId val="107387904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2950,7 +2950,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108434560"/>
+        <c:crossAx val="107385984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3038,7 +3038,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.492125984500003" footer="0.492125984500003"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000306" footer="0.49212598450000306"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3075,7 +3075,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225658"/>
+          <c:x val="0.3703257666722567"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3093,9 +3093,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532601"/>
+          <c:y val="0.15742128935532607"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192703"/>
+          <c:h val="0.70464767616192714"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3405,11 +3405,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="108486016"/>
-        <c:axId val="108504576"/>
+        <c:axId val="107441536"/>
+        <c:axId val="107460096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="108486016"/>
+        <c:axId val="107441536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3441,7 +3441,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108504576"/>
+        <c:crossAx val="107460096"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3449,7 +3449,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108504576"/>
+        <c:axId val="107460096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3491,7 +3491,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108486016"/>
+        <c:crossAx val="107441536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3579,7 +3579,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000311" footer="0.49212598450000311"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000317" footer="0.49212598450000317"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3616,7 +3616,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37032576667225686"/>
+          <c:x val="0.37032576667225697"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3634,9 +3634,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532615"/>
+          <c:y val="0.15742128935532623"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192725"/>
+          <c:h val="0.70464767616192736"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3742,13 +3742,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>37</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>#N/A</c:v>
@@ -3894,63 +3894,63 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>37</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34.533333333333331</c:v>
+                  <c:v>32.666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32.066666666666663</c:v>
+                  <c:v>30.333333333333332</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29.599999999999994</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27.133333333333326</c:v>
+                  <c:v>25.666666666666668</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24.666666666666657</c:v>
+                  <c:v>23.333333333333336</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22.199999999999989</c:v>
+                  <c:v>21.000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19.73333333333332</c:v>
+                  <c:v>18.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17.266666666666652</c:v>
+                  <c:v>16.333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14.799999999999985</c:v>
+                  <c:v>14.000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12.333333333333318</c:v>
+                  <c:v>11.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.8666666666666512</c:v>
+                  <c:v>9.3333333333333375</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.3999999999999844</c:v>
+                  <c:v>7.0000000000000036</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.9333333333333176</c:v>
+                  <c:v>4.6666666666666696</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.4666666666666508</c:v>
+                  <c:v>2.3333333333333361</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-1.5987211554602254E-14</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="108558208"/>
-        <c:axId val="108564480"/>
+        <c:axId val="107509632"/>
+        <c:axId val="107520000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="108558208"/>
+        <c:axId val="107509632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3982,7 +3982,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108564480"/>
+        <c:crossAx val="107520000"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3990,7 +3990,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108564480"/>
+        <c:axId val="107520000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4032,7 +4032,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108558208"/>
+        <c:crossAx val="107509632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4120,7 +4120,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000322" footer="0.49212598450000322"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000328" footer="0.49212598450000328"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -13339,7 +13339,7 @@
   <dimension ref="A1:DP79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -13536,13 +13536,13 @@
         <v>33</v>
       </c>
       <c r="C3" s="158">
+        <v>4</v>
+      </c>
+      <c r="D3" s="158">
+        <v>3</v>
+      </c>
+      <c r="E3" s="102">
         <v>2</v>
-      </c>
-      <c r="D3" s="158">
-        <v>1</v>
-      </c>
-      <c r="E3" s="102">
-        <v>1</v>
       </c>
       <c r="F3" s="87"/>
       <c r="G3" s="87"/>
@@ -13626,13 +13626,13 @@
         <v>36</v>
       </c>
       <c r="C6" s="141">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D6" s="141">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E6" s="71">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F6" s="93"/>
       <c r="G6" s="93"/>
@@ -13777,15 +13777,15 @@
       </c>
       <c r="C11" s="37">
         <f t="array" ref="C11">IF(ISBLANK(C3:C9), NA(), SUM(C3:C9))</f>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D11" s="37">
         <f t="array" ref="D11">IF(ISBLANK(D3:D9), NA(), SUM(D3:D9))</f>
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E11" s="37">
         <f t="array" ref="E11">IF(ISBLANK(E3:E9), NA(), SUM(E3:E9))</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F11" s="37" t="e">
         <f t="array" ref="F11">IF(ISBLANK(F3:F9), NA(), SUM(F3:F9))</f>
@@ -13950,11 +13950,11 @@
       <c r="C12" s="37"/>
       <c r="D12" s="37">
         <f t="shared" ref="D12:R12" si="0">C11-D11</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E12" s="37">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F12" s="37" t="e">
         <f t="shared" si="0"/>
@@ -14118,67 +14118,67 @@
       </c>
       <c r="C13" s="44">
         <f>C11</f>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D13" s="45">
         <f t="shared" ref="D13:R13" si="1">C13-$C$11/COUNTA($C$2:$Q$2)</f>
-        <v>34.533333333333331</v>
+        <v>32.666666666666664</v>
       </c>
       <c r="E13" s="45">
         <f t="shared" si="1"/>
-        <v>32.066666666666663</v>
+        <v>30.333333333333332</v>
       </c>
       <c r="F13" s="45">
         <f t="shared" si="1"/>
-        <v>29.599999999999994</v>
+        <v>28</v>
       </c>
       <c r="G13" s="45">
         <f t="shared" si="1"/>
-        <v>27.133333333333326</v>
+        <v>25.666666666666668</v>
       </c>
       <c r="H13" s="45">
         <f t="shared" si="1"/>
-        <v>24.666666666666657</v>
+        <v>23.333333333333336</v>
       </c>
       <c r="I13" s="45">
         <f t="shared" si="1"/>
-        <v>22.199999999999989</v>
+        <v>21.000000000000004</v>
       </c>
       <c r="J13" s="45">
         <f t="shared" si="1"/>
-        <v>19.73333333333332</v>
+        <v>18.666666666666671</v>
       </c>
       <c r="K13" s="45">
         <f t="shared" si="1"/>
-        <v>17.266666666666652</v>
+        <v>16.333333333333339</v>
       </c>
       <c r="L13" s="45">
         <f t="shared" si="1"/>
-        <v>14.799999999999985</v>
+        <v>14.000000000000005</v>
       </c>
       <c r="M13" s="45">
         <f t="shared" si="1"/>
-        <v>12.333333333333318</v>
+        <v>11.666666666666671</v>
       </c>
       <c r="N13" s="45">
         <f t="shared" si="1"/>
-        <v>9.8666666666666512</v>
+        <v>9.3333333333333375</v>
       </c>
       <c r="O13" s="45">
         <f t="shared" si="1"/>
-        <v>7.3999999999999844</v>
+        <v>7.0000000000000036</v>
       </c>
       <c r="P13" s="45">
         <f t="shared" si="1"/>
-        <v>4.9333333333333176</v>
+        <v>4.6666666666666696</v>
       </c>
       <c r="Q13" s="45">
         <f t="shared" si="1"/>
-        <v>2.4666666666666508</v>
+        <v>2.3333333333333361</v>
       </c>
       <c r="R13" s="51">
         <f t="shared" si="1"/>
-        <v>-1.5987211554602254E-14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:120" s="55" customFormat="1">
@@ -14192,11 +14192,11 @@
       </c>
       <c r="D14" s="57">
         <f t="shared" ref="D14:R14" si="2">1-D11/$C$11</f>
-        <v>0.13513513513513509</v>
+        <v>0.17142857142857137</v>
       </c>
       <c r="E14" s="57">
         <f t="shared" si="2"/>
-        <v>0.35135135135135132</v>
+        <v>0.34285714285714286</v>
       </c>
       <c r="F14" s="57" t="e">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Description champ select manquante dans la création d'un élément
</commit_message>
<xml_diff>
--- a/doc/Backlog [ACONIT].xlsx
+++ b/doc/Backlog [ACONIT].xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10155" yWindow="0" windowWidth="8835" windowHeight="10065" tabRatio="900" activeTab="4"/>
+    <workbookView xWindow="10155" yWindow="0" windowWidth="8835" windowHeight="10065" tabRatio="900" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="20" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Product backlog'!$5:$5</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Iteration 1'!$R$12:$Z$22</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Iteration 2'!$R$16:$Z$25</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'Iteration 3'!$R$13:$Z$19</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Iteration 3'!$R$13:$Z$18</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'Iteration 4'!$R$10:$Z$19</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Product backlog'!#REF!</definedName>
   </definedNames>
@@ -366,16 +366,7 @@
     <t>Système de log pour tracer toutes les actions</t>
   </si>
   <si>
-    <t xml:space="preserve">        - Gestion de plusieurs sous-parcours </t>
-  </si>
-  <si>
     <t xml:space="preserve">        - Gestion de plusieurs sous-parcours</t>
-  </si>
-  <si>
-    <t>Visualisation graphique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        - Edition parcours avec transitions secondaires</t>
   </si>
   <si>
     <t>Divers</t>
@@ -421,6 +412,15 @@
   </si>
   <si>
     <t>Fournir une aide pour utiliser l'application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Visualisation graphique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Edition parcours avec transitions secondaires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Gestion de plusieurs sous-parcours </t>
   </si>
 </sst>
 </file>
@@ -1981,7 +1981,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.3703257666722567"/>
+          <c:x val="0.37032576667225697"/>
           <c:y val="2.6986506746626688E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -1999,9 +1999,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532607"/>
+          <c:y val="0.15742128935532623"/>
           <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192714"/>
+          <c:h val="0.70464767616192736"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2311,11 +2311,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="109107456"/>
-        <c:axId val="109265280"/>
+        <c:axId val="110549248"/>
+        <c:axId val="110838144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="109107456"/>
+        <c:axId val="110549248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2347,7 +2347,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="109265280"/>
+        <c:crossAx val="110838144"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2355,7 +2355,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109265280"/>
+        <c:axId val="110838144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2397,548 +2397,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="109107456"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.82639198178585549"/>
-          <c:y val="3.2983508245877091E-2"/>
-          <c:w val="0.11675295106908352"/>
-          <c:h val="9.145427286356822E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="3175">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1445" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:ea typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
-    </a:solidFill>
-    <a:ln w="3175">
-      <a:solidFill>
-        <a:srgbClr val="000000"/>
-      </a:solidFill>
-      <a:prstDash val="solid"/>
-    </a:ln>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr sz="1575" b="0" i="0" u="none" strike="noStrike" baseline="0">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:latin typeface="Arial"/>
-          <a:ea typeface="Arial"/>
-          <a:cs typeface="Arial"/>
-        </a:defRPr>
-      </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000317" footer="0.49212598450000317"/>
-    <c:pageSetup paperSize="9" orientation="landscape"/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="fr-FR"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1900" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-                <a:ea typeface="Arial"/>
-                <a:cs typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="fr-FR"/>
-              <a:t>Suivi charge Iteration 2</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.37032576667225697"/>
-          <c:y val="2.6986506746626688E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="25400">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="5.5640078243859845E-2"/>
-          <c:y val="0.15742128935532623"/>
-          <c:w val="0.92946294640153049"/>
-          <c:h val="0.70464767616192736"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Iteration 2'!$B$17</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Iteration </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="12700">
-              <a:solidFill>
-                <a:srgbClr val="000080"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="000080"/>
-              </a:solidFill>
-              <a:ln>
-                <a:solidFill>
-                  <a:srgbClr val="000080"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Iteration 2'!$C$2:$R$2</c:f>
-              <c:numCache>
-                <c:formatCode>[$-40C]d\-mmm;@</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>41407</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41408</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41409</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>41410</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>41411</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>41414</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>41415</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>41416</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>41417</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>41418</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>41421</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41422</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41423</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41424</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41425</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>41428</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Iteration 2'!$C$17:$R$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Iteration 2'!$B$19</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>REF</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="12700">
-              <a:solidFill>
-                <a:srgbClr val="FF00FF"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FF00FF"/>
-              </a:solidFill>
-              <a:ln>
-                <a:solidFill>
-                  <a:srgbClr val="FF00FF"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Iteration 2'!$C$2:$R$2</c:f>
-              <c:numCache>
-                <c:formatCode>[$-40C]d\-mmm;@</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>41407</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41408</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41409</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>41410</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>41411</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>41414</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>41415</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>41416</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>41417</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>41418</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>41421</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41422</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41423</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41424</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41425</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>41428</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Iteration 2'!$C$19:$R$19</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>45.733333333333334</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42.466666666666669</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>39.200000000000003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>35.933333333333337</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.666666666666671</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>29.400000000000006</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>26.13333333333334</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>22.866666666666674</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>19.600000000000009</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>16.333333333333343</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>13.066666666666677</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>9.8000000000000114</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6.5333333333333448</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.2666666666666782</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.1546319456101628E-14</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="110797952"/>
-        <c:axId val="110799872"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="110797952"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="[$-40C]d\-mmm;@" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="3175">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:prstDash val="solid"/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="0" vert="horz"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1575" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-                <a:ea typeface="Arial"/>
-                <a:cs typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="110799872"/>
-        <c:crosses val="autoZero"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:tickLblSkip val="1"/>
-        <c:tickMarkSkip val="1"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="110799872"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="3175">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="3175">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:prstDash val="solid"/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="0" vert="horz"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1575" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-                <a:ea typeface="Arial"/>
-                <a:cs typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="110797952"/>
+        <c:crossAx val="110549248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3032,7 +2491,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="fr-FR"/>
   <c:chart>
@@ -3054,7 +2513,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-FR"/>
-              <a:t>Suivi charge Iteration 3</a:t>
+              <a:t>Suivi charge Iteration 2</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3093,7 +2552,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Iteration 3'!$B$14</c:f>
+              <c:f>'Iteration 2'!$B$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3127,111 +2586,111 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Iteration 3'!$C$2:$R$2</c:f>
+              <c:f>'Iteration 2'!$C$2:$R$2</c:f>
               <c:numCache>
                 <c:formatCode>[$-40C]d\-mmm;@</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
+                  <c:v>41407</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41408</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41409</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41410</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41411</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41414</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41415</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41416</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41417</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41418</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41421</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41422</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41423</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41424</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41425</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>41428</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41429</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41430</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>41431</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>41432</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>41435</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>41436</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>41437</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>41438</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>41439</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>41442</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41443</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41444</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41445</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41446</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>41449</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Iteration 3'!$C$14:$R$14</c:f>
+              <c:f>'Iteration 2'!$C$17:$R$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>47</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>17</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -3245,7 +2704,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Iteration 3'!$B$16</c:f>
+              <c:f>'Iteration 2'!$B$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3279,125 +2738,125 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Iteration 3'!$C$2:$R$2</c:f>
+              <c:f>'Iteration 2'!$C$2:$R$2</c:f>
               <c:numCache>
                 <c:formatCode>[$-40C]d\-mmm;@</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
+                  <c:v>41407</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41408</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41409</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41410</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41411</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41414</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41415</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41416</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41417</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41418</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41421</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41422</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41423</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41424</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41425</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>41428</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41429</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41430</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>41431</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>41432</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>41435</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>41436</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>41437</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>41438</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>41439</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>41442</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41443</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41444</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41445</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41446</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>41449</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Iteration 3'!$C$16:$R$16</c:f>
+              <c:f>'Iteration 2'!$C$19:$R$19</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>47</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43.866666666666667</c:v>
+                  <c:v>45.733333333333334</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40.733333333333334</c:v>
+                  <c:v>42.466666666666669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37.6</c:v>
+                  <c:v>39.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>34.466666666666669</c:v>
+                  <c:v>35.933333333333337</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31.333333333333336</c:v>
+                  <c:v>32.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28.200000000000003</c:v>
+                  <c:v>29.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25.06666666666667</c:v>
+                  <c:v>26.13333333333334</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21.933333333333337</c:v>
+                  <c:v>22.866666666666674</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18.800000000000004</c:v>
+                  <c:v>19.600000000000009</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15.666666666666671</c:v>
+                  <c:v>16.333333333333343</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12.533333333333339</c:v>
+                  <c:v>13.066666666666677</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.4000000000000057</c:v>
+                  <c:v>9.8000000000000114</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.2666666666666728</c:v>
+                  <c:v>6.5333333333333448</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.1333333333333395</c:v>
+                  <c:v>3.2666666666666782</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.2172489379008766E-15</c:v>
+                  <c:v>1.1546319456101628E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="110849408"/>
-        <c:axId val="110867968"/>
+        <c:axId val="111191168"/>
+        <c:axId val="111193088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="110849408"/>
+        <c:axId val="111191168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3429,7 +2888,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="110867968"/>
+        <c:crossAx val="111193088"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3437,7 +2896,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110867968"/>
+        <c:axId val="111193088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3479,7 +2938,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="110849408"/>
+        <c:crossAx val="111191168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3573,7 +3032,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="fr-FR"/>
   <c:chart>
@@ -3595,7 +3054,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-FR"/>
-              <a:t>Suivi charge Iteration 4</a:t>
+              <a:t>Suivi charge Iteration 3</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3634,7 +3093,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Iteration 4'!$B$11</c:f>
+              <c:f>'Iteration 3'!$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3668,114 +3127,114 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Iteration 4'!$C$2:$R$2</c:f>
+              <c:f>'Iteration 3'!$C$2:$R$2</c:f>
               <c:numCache>
                 <c:formatCode>[$-40C]d\-mmm;@</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
+                  <c:v>41428</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41429</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41430</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41431</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41432</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41435</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41436</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41437</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41438</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41439</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41442</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41443</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41444</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41445</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41446</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>41449</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41450</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41451</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>41452</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>41453</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>41456</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>41457</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>41458</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>41459</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>41460</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>41463</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41464</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41465</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41466</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41467</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>41470</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Iteration 4'!$C$11:$R$11</c:f>
+              <c:f>'Iteration 3'!$C$13:$R$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>#N/A</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>#N/A</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>#N/A</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>#N/A</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>#N/A</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3786,7 +3245,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Iteration 4'!$B$13</c:f>
+              <c:f>'Iteration 3'!$B$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3820,125 +3279,125 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Iteration 4'!$C$2:$R$2</c:f>
+              <c:f>'Iteration 3'!$C$2:$R$2</c:f>
               <c:numCache>
                 <c:formatCode>[$-40C]d\-mmm;@</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
+                  <c:v>41428</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41429</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41430</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41431</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41432</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41435</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41436</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41437</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41438</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41439</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41442</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41443</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41444</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41445</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41446</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>41449</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41450</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41451</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>41452</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>41453</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>41456</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>41457</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>41458</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>41459</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>41460</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>41463</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41464</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41465</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41466</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41467</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>41470</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Iteration 4'!$C$13:$R$13</c:f>
+              <c:f>'Iteration 3'!$C$15:$R$15</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>35</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32.666666666666664</c:v>
+                  <c:v>43.866666666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30.333333333333332</c:v>
+                  <c:v>40.733333333333334</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28</c:v>
+                  <c:v>37.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25.666666666666668</c:v>
+                  <c:v>34.466666666666669</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.333333333333336</c:v>
+                  <c:v>31.333333333333336</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.000000000000004</c:v>
+                  <c:v>28.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18.666666666666671</c:v>
+                  <c:v>25.06666666666667</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16.333333333333339</c:v>
+                  <c:v>21.933333333333337</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14.000000000000005</c:v>
+                  <c:v>18.800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.666666666666671</c:v>
+                  <c:v>15.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.3333333333333375</c:v>
+                  <c:v>12.533333333333339</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.0000000000000036</c:v>
+                  <c:v>9.4000000000000057</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.6666666666666696</c:v>
+                  <c:v>6.2666666666666728</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.3333333333333361</c:v>
+                  <c:v>3.1333333333333395</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>6.2172489379008766E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="110917504"/>
-        <c:axId val="110927872"/>
+        <c:axId val="111242624"/>
+        <c:axId val="111261184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="110917504"/>
+        <c:axId val="111242624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3970,7 +3429,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="110927872"/>
+        <c:crossAx val="111261184"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3978,7 +3437,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110927872"/>
+        <c:axId val="111261184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4020,7 +3479,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="110917504"/>
+        <c:crossAx val="111242624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4114,6 +3573,547 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="fr-FR"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1900" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Suivi charge Iteration 4</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.37032576667225769"/>
+          <c:y val="2.6986506746626688E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.5640078243859845E-2"/>
+          <c:y val="0.15742128935532657"/>
+          <c:w val="0.92946294640153049"/>
+          <c:h val="0.70464767616192825"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Iteration 4'!$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Iteration </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:srgbClr val="000080"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="000080"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="000080"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Iteration 4'!$C$2:$R$2</c:f>
+              <c:numCache>
+                <c:formatCode>[$-40C]d\-mmm;@</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>41449</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41450</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41451</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41452</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41453</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41456</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41457</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41458</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41459</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41460</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41463</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41464</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41465</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41466</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41467</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41470</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Iteration 4'!$C$11:$R$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Iteration 4'!$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>REF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:srgbClr val="FF00FF"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF00FF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="FF00FF"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Iteration 4'!$C$2:$R$2</c:f>
+              <c:numCache>
+                <c:formatCode>[$-40C]d\-mmm;@</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>41449</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41450</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41451</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41452</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41453</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41456</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41457</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41458</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41459</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41460</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41463</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41464</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41465</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41466</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41467</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41470</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Iteration 4'!$C$13:$R$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.666666666666668</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.333333333333336</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18.666666666666671</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.333333333333339</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.666666666666671</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.3333333333333375</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.0000000000000036</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.6666666666666696</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.3333333333333361</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="111310720"/>
+        <c:axId val="111321088"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="111310720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="[$-40C]d\-mmm;@" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="3175">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1575" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="111321088"/>
+        <c:crosses val="autoZero"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="111321088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="3175">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="3175">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1575" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="111310720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.82639198178585549"/>
+          <c:y val="3.2983508245877091E-2"/>
+          <c:w val="0.11675295106908352"/>
+          <c:h val="9.145427286356822E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="3175">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1445" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:ea typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln w="3175">
+      <a:solidFill>
+        <a:srgbClr val="000000"/>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1575" b="0" i="0" u="none" strike="noStrike" baseline="0">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Arial"/>
+          <a:ea typeface="Arial"/>
+          <a:cs typeface="Arial"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter alignWithMargins="0"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000361" footer="0.49212598450000361"/>
+    <c:pageSetup paperSize="9" orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -4193,15 +4193,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>112059</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>65444</xdr:rowOff>
+      <xdr:colOff>44824</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76651</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>11204</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>62002</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>661146</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>100854</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5438,7 +5438,7 @@
         <v>1</v>
       </c>
       <c r="D37" s="69" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E37" s="69"/>
       <c r="F37" s="71" t="s">
@@ -5507,7 +5507,7 @@
         <v>1</v>
       </c>
       <c r="D40" s="81" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E40" s="70"/>
       <c r="F40" s="71" t="s">
@@ -5573,10 +5573,10 @@
       </c>
       <c r="C43" s="67"/>
       <c r="D43" s="69" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E43" s="69" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F43" s="71" t="s">
         <v>31</v>
@@ -5598,10 +5598,10 @@
       </c>
       <c r="C44" s="67"/>
       <c r="D44" s="69" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E44" s="69" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F44" s="71" t="s">
         <v>31</v>
@@ -5623,10 +5623,10 @@
       </c>
       <c r="C45" s="99"/>
       <c r="D45" s="83" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E45" s="83" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F45" s="71" t="s">
         <v>31</v>
@@ -5648,10 +5648,10 @@
       </c>
       <c r="C46" s="67"/>
       <c r="D46" s="69" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E46" s="69" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F46" s="71" t="s">
         <v>31</v>
@@ -5671,7 +5671,7 @@
       <c r="B47" s="68"/>
       <c r="C47" s="67"/>
       <c r="D47" s="69" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E47" s="69"/>
       <c r="F47" s="71" t="s">
@@ -5694,7 +5694,7 @@
       </c>
       <c r="C48" s="67"/>
       <c r="D48" s="69" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E48" s="69"/>
       <c r="F48" s="71" t="s">
@@ -5715,10 +5715,10 @@
       <c r="B49" s="68"/>
       <c r="C49" s="67"/>
       <c r="D49" s="69" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E49" s="69" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F49" s="71" t="s">
         <v>31</v>
@@ -5738,10 +5738,10 @@
       <c r="B50" s="68"/>
       <c r="C50" s="67"/>
       <c r="D50" s="69" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E50" s="69" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F50" s="71" t="s">
         <v>31</v>
@@ -11176,11 +11176,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DP79"/>
+  <dimension ref="A1:DP78"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
@@ -11578,7 +11576,7 @@
     </row>
     <row r="8" spans="1:120" ht="24.95" customHeight="1">
       <c r="A8" s="69" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="B8" s="74">
         <v>23</v>
@@ -11656,7 +11654,7 @@
     </row>
     <row r="10" spans="1:120" s="155" customFormat="1" ht="24.95" customHeight="1">
       <c r="A10" s="145" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="B10" s="141"/>
       <c r="C10" s="141">
@@ -11710,7 +11708,7 @@
     </row>
     <row r="11" spans="1:120" ht="24.95" customHeight="1">
       <c r="A11" s="69" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="B11" s="74">
         <v>27</v>
@@ -11766,7 +11764,7 @@
     </row>
     <row r="12" spans="1:120" ht="24.95" customHeight="1">
       <c r="A12" s="81" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B12" s="74">
         <v>30</v>
@@ -11820,291 +11818,308 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:120">
-      <c r="A13" s="37"/>
-    </row>
-    <row r="14" spans="1:120" s="55" customFormat="1">
-      <c r="A14" s="54"/>
-      <c r="B14" s="42" t="s">
+    <row r="13" spans="1:120" s="55" customFormat="1">
+      <c r="A13" s="54"/>
+      <c r="B13" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="37">
-        <f t="shared" ref="C14:R14" si="0">IF(ISBLANK(C3:C12), NA(), SUM(C3:C12))</f>
+      <c r="C13" s="37">
+        <f t="shared" ref="C13:R13" si="0">IF(ISBLANK(C3:C12), NA(), SUM(C3:C12))</f>
         <v>47</v>
       </c>
-      <c r="D14" s="37">
+      <c r="D13" s="37">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="E14" s="37">
+      <c r="E13" s="37">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="F14" s="37">
+      <c r="F13" s="37">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="G14" s="37">
+      <c r="G13" s="37">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="H14" s="37">
+      <c r="H13" s="37">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="I14" s="37">
+      <c r="I13" s="37">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="J14" s="37">
+      <c r="J13" s="37">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="K14" s="37">
+      <c r="K13" s="37">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="L14" s="37">
+      <c r="L13" s="37">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="M14" s="37">
+      <c r="M13" s="37">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="N14" s="37">
+      <c r="N13" s="37">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="O14" s="37">
+      <c r="O13" s="37">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="P14" s="37">
+      <c r="P13" s="37">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="Q14" s="37">
+      <c r="Q13" s="37">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="R14" s="37">
+      <c r="R13" s="37">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:120" ht="25.5">
-      <c r="A15" s="37"/>
-      <c r="B15" s="42" t="s">
+    <row r="14" spans="1:120" ht="25.5">
+      <c r="A14" s="37"/>
+      <c r="B14" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37">
-        <f t="shared" ref="D15:R15" si="1">C14-D14</f>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37">
+        <f t="shared" ref="D14:R14" si="1">C13-D13</f>
         <v>5</v>
       </c>
-      <c r="E15" s="37">
+      <c r="E14" s="37">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F15" s="37">
+      <c r="F14" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G15" s="37">
+      <c r="G14" s="37">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="H15" s="37">
+      <c r="H14" s="37">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I15" s="37">
+      <c r="I14" s="37">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="J15" s="37">
+      <c r="J14" s="37">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="K15" s="37">
+      <c r="K14" s="37">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="L15" s="37">
+      <c r="L14" s="37">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="M15" s="37">
+      <c r="M14" s="37">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="N15" s="37">
+      <c r="N14" s="37">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="O15" s="37">
+      <c r="O14" s="37">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="P15" s="37">
+      <c r="P14" s="37">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="Q15" s="37">
+      <c r="Q14" s="37">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="R15" s="50">
+      <c r="R14" s="50">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
+    <row r="15" spans="1:120">
+      <c r="A15" s="37"/>
+      <c r="B15" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="44">
+        <f>C13</f>
+        <v>47</v>
+      </c>
+      <c r="D15" s="45">
+        <f>C15-$C$13/COUNTA($C$2:$Q$2)</f>
+        <v>43.866666666666667</v>
+      </c>
+      <c r="E15" s="45">
+        <f>D15-$C$13/COUNTA($C$2:$Q$2)</f>
+        <v>40.733333333333334</v>
+      </c>
+      <c r="F15" s="45">
+        <f>E15-$C$13/COUNTA($C$2:$Q$2)</f>
+        <v>37.6</v>
+      </c>
+      <c r="G15" s="45">
+        <f>F15-$C$13/COUNTA($C$2:$Q$2)</f>
+        <v>34.466666666666669</v>
+      </c>
+      <c r="H15" s="45">
+        <f>G15-$C$13/COUNTA($C$2:$Q$2)</f>
+        <v>31.333333333333336</v>
+      </c>
+      <c r="I15" s="45">
+        <f>H15-$C$13/COUNTA($C$2:$Q$2)</f>
+        <v>28.200000000000003</v>
+      </c>
+      <c r="J15" s="45">
+        <f>I15-$C$13/COUNTA($C$2:$Q$2)</f>
+        <v>25.06666666666667</v>
+      </c>
+      <c r="K15" s="45">
+        <f>J15-$C$13/COUNTA($C$2:$Q$2)</f>
+        <v>21.933333333333337</v>
+      </c>
+      <c r="L15" s="45">
+        <f>K15-$C$13/COUNTA($C$2:$Q$2)</f>
+        <v>18.800000000000004</v>
+      </c>
+      <c r="M15" s="45">
+        <f>L15-$C$13/COUNTA($C$2:$Q$2)</f>
+        <v>15.666666666666671</v>
+      </c>
+      <c r="N15" s="45">
+        <f>M15-$C$13/COUNTA($C$2:$Q$2)</f>
+        <v>12.533333333333339</v>
+      </c>
+      <c r="O15" s="45">
+        <f>N15-$C$13/COUNTA($C$2:$Q$2)</f>
+        <v>9.4000000000000057</v>
+      </c>
+      <c r="P15" s="45">
+        <f>O15-$C$13/COUNTA($C$2:$Q$2)</f>
+        <v>6.2666666666666728</v>
+      </c>
+      <c r="Q15" s="45">
+        <f>P15-$C$13/COUNTA($C$2:$Q$2)</f>
+        <v>3.1333333333333395</v>
+      </c>
+      <c r="R15" s="51">
+        <f>Q15-$C$13/COUNTA($C$2:$Q$2)</f>
+        <v>6.2172489379008766E-15</v>
+      </c>
+    </row>
     <row r="16" spans="1:120">
       <c r="A16" s="37"/>
-      <c r="B16" s="43" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="44">
-        <f>C14</f>
-        <v>47</v>
-      </c>
-      <c r="D16" s="45">
-        <f t="shared" ref="D16:R16" si="2">C16-$C$14/COUNTA($C$2:$Q$2)</f>
-        <v>43.866666666666667</v>
-      </c>
-      <c r="E16" s="45">
+      <c r="B16" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="57">
+        <f t="shared" ref="C16:R16" si="2">1-C13/$C$13</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="57">
         <f t="shared" si="2"/>
-        <v>40.733333333333334</v>
-      </c>
-      <c r="F16" s="45">
+        <v>0.1063829787234043</v>
+      </c>
+      <c r="E16" s="57">
         <f t="shared" si="2"/>
-        <v>37.6</v>
-      </c>
-      <c r="G16" s="45">
+        <v>0.14893617021276595</v>
+      </c>
+      <c r="F16" s="57">
         <f t="shared" si="2"/>
-        <v>34.466666666666669</v>
-      </c>
-      <c r="H16" s="45">
+        <v>0.14893617021276595</v>
+      </c>
+      <c r="G16" s="57">
         <f t="shared" si="2"/>
-        <v>31.333333333333336</v>
-      </c>
-      <c r="I16" s="45">
+        <v>0.21276595744680848</v>
+      </c>
+      <c r="H16" s="57">
         <f t="shared" si="2"/>
-        <v>28.200000000000003</v>
-      </c>
-      <c r="J16" s="45">
+        <v>0.2978723404255319</v>
+      </c>
+      <c r="I16" s="57">
         <f t="shared" si="2"/>
-        <v>25.06666666666667</v>
-      </c>
-      <c r="K16" s="45">
+        <v>0.4042553191489362</v>
+      </c>
+      <c r="J16" s="57">
         <f t="shared" si="2"/>
-        <v>21.933333333333337</v>
-      </c>
-      <c r="L16" s="45">
+        <v>0.48936170212765961</v>
+      </c>
+      <c r="K16" s="57">
         <f t="shared" si="2"/>
-        <v>18.800000000000004</v>
-      </c>
-      <c r="M16" s="45">
+        <v>0.53191489361702127</v>
+      </c>
+      <c r="L16" s="57">
         <f t="shared" si="2"/>
-        <v>15.666666666666671</v>
-      </c>
-      <c r="N16" s="45">
+        <v>0.63829787234042556</v>
+      </c>
+      <c r="M16" s="57">
         <f t="shared" si="2"/>
-        <v>12.533333333333339</v>
-      </c>
-      <c r="O16" s="45">
+        <v>0.7021276595744681</v>
+      </c>
+      <c r="N16" s="57">
         <f t="shared" si="2"/>
-        <v>9.4000000000000057</v>
-      </c>
-      <c r="P16" s="45">
+        <v>0.74468085106382986</v>
+      </c>
+      <c r="O16" s="57">
         <f t="shared" si="2"/>
-        <v>6.2666666666666728</v>
-      </c>
-      <c r="Q16" s="45">
+        <v>0.82978723404255317</v>
+      </c>
+      <c r="P16" s="57">
         <f t="shared" si="2"/>
-        <v>3.1333333333333395</v>
-      </c>
-      <c r="R16" s="51">
+        <v>0.91489361702127658</v>
+      </c>
+      <c r="Q16" s="57">
         <f t="shared" si="2"/>
-        <v>6.2172489379008766E-15</v>
+        <v>0.95744680851063835</v>
+      </c>
+      <c r="R16" s="57">
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:18">
       <c r="A17" s="37"/>
-      <c r="B17" s="56" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="57">
-        <f t="shared" ref="C17:R17" si="3">1-C14/$C$14</f>
-        <v>0</v>
-      </c>
-      <c r="D17" s="57">
-        <f t="shared" si="3"/>
-        <v>0.1063829787234043</v>
-      </c>
-      <c r="E17" s="57">
-        <f t="shared" si="3"/>
-        <v>0.14893617021276595</v>
-      </c>
-      <c r="F17" s="57">
-        <f t="shared" si="3"/>
-        <v>0.14893617021276595</v>
-      </c>
-      <c r="G17" s="57">
-        <f t="shared" si="3"/>
-        <v>0.21276595744680848</v>
-      </c>
-      <c r="H17" s="57">
-        <f t="shared" si="3"/>
-        <v>0.2978723404255319</v>
-      </c>
-      <c r="I17" s="57">
-        <f t="shared" si="3"/>
-        <v>0.4042553191489362</v>
-      </c>
-      <c r="J17" s="57">
-        <f t="shared" si="3"/>
-        <v>0.48936170212765961</v>
-      </c>
-      <c r="K17" s="57">
-        <f t="shared" si="3"/>
-        <v>0.53191489361702127</v>
-      </c>
-      <c r="L17" s="57">
-        <f t="shared" si="3"/>
-        <v>0.63829787234042556</v>
-      </c>
-      <c r="M17" s="57">
-        <f t="shared" si="3"/>
-        <v>0.7021276595744681</v>
-      </c>
-      <c r="N17" s="57">
-        <f t="shared" si="3"/>
-        <v>0.74468085106382986</v>
-      </c>
-      <c r="O17" s="57">
-        <f t="shared" si="3"/>
-        <v>0.82978723404255317</v>
-      </c>
-      <c r="P17" s="57">
-        <f t="shared" si="3"/>
-        <v>0.91489361702127658</v>
-      </c>
-      <c r="Q17" s="57">
-        <f t="shared" si="3"/>
-        <v>0.95744680851063835</v>
-      </c>
-      <c r="R17" s="57">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="37"/>
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="37"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="37"/>
+      <c r="P19" s="37"/>
+      <c r="Q19" s="37"/>
+      <c r="R19" s="37"/>
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="37"/>
@@ -13286,32 +13301,12 @@
       <c r="Q78" s="37"/>
       <c r="R78" s="37"/>
     </row>
-    <row r="79" spans="1:18">
-      <c r="A79" s="37"/>
-      <c r="B79" s="37"/>
-      <c r="C79" s="37"/>
-      <c r="D79" s="37"/>
-      <c r="E79" s="37"/>
-      <c r="F79" s="37"/>
-      <c r="G79" s="37"/>
-      <c r="H79" s="37"/>
-      <c r="I79" s="37"/>
-      <c r="J79" s="37"/>
-      <c r="K79" s="37"/>
-      <c r="L79" s="37"/>
-      <c r="M79" s="37"/>
-      <c r="N79" s="37"/>
-      <c r="O79" s="37"/>
-      <c r="P79" s="37"/>
-      <c r="Q79" s="37"/>
-      <c r="R79" s="37"/>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="I11:J12 G3:I3 J9:N12 I9 I3:O7 A3:B12 O3:R12">
-    <cfRule type="expression" dxfId="19" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="31" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="32" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13326,7 +13321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:DP79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
@@ -13518,7 +13513,7 @@
     </row>
     <row r="3" spans="1:120" ht="24.95" customHeight="1">
       <c r="A3" s="69" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B3" s="74">
         <v>33</v>
@@ -13562,7 +13557,7 @@
     </row>
     <row r="4" spans="1:120" ht="24.95" customHeight="1">
       <c r="A4" s="69" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B4" s="74">
         <v>34</v>
@@ -13606,7 +13601,7 @@
     </row>
     <row r="5" spans="1:120" ht="24.95" customHeight="1">
       <c r="A5" s="83" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B5" s="74">
         <v>35</v>
@@ -13650,7 +13645,7 @@
     </row>
     <row r="6" spans="1:120" s="92" customFormat="1" ht="24.95" customHeight="1">
       <c r="A6" s="69" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B6" s="74">
         <v>36</v>
@@ -13694,7 +13689,7 @@
     </row>
     <row r="7" spans="1:120" s="92" customFormat="1" ht="24.95" customHeight="1">
       <c r="A7" s="69" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B7" s="74">
         <v>37</v>
@@ -13738,7 +13733,7 @@
     </row>
     <row r="8" spans="1:120" ht="24.95" customHeight="1">
       <c r="A8" s="69" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B8" s="74">
         <v>38</v>
@@ -13782,7 +13777,7 @@
     </row>
     <row r="9" spans="1:120" ht="24.95" customHeight="1">
       <c r="A9" s="69" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B9" s="74">
         <v>39</v>
@@ -13826,7 +13821,7 @@
     </row>
     <row r="10" spans="1:120" ht="24.95" customHeight="1">
       <c r="A10" s="69" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B10" s="74">
         <v>40</v>
@@ -15653,74 +15648,74 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:B9 M3:R9">
-    <cfRule type="expression" dxfId="17" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="33" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="34" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B9 A6:B9">
-    <cfRule type="expression" dxfId="15" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="31" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="32" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
-    <cfRule type="expression" dxfId="13" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="29" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="30" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B8">
-    <cfRule type="expression" dxfId="11" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="13" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="14" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A10">
-    <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="12" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B8">
-    <cfRule type="expression" dxfId="7" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:A10">
-    <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="8" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B7">
-    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B10">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
       <formula>#REF!="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
       <formula>#REF!="O"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>